<commit_message>
Modified Reg Client Configs #54, 55, 72-74, Process 14
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E964C68-B00F-454A-9A1D-B843D4BD6207}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1B3F6-9D8D-4523-8BDB-DDF8A3670405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,19 +937,6 @@
   </si>
   <si>
     <t>Frequency of virus scan of registration packets</t>
-  </si>
-  <si>
-    <t>Name
-Age/DoB
-Gender
-Foreigner/National
-Address
-Contact details
-CNIE/EC/Residence Card Number
-Parent/Guardian details
-Biometrics-Exception
-Biometrics-Fingerprint
-Biometrics-Iris</t>
   </si>
   <si>
     <t>Config in Config Server</t>
@@ -3269,6 +3256,18 @@
   <si>
     <t>Retrieve lost UIN acknowledgement SMS will be sent using this template.
 On change: Notifications already queued up when the old template was in force will use the old template. Others will use the updated template.</t>
+  </si>
+  <si>
+    <t>Name
+Age/DoB
+Gender
+Foreigner/National
+Address
+Phone
+Email
+CNIE/EC/Residence Card Number
+Parent/Guardian details
+Biometrics</t>
   </si>
 </sst>
 </file>
@@ -5379,10 +5378,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -5436,16 +5435,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I4" s="69" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="3"/>
@@ -5479,16 +5478,16 @@
         <v>9</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I5" s="69" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
@@ -5522,16 +5521,16 @@
         <v>9</v>
       </c>
       <c r="D6" s="58" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E6" s="58"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I6" s="69" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="3"/>
@@ -5571,10 +5570,10 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I7" s="69" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="3"/>
@@ -5614,10 +5613,10 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="3"/>
@@ -5651,16 +5650,16 @@
         <v>9</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E9" s="58"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I9" s="69" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="3"/>
@@ -5694,16 +5693,16 @@
         <v>9</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E10" s="58"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I10" s="69" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="3"/>
@@ -5737,16 +5736,16 @@
         <v>9</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E11" s="58"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I11" s="69" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="3"/>
@@ -5780,16 +5779,16 @@
         <v>9</v>
       </c>
       <c r="D12" s="58" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E12" s="58"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I12" s="69" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="3"/>
@@ -5829,10 +5828,10 @@
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I13" s="69" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="3"/>
@@ -5966,10 +5965,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I2" s="116" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -5993,10 +5992,10 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="20" customFormat="1" ht="66" x14ac:dyDescent="0.3">
@@ -6018,10 +6017,10 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
@@ -6029,13 +6028,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>32</v>
@@ -6045,10 +6044,10 @@
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
@@ -6062,7 +6061,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>32</v>
@@ -6072,10 +6071,10 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
@@ -6089,7 +6088,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>32</v>
@@ -6099,10 +6098,10 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
@@ -6110,7 +6109,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>9</v>
@@ -6126,10 +6125,10 @@
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="101" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -6137,26 +6136,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.3">
@@ -6164,7 +6163,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>9</v>
@@ -6176,14 +6175,14 @@
         <v>32</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="115" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
@@ -6191,7 +6190,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>9</v>
@@ -6203,14 +6202,14 @@
         <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="115" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
@@ -6218,7 +6217,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>9</v>
@@ -6230,14 +6229,14 @@
         <v>32</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="115" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
@@ -6245,26 +6244,26 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
@@ -6272,13 +6271,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>32</v>
@@ -6286,10 +6285,10 @@
       <c r="F14" s="50"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -6297,13 +6296,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>32</v>
@@ -6311,7 +6310,7 @@
       <c r="F15" s="50"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I15" s="19"/>
     </row>
@@ -6330,7 +6329,7 @@
       </c>
       <c r="E16" s="47"/>
       <c r="F16" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -6349,7 +6348,7 @@
       <c r="D17" s="47"/>
       <c r="E17" s="47"/>
       <c r="F17" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -6368,7 +6367,7 @@
       <c r="D18" s="47"/>
       <c r="E18" s="47"/>
       <c r="F18" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -6387,7 +6386,7 @@
       <c r="D19" s="47"/>
       <c r="E19" s="47"/>
       <c r="F19" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -6406,7 +6405,7 @@
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="F20" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -6425,7 +6424,7 @@
       <c r="D21" s="47"/>
       <c r="E21" s="47"/>
       <c r="F21" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -6444,7 +6443,7 @@
       <c r="D22" s="47"/>
       <c r="E22" s="47"/>
       <c r="F22" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -6463,7 +6462,7 @@
       <c r="D23" s="47"/>
       <c r="E23" s="47"/>
       <c r="F23" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -6482,7 +6481,7 @@
       <c r="D24" s="47"/>
       <c r="E24" s="47"/>
       <c r="F24" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -6505,7 +6504,7 @@
         <v>44</v>
       </c>
       <c r="F25" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -6524,7 +6523,7 @@
       <c r="D26" s="47"/>
       <c r="E26" s="47"/>
       <c r="F26" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -6543,7 +6542,7 @@
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -6564,7 +6563,7 @@
       </c>
       <c r="E28" s="47"/>
       <c r="F28" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -6585,7 +6584,7 @@
       </c>
       <c r="E29" s="66"/>
       <c r="F29" s="65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
@@ -6608,7 +6607,7 @@
   <dimension ref="A1:AML75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
@@ -6657,10 +6656,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -6677,16 +6676,16 @@
         <v>55</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F3" s="43" t="s">
         <v>166</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="211.2" x14ac:dyDescent="0.3">
@@ -6710,10 +6709,10 @@
         <v>11</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
@@ -6733,10 +6732,10 @@
         <v>156</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
@@ -6756,10 +6755,10 @@
         <v>61</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -6783,10 +6782,10 @@
         <v>157</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -6810,10 +6809,10 @@
         <v>66</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
@@ -6837,10 +6836,10 @@
         <v>11</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -6864,10 +6863,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
@@ -6891,10 +6890,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
@@ -6918,10 +6917,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -6939,16 +6938,16 @@
         <v>55</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>154</v>
       </c>
       <c r="G13" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
@@ -6966,16 +6965,16 @@
         <v>55</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -6995,10 +6994,10 @@
         <v>11</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="66" x14ac:dyDescent="0.3">
@@ -7018,10 +7017,10 @@
         <v>11</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -7041,10 +7040,10 @@
         <v>11</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -7064,10 +7063,10 @@
         <v>11</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -7088,7 +7087,7 @@
       </c>
       <c r="G19" s="47"/>
       <c r="H19" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -7109,7 +7108,7 @@
       </c>
       <c r="G20" s="47"/>
       <c r="H20" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -7129,10 +7128,10 @@
         <v>11</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -7152,10 +7151,10 @@
         <v>11</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -7176,7 +7175,7 @@
       </c>
       <c r="G23" s="47"/>
       <c r="H23" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -7197,7 +7196,7 @@
       </c>
       <c r="G24" s="47"/>
       <c r="H24" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
@@ -7212,17 +7211,17 @@
         <v>9</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="100" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -7231,21 +7230,21 @@
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="66" x14ac:dyDescent="0.3">
@@ -7260,17 +7259,17 @@
         <v>9</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="66" x14ac:dyDescent="0.3">
@@ -7285,17 +7284,17 @@
         <v>9</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
@@ -7317,10 +7316,10 @@
         <v>11</v>
       </c>
       <c r="G29" s="50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="198" x14ac:dyDescent="0.3">
@@ -7329,7 +7328,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>9</v>
@@ -7338,16 +7337,16 @@
         <v>85</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="132" x14ac:dyDescent="0.3">
@@ -7356,7 +7355,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>9</v>
@@ -7365,16 +7364,16 @@
         <v>85</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -7392,16 +7391,16 @@
         <v>87</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="33" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
@@ -7419,16 +7418,16 @@
         <v>100</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="34" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
@@ -7452,10 +7451,10 @@
         <v>11</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="35" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
@@ -7479,10 +7478,10 @@
         <v>11</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="36" spans="1:1026" ht="171.6" x14ac:dyDescent="0.3">
@@ -7506,10 +7505,10 @@
         <v>11</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="37" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
@@ -7530,7 +7529,7 @@
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
@@ -7539,23 +7538,23 @@
         <v>36</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="21" t="s">
+        <v>447</v>
+      </c>
+      <c r="E38" s="21" t="s">
         <v>448</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>449</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="39" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
@@ -7577,10 +7576,10 @@
         <v>11</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="40" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
@@ -7598,16 +7597,16 @@
         <v>55</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G40" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="41" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
@@ -7625,16 +7624,16 @@
         <v>55</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="42" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
@@ -7658,10 +7657,10 @@
         <v>11</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H42" s="45" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -8701,10 +8700,10 @@
         <v>11</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -9742,10 +9741,10 @@
       <c r="E44" s="36"/>
       <c r="F44" s="50"/>
       <c r="G44" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="45" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
@@ -9754,7 +9753,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C45" s="37" t="s">
         <v>9</v>
@@ -9768,7 +9767,7 @@
         <v>142</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="46" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
@@ -9788,10 +9787,10 @@
       <c r="E46" s="36"/>
       <c r="F46" s="50"/>
       <c r="G46" s="50" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="47" spans="1:1026" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -9811,10 +9810,10 @@
       <c r="E47" s="36"/>
       <c r="F47" s="50"/>
       <c r="G47" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="48" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
@@ -9832,14 +9831,14 @@
         <v>180</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F48" s="50"/>
       <c r="G48" s="50" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -9857,14 +9856,14 @@
         <v>180</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F49" s="50"/>
       <c r="G49" s="50" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="66" x14ac:dyDescent="0.3">
@@ -9882,14 +9881,14 @@
         <v>180</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F50" s="50"/>
       <c r="G50" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="132" x14ac:dyDescent="0.3">
@@ -9907,14 +9906,14 @@
         <v>100</v>
       </c>
       <c r="E51" s="36" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F51" s="50"/>
       <c r="G51" s="50" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -9934,10 +9933,10 @@
       <c r="E52" s="36"/>
       <c r="F52" s="50"/>
       <c r="G52" s="50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -9957,10 +9956,10 @@
       <c r="E53" s="36"/>
       <c r="F53" s="50"/>
       <c r="G53" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -9980,10 +9979,10 @@
       <c r="E54" s="36"/>
       <c r="F54" s="50"/>
       <c r="G54" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -9992,7 +9991,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>9</v>
@@ -10003,10 +10002,10 @@
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
@@ -10015,7 +10014,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C56" s="37" t="s">
         <v>9</v>
@@ -10024,10 +10023,10 @@
       <c r="E56" s="28"/>
       <c r="F56" s="28"/>
       <c r="G56" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="345.6" x14ac:dyDescent="0.3">
@@ -10042,15 +10041,15 @@
         <v>9</v>
       </c>
       <c r="D57" s="36" t="s">
-        <v>231</v>
+        <v>642</v>
       </c>
       <c r="E57" s="41"/>
       <c r="F57" s="49"/>
       <c r="G57" s="50" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="132" x14ac:dyDescent="0.3">
@@ -10068,14 +10067,14 @@
         <v>180</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F58" s="50"/>
       <c r="G58" s="50" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -10093,14 +10092,14 @@
         <v>180</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F59" s="50"/>
       <c r="G59" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -10108,23 +10107,23 @@
         <v>59</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C60" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="36" t="s">
+        <v>466</v>
+      </c>
+      <c r="E60" s="36" t="s">
         <v>467</v>
-      </c>
-      <c r="E60" s="36" t="s">
-        <v>468</v>
       </c>
       <c r="F60" s="36"/>
       <c r="G60" s="36" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H60" s="36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -10132,23 +10131,23 @@
         <v>60</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C61" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="36" t="s">
+        <v>466</v>
+      </c>
+      <c r="E61" s="36" t="s">
         <v>467</v>
-      </c>
-      <c r="E61" s="36" t="s">
-        <v>468</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H61" s="36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -10156,21 +10155,21 @@
         <v>61</v>
       </c>
       <c r="B62" s="36" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C62" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="36" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E62" s="36"/>
       <c r="F62" s="36"/>
       <c r="G62" s="36" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H62" s="36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -10178,23 +10177,23 @@
         <v>62</v>
       </c>
       <c r="B63" s="36" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C63" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D63" s="36" t="s">
+        <v>466</v>
+      </c>
+      <c r="E63" s="36" t="s">
         <v>467</v>
-      </c>
-      <c r="E63" s="36" t="s">
-        <v>468</v>
       </c>
       <c r="F63" s="36"/>
       <c r="G63" s="36" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H63" s="36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -10202,23 +10201,23 @@
         <v>63</v>
       </c>
       <c r="B64" s="36" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C64" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="36" t="s">
+        <v>466</v>
+      </c>
+      <c r="E64" s="36" t="s">
         <v>467</v>
-      </c>
-      <c r="E64" s="36" t="s">
-        <v>468</v>
       </c>
       <c r="F64" s="36"/>
       <c r="G64" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H64" s="36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -10226,23 +10225,23 @@
         <v>64</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C65" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="36" t="s">
+        <v>466</v>
+      </c>
+      <c r="E65" s="36" t="s">
         <v>467</v>
-      </c>
-      <c r="E65" s="36" t="s">
-        <v>468</v>
       </c>
       <c r="F65" s="36"/>
       <c r="G65" s="36" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H65" s="36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -10250,23 +10249,23 @@
         <v>65</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C66" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="36" t="s">
+        <v>466</v>
+      </c>
+      <c r="E66" s="36" t="s">
         <v>467</v>
-      </c>
-      <c r="E66" s="36" t="s">
-        <v>468</v>
       </c>
       <c r="F66" s="36"/>
       <c r="G66" s="36" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H66" s="36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -10274,7 +10273,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>9</v>
@@ -10285,10 +10284,10 @@
       <c r="E67" s="36"/>
       <c r="F67" s="36"/>
       <c r="G67" s="36" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H67" s="36" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -10296,7 +10295,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="36" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C68" s="36" t="s">
         <v>9</v>
@@ -10307,7 +10306,7 @@
       <c r="E68" s="36"/>
       <c r="F68" s="36"/>
       <c r="G68" s="36" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H68" s="36"/>
     </row>
@@ -10316,18 +10315,18 @@
         <v>68</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C69" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E69" s="36"/>
       <c r="F69" s="36"/>
       <c r="G69" s="36" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H69" s="36"/>
     </row>
@@ -10336,18 +10335,18 @@
         <v>69</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C70" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="36" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E70" s="36"/>
       <c r="F70" s="36"/>
       <c r="G70" s="36" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H70" s="36"/>
     </row>
@@ -10356,18 +10355,18 @@
         <v>70</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C71" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E71" s="36"/>
       <c r="F71" s="36"/>
       <c r="G71" s="36" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H71" s="36"/>
     </row>
@@ -10376,18 +10375,18 @@
         <v>71</v>
       </c>
       <c r="B72" s="36" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C72" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D72" s="36" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E72" s="36"/>
       <c r="F72" s="36"/>
       <c r="G72" s="36" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H72" s="36"/>
     </row>
@@ -10396,21 +10395,21 @@
         <v>72</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C73" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E73" s="36" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -10418,7 +10417,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>9</v>
@@ -10428,7 +10427,7 @@
       <c r="F74" s="8"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
@@ -10437,7 +10436,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>9</v>
@@ -10447,7 +10446,7 @@
       <c r="F75" s="8"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -10520,10 +10519,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
@@ -10531,20 +10530,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>386</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>387</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="10"/>
       <c r="G3" s="26"/>
       <c r="H3" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="I3" s="45" t="s">
         <v>388</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
@@ -10555,17 +10554,17 @@
         <v>98</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
       <c r="H4" s="26" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
@@ -10573,20 +10572,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
       <c r="H5" s="26" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
@@ -10594,20 +10593,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
@@ -10615,20 +10614,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I7" s="45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -10636,20 +10635,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="H8" s="26" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
@@ -10660,7 +10659,7 @@
         <v>99</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>100</v>
@@ -10669,10 +10668,10 @@
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
       <c r="H9" s="102" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I9" s="103" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
@@ -10680,22 +10679,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="D10" s="28" t="s">
         <v>400</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>387</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>401</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
       <c r="H10" s="102" t="s">
+        <v>401</v>
+      </c>
+      <c r="I10" s="103" t="s">
         <v>402</v>
-      </c>
-      <c r="I10" s="103" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
@@ -10703,20 +10702,20 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="26" t="s">
+        <v>406</v>
+      </c>
+      <c r="I11" s="45" t="s">
         <v>407</v>
-      </c>
-      <c r="I11" s="45" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
@@ -10724,20 +10723,20 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="I12" s="45" t="s">
         <v>410</v>
-      </c>
-      <c r="I12" s="45" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -10745,20 +10744,20 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="I13" s="45" t="s">
         <v>413</v>
-      </c>
-      <c r="I13" s="45" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
@@ -10766,20 +10765,20 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="26" t="s">
+        <v>415</v>
+      </c>
+      <c r="I14" s="45" t="s">
         <v>416</v>
-      </c>
-      <c r="I14" s="45" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
@@ -10787,20 +10786,20 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
       <c r="H15" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="I15" s="45" t="s">
         <v>419</v>
-      </c>
-      <c r="I15" s="45" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="132" x14ac:dyDescent="0.3">
@@ -10808,22 +10807,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="I16" s="45" t="s">
         <v>423</v>
-      </c>
-      <c r="I16" s="45" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.3">
@@ -10831,20 +10830,20 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="I17" s="45" t="s">
         <v>426</v>
-      </c>
-      <c r="I17" s="45" t="s">
-        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -10920,10 +10919,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:1027" s="84" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
@@ -10943,7 +10942,7 @@
         <v>104</v>
       </c>
       <c r="F3" s="79" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G3" s="79"/>
       <c r="H3" s="79"/>
@@ -11984,7 +11983,7 @@
         <v>107</v>
       </c>
       <c r="F4" s="79" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G4" s="79"/>
       <c r="H4" s="79"/>
@@ -16262,7 +16261,7 @@
       <c r="D14" s="54"/>
       <c r="E14" s="54"/>
       <c r="F14" s="54" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G14" s="72"/>
       <c r="H14" s="72"/>
@@ -17307,10 +17306,10 @@
       </c>
       <c r="G15" s="36"/>
       <c r="H15" s="36" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17334,10 +17333,10 @@
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="17" spans="1:1027" ht="224.4" x14ac:dyDescent="0.3">
@@ -17361,10 +17360,10 @@
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="18" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -17388,10 +17387,10 @@
       </c>
       <c r="G18" s="36"/>
       <c r="H18" s="36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="19" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
@@ -19483,7 +19482,7 @@
         <v>125</v>
       </c>
       <c r="F21" s="88" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G21" s="91"/>
       <c r="H21" s="91"/>
@@ -20512,7 +20511,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C22" s="37" t="s">
         <v>9</v>
@@ -20521,17 +20520,17 @@
         <v>131</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F22" s="36" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -20539,24 +20538,24 @@
         <v>6</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="39" t="s">
+        <v>606</v>
+      </c>
+      <c r="E23" s="38" t="s">
         <v>607</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>608</v>
       </c>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="36" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="24" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -20564,24 +20563,24 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="39" t="s">
+        <v>610</v>
+      </c>
+      <c r="E24" s="38" t="s">
         <v>611</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>612</v>
       </c>
       <c r="F24" s="36"/>
       <c r="G24" s="36"/>
       <c r="H24" s="36" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:1027" ht="138" x14ac:dyDescent="0.3">
@@ -20605,10 +20604,10 @@
       </c>
       <c r="G25" s="112"/>
       <c r="H25" s="112" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I25" s="112" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="26" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
@@ -20632,10 +20631,10 @@
       </c>
       <c r="G26" s="36"/>
       <c r="H26" s="36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="27" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
@@ -20649,7 +20648,7 @@
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
       <c r="F27" s="88" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G27" s="36"/>
       <c r="H27" s="36"/>
@@ -20666,7 +20665,7 @@
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
       <c r="F28" s="88" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="36"/>
@@ -20698,13 +20697,13 @@
         <v>9</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E30" s="39" t="s">
         <v>5</v>
@@ -20712,10 +20711,10 @@
       <c r="F30" s="88"/>
       <c r="G30" s="36"/>
       <c r="H30" s="36" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I30" s="36" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="31" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -20723,7 +20722,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C31" s="40" t="s">
         <v>9</v>
@@ -20732,15 +20731,15 @@
         <v>22</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F31" s="88"/>
       <c r="G31" s="36"/>
       <c r="H31" s="36" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="32" spans="1:1027" s="99" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
@@ -20748,13 +20747,13 @@
         <v>11</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C32" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="96" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E32" s="38" t="s">
         <v>5</v>
@@ -20762,10 +20761,10 @@
       <c r="F32" s="36"/>
       <c r="G32" s="97"/>
       <c r="H32" s="97" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="J32" s="98"/>
       <c r="K32" s="98"/>
@@ -21852,10 +21851,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
@@ -22059,10 +22058,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I2" s="70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -22076,7 +22075,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
@@ -22084,10 +22083,10 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -22127,10 +22126,10 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -22162,7 +22161,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
@@ -22170,10 +22169,10 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="36" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -22211,10 +22210,10 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="36" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -22254,10 +22253,10 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -22295,10 +22294,10 @@
       <c r="F8" s="8"/>
       <c r="G8" s="7"/>
       <c r="H8" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="I8" s="36" t="s">
         <v>309</v>
-      </c>
-      <c r="I8" s="36" t="s">
-        <v>310</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -22336,10 +22335,10 @@
       <c r="F9" s="8"/>
       <c r="G9" s="7"/>
       <c r="H9" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -22371,7 +22370,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="105" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E10" s="41"/>
       <c r="F10" s="8" t="s">
@@ -22379,10 +22378,10 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="41" t="s">
+        <v>312</v>
+      </c>
+      <c r="I10" s="36" t="s">
         <v>313</v>
-      </c>
-      <c r="I10" s="36" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
@@ -22405,10 +22404,10 @@
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -22448,10 +22447,10 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -22489,10 +22488,10 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -22532,10 +22531,10 @@
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -22573,10 +22572,10 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -22614,10 +22613,10 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -22655,10 +22654,10 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -24770,10 +24769,10 @@
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="21" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
@@ -24796,10 +24795,10 @@
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="22" spans="1:1025" s="75" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -25860,10 +25859,10 @@
       </c>
       <c r="G23" s="41"/>
       <c r="H23" s="41" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="24" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
@@ -25884,10 +25883,10 @@
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="25" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
@@ -25908,10 +25907,10 @@
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I25" s="36" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="26" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
@@ -25932,10 +25931,10 @@
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="27" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
@@ -25950,16 +25949,16 @@
         <v>9</v>
       </c>
       <c r="D27" s="106" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
       <c r="H27" s="41" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="28" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
@@ -25980,10 +25979,10 @@
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="29" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
@@ -26004,10 +26003,10 @@
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="30" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
@@ -26022,16 +26021,16 @@
         <v>9</v>
       </c>
       <c r="D30" s="107" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E30" s="41"/>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I30" s="36" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
@@ -26052,10 +26051,10 @@
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="32" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
@@ -26076,10 +26075,10 @@
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
       <c r="H32" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="33" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
@@ -26094,16 +26093,16 @@
         <v>9</v>
       </c>
       <c r="D33" s="106" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E33" s="41"/>
       <c r="F33" s="41"/>
       <c r="G33" s="41"/>
       <c r="H33" s="41" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I33" s="36" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
@@ -27158,10 +27157,10 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="41" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I35" s="36" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="36" spans="1:1025" ht="132" x14ac:dyDescent="0.3">
@@ -27182,10 +27181,10 @@
       <c r="F36" s="41"/>
       <c r="G36" s="41"/>
       <c r="H36" s="41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I36" s="36" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="37" spans="1:1025" ht="79.2" x14ac:dyDescent="0.3">
@@ -27206,10 +27205,10 @@
       <c r="F37" s="41"/>
       <c r="G37" s="41"/>
       <c r="H37" s="41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I37" s="36" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="38" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
@@ -27218,7 +27217,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C38" s="41" t="s">
         <v>9</v>
@@ -27230,10 +27229,10 @@
       <c r="F38" s="41"/>
       <c r="G38" s="41"/>
       <c r="H38" s="41" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I38" s="36" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="39" spans="1:1025" x14ac:dyDescent="0.3">
@@ -27242,19 +27241,19 @@
         <v>36</v>
       </c>
       <c r="B39" s="60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="41"/>
       <c r="G39" s="41"/>
       <c r="H39" s="36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I39" s="41"/>
     </row>
@@ -27264,7 +27263,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="60" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C40" s="41" t="s">
         <v>9</v>
@@ -27276,10 +27275,10 @@
       <c r="F40" s="41"/>
       <c r="G40" s="41"/>
       <c r="H40" s="41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I40" s="36" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="41" spans="1:1025" ht="409.6" x14ac:dyDescent="0.3">
@@ -27288,22 +27287,22 @@
         <v>38</v>
       </c>
       <c r="B41" s="60" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C41" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="105" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E41" s="41"/>
       <c r="F41" s="41"/>
       <c r="G41" s="41"/>
       <c r="H41" s="41" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I41" s="36" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="42" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
@@ -27311,7 +27310,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C42" s="41" t="s">
         <v>9</v>
@@ -27323,10 +27322,10 @@
       <c r="F42" s="41"/>
       <c r="G42" s="41"/>
       <c r="H42" s="41" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I42" s="36" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="43" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
@@ -27334,7 +27333,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C43" s="41" t="s">
         <v>9</v>
@@ -27346,10 +27345,10 @@
       <c r="F43" s="41"/>
       <c r="G43" s="41"/>
       <c r="H43" s="41" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="44" spans="1:1025" ht="39.6" x14ac:dyDescent="0.3">
@@ -27357,22 +27356,22 @@
         <v>41</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C44" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E44" s="41"/>
       <c r="F44" s="41"/>
       <c r="G44" s="41"/>
       <c r="H44" s="41" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I44" s="36" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="45" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
@@ -27380,22 +27379,22 @@
         <v>42</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C45" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="105" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E45" s="41"/>
       <c r="F45" s="41"/>
       <c r="G45" s="41"/>
       <c r="H45" s="41" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I45" s="36" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="46" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
@@ -27403,22 +27402,22 @@
         <v>43</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C46" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E46" s="41"/>
       <c r="F46" s="41"/>
       <c r="G46" s="41"/>
       <c r="H46" s="41" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I46" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
@@ -27426,7 +27425,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C47" s="41" t="s">
         <v>9</v>
@@ -27438,10 +27437,10 @@
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
       <c r="H47" s="104" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="48" spans="1:1025" x14ac:dyDescent="0.3">
@@ -27461,7 +27460,7 @@
       <c r="F48" s="41"/>
       <c r="G48" s="41"/>
       <c r="H48" s="104" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I48" s="36"/>
     </row>
@@ -27482,7 +27481,7 @@
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
       <c r="H49" s="104" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I49" s="36"/>
     </row>
@@ -27503,7 +27502,7 @@
       <c r="F50" s="41"/>
       <c r="G50" s="41"/>
       <c r="H50" s="104" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I50" s="36"/>
     </row>
@@ -27512,22 +27511,22 @@
         <v>48</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C51" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E51" s="41"/>
       <c r="F51" s="41"/>
       <c r="G51" s="41"/>
       <c r="H51" s="104" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I51" s="36" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="66" x14ac:dyDescent="0.3">
@@ -27535,7 +27534,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C52" s="41" t="s">
         <v>9</v>
@@ -27547,10 +27546,10 @@
       <c r="F52" s="41"/>
       <c r="G52" s="41"/>
       <c r="H52" s="104" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I52" s="36" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Requirements for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1B3F6-9D8D-4523-8BDB-DDF8A3670405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{70C4B283-822D-42B8-827D-A72E1AD9618B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8535" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,7 @@
     <sheet name="Resident Services" sheetId="6" r:id="rId6"/>
     <sheet name="Global Configurations" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -3050,19 +3043,6 @@
     <t>static.token.enable</t>
   </si>
   <si>
-    <t xml:space="preserve">  
-Single:fgrmin.threshold
-Composite: fgrmin.composite.threshold
-</t>
-  </si>
-  <si>
-    <t>Single: irisimg.threshold
-Composite: irisimg.composite.threshold</t>
-  </si>
-  <si>
-    <t>allowed.auth.types</t>
-  </si>
-  <si>
     <t>Configure authentications permissable for e-KYC for a country</t>
   </si>
   <si>
@@ -3268,6 +3248,19 @@
 CNIE/EC/Residence Card Number
 Parent/Guardian details
 Biometrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+Single:fgrmin.single.threshold
+Composite: fgrmin.composite.threshold
+</t>
+  </si>
+  <si>
+    <t>Single: irisimg.single.threshold
+Composite: irisimg.composite.threshold</t>
+  </si>
+  <si>
+    <t>auth.types.allowed</t>
   </si>
 </sst>
 </file>
@@ -5327,21 +5320,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="3" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
@@ -5355,7 +5348,7 @@
       <c r="I1" s="118"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -5385,7 +5378,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="67">
         <v>1</v>
       </c>
@@ -5423,7 +5416,7 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>2</v>
@@ -5466,7 +5459,7 @@
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
     </row>
-    <row r="5" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5509,7 +5502,7 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
     </row>
-    <row r="6" spans="1:28" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5552,7 +5545,7 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5595,7 +5588,7 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
     </row>
-    <row r="8" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5638,7 +5631,7 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
     </row>
-    <row r="9" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5681,7 +5674,7 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
     </row>
-    <row r="10" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5724,7 +5717,7 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
     </row>
-    <row r="11" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5767,7 +5760,7 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
     </row>
-    <row r="12" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5810,7 +5803,7 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
     </row>
-    <row r="13" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5853,7 +5846,7 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5915,21 +5908,21 @@
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="14" customWidth="1"/>
     <col min="2" max="2" width="72" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="15" customWidth="1"/>
     <col min="5" max="5" width="16" style="15" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="33.77734375" style="16" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="36.21875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="35.21875" style="16" customWidth="1"/>
-    <col min="10" max="1025" width="9.21875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="35.28515625" style="16" customWidth="1"/>
+    <col min="10" max="1025" width="9.28515625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="119" t="s">
         <v>26</v>
       </c>
@@ -5942,7 +5935,7 @@
       <c r="H1" s="119"/>
       <c r="I1" s="119"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -5971,7 +5964,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -5992,13 +5985,13 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="20" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -6017,18 +6010,18 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>9</v>
@@ -6050,7 +6043,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -6071,13 +6064,13 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -6098,13 +6091,13 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -6125,40 +6118,40 @@
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="101" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="I9" s="19" t="s">
         <v>622</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>625</v>
-      </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>8</v>
       </c>
@@ -6185,7 +6178,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>9</v>
       </c>
@@ -6212,7 +6205,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>10</v>
       </c>
@@ -6233,13 +6226,13 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="115" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>11</v>
       </c>
@@ -6256,7 +6249,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
@@ -6266,7 +6259,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>12</v>
       </c>
@@ -6291,18 +6284,18 @@
         <v>366</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>32</v>
@@ -6310,11 +6303,11 @@
       <c r="F15" s="50"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>14</v>
       </c>
@@ -6335,7 +6328,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -6354,7 +6347,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>16</v>
       </c>
@@ -6373,7 +6366,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>17</v>
       </c>
@@ -6392,7 +6385,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>18</v>
       </c>
@@ -6411,7 +6404,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>19</v>
       </c>
@@ -6430,7 +6423,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>20</v>
       </c>
@@ -6449,7 +6442,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>21</v>
       </c>
@@ -6468,7 +6461,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>22</v>
       </c>
@@ -6487,7 +6480,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>23</v>
       </c>
@@ -6510,7 +6503,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>24</v>
       </c>
@@ -6529,7 +6522,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>25</v>
       </c>
@@ -6548,7 +6541,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>26</v>
       </c>
@@ -6569,7 +6562,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="62"/>
     </row>
-    <row r="29" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>27</v>
       </c>
@@ -6606,25 +6599,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AML75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="46.5546875" style="15" customWidth="1"/>
-    <col min="9" max="1026" width="9.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="46.5703125" style="15" customWidth="1"/>
+    <col min="9" max="1026" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="109" t="s">
         <v>53</v>
       </c>
@@ -6636,7 +6629,7 @@
       <c r="G1" s="109"/>
       <c r="H1" s="109"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -6662,7 +6655,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -6688,7 +6681,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="211.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A59" si="0">A3+1</f>
         <v>2</v>
@@ -6715,7 +6708,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6738,7 +6731,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6761,7 +6754,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6788,7 +6781,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6815,7 +6808,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6842,7 +6835,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6869,7 +6862,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6896,7 +6889,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6923,7 +6916,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6950,7 +6943,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6977,7 +6970,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7000,7 +6993,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7023,7 +7016,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7046,7 +7039,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7069,7 +7062,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7090,7 +7083,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7111,7 +7104,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7134,7 +7127,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7157,7 +7150,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -7178,7 +7171,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -7199,7 +7192,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7224,7 +7217,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -7247,7 +7240,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -7272,7 +7265,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -7297,7 +7290,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -7322,7 +7315,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="198" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7349,7 +7342,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7376,7 +7369,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7403,7 +7396,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="33" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7430,7 +7423,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="34" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7457,7 +7450,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="35" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7484,7 +7477,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="36" spans="1:1026" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1026" ht="195" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7511,7 +7504,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="37" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7532,7 +7525,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7557,7 +7550,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="39" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7582,7 +7575,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="40" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7609,7 +7602,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="41" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7636,7 +7629,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="42" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -8681,7 +8674,7 @@
       <c r="AMK42" s="15"/>
       <c r="AML42" s="15"/>
     </row>
-    <row r="43" spans="1:1026" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1026" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -9724,7 +9717,7 @@
       <c r="AMK43" s="15"/>
       <c r="AML43" s="15"/>
     </row>
-    <row r="44" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9747,7 +9740,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="45" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -9770,7 +9763,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="46" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9793,7 +9786,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="47" spans="1:1026" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1026" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9816,7 +9809,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="48" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9841,7 +9834,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9866,7 +9859,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9891,7 +9884,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9916,7 +9909,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9939,7 +9932,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -9962,7 +9955,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -9985,7 +9978,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -10008,13 +10001,13 @@
         <v>579</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C56" s="37" t="s">
         <v>9</v>
@@ -10026,10 +10019,10 @@
         <v>461</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="375" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -10041,7 +10034,7 @@
         <v>9</v>
       </c>
       <c r="D57" s="36" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E57" s="41"/>
       <c r="F57" s="49"/>
@@ -10052,7 +10045,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -10077,7 +10070,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -10102,7 +10095,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -10126,7 +10119,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -10150,7 +10143,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -10172,7 +10165,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -10196,7 +10189,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -10220,7 +10213,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -10244,7 +10237,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -10268,7 +10261,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -10290,7 +10283,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -10310,7 +10303,7 @@
       </c>
       <c r="H68" s="36"/>
     </row>
-    <row r="69" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -10330,7 +10323,7 @@
       </c>
       <c r="H69" s="36"/>
     </row>
-    <row r="70" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -10350,7 +10343,7 @@
       </c>
       <c r="H70" s="36"/>
     </row>
-    <row r="71" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -10370,7 +10363,7 @@
       </c>
       <c r="H71" s="36"/>
     </row>
-    <row r="72" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -10390,18 +10383,18 @@
       </c>
       <c r="H72" s="36"/>
     </row>
-    <row r="73" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>72</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C73" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="E73" s="36" t="s">
         <v>591</v>
@@ -10409,15 +10402,15 @@
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>9</v>
@@ -10427,16 +10420,16 @@
       <c r="F74" s="8"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <f t="shared" ref="A75" si="1">A74+1</f>
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>9</v>
@@ -10446,7 +10439,7 @@
       <c r="F75" s="8"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -10469,21 +10462,21 @@
       <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5546875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="30.44140625" style="24" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="40.21875" style="24" customWidth="1"/>
-    <col min="9" max="9" width="62.77734375" style="24" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="24" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="62.7109375" style="24" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="120" t="s">
         <v>155</v>
       </c>
@@ -10496,7 +10489,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -10525,7 +10518,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -10546,7 +10539,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -10567,7 +10560,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>3</v>
       </c>
@@ -10588,7 +10581,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>4</v>
       </c>
@@ -10609,7 +10602,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>5</v>
       </c>
@@ -10630,7 +10623,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -10651,7 +10644,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -10674,7 +10667,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="28">
         <v>8</v>
       </c>
@@ -10697,7 +10690,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -10718,7 +10711,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>10</v>
       </c>
@@ -10739,7 +10732,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>11</v>
       </c>
@@ -10760,7 +10753,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="28">
         <v>12</v>
       </c>
@@ -10781,7 +10774,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <v>13</v>
       </c>
@@ -10802,7 +10795,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="132" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -10825,7 +10818,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -10862,28 +10855,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMM32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="44.5546875" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1027" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="120" t="s">
         <v>101</v>
       </c>
@@ -10896,7 +10889,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:1027" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1027" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -10925,7 +10918,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:1027" s="84" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" s="84" customFormat="1" ht="330" x14ac:dyDescent="0.25">
       <c r="A3" s="78">
         <v>1</v>
       </c>
@@ -11966,7 +11959,7 @@
       <c r="AML3" s="83"/>
       <c r="AMM3" s="83"/>
     </row>
-    <row r="4" spans="1:1027" s="84" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1027" s="84" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="78">
         <v>2</v>
       </c>
@@ -13007,7 +13000,7 @@
       <c r="AML4" s="83"/>
       <c r="AMM4" s="83"/>
     </row>
-    <row r="5" spans="1:1027" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -13030,7 +13023,7 @@
       <c r="H5" s="57"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -13051,7 +13044,7 @@
       <c r="H6" s="53"/>
       <c r="I6" s="41"/>
     </row>
-    <row r="7" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -13072,7 +13065,7 @@
       <c r="H7" s="53"/>
       <c r="I7" s="41"/>
     </row>
-    <row r="8" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -13095,7 +13088,7 @@
       <c r="H8" s="53"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -13116,7 +13109,7 @@
       <c r="H9" s="53"/>
       <c r="I9" s="41"/>
     </row>
-    <row r="10" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -13137,7 +13130,7 @@
       <c r="H10" s="53"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="85">
         <v>9</v>
       </c>
@@ -14174,7 +14167,7 @@
       <c r="AML11" s="74"/>
       <c r="AMM11" s="74"/>
     </row>
-    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="85">
         <v>10</v>
       </c>
@@ -15211,7 +15204,7 @@
       <c r="AML12" s="74"/>
       <c r="AMM12" s="74"/>
     </row>
-    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="85">
         <v>11</v>
       </c>
@@ -16248,7 +16241,7 @@
       <c r="AML13" s="74"/>
       <c r="AMM13" s="74"/>
     </row>
-    <row r="14" spans="1:1027" s="75" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1027" s="75" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="85">
         <v>12</v>
       </c>
@@ -17285,7 +17278,7 @@
       <c r="AML14" s="74"/>
       <c r="AMM14" s="74"/>
     </row>
-    <row r="15" spans="1:1027" ht="211.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>1</v>
       </c>
@@ -17312,7 +17305,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>2</v>
       </c>
@@ -17333,13 +17326,13 @@
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36" t="s">
-        <v>601</v>
+        <v>640</v>
       </c>
       <c r="I16" s="36" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="17" spans="1:1027" ht="224.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>3</v>
       </c>
@@ -17360,13 +17353,13 @@
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36" t="s">
-        <v>602</v>
+        <v>641</v>
       </c>
       <c r="I17" s="36" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="18" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>4</v>
       </c>
@@ -17393,7 +17386,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="19" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1027" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="78">
         <v>17</v>
       </c>
@@ -18430,7 +18423,7 @@
       <c r="AML19" s="83"/>
       <c r="AMM19" s="83"/>
     </row>
-    <row r="20" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1027" s="84" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="78">
         <v>18</v>
       </c>
@@ -19467,7 +19460,7 @@
       <c r="AML20" s="83"/>
       <c r="AMM20" s="83"/>
     </row>
-    <row r="21" spans="1:1027" s="94" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1027" s="94" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="87"/>
       <c r="B21" s="88" t="s">
         <v>130</v>
@@ -20506,12 +20499,12 @@
       <c r="AML21" s="93"/>
       <c r="AMM21" s="93"/>
     </row>
-    <row r="22" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
       <c r="A22" s="87">
         <v>5</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C22" s="37" t="s">
         <v>9</v>
@@ -20527,63 +20520,63 @@
       </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I22" s="36" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="23" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="87">
         <v>6</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="36" t="s">
-        <v>603</v>
+        <v>642</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="24" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="87">
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="F24" s="36"/>
       <c r="G24" s="36"/>
       <c r="H24" s="36" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="25" spans="1:1027" ht="138" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1027" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A25" s="111">
         <v>19</v>
       </c>
@@ -20607,10 +20600,10 @@
         <v>347</v>
       </c>
       <c r="I25" s="112" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="87">
         <v>8</v>
       </c>
@@ -20637,7 +20630,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="27" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="87"/>
       <c r="B27" s="88" t="s">
         <v>138</v>
@@ -20654,7 +20647,7 @@
       <c r="H27" s="36"/>
       <c r="I27" s="41"/>
     </row>
-    <row r="28" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="87"/>
       <c r="B28" s="88" t="s">
         <v>139</v>
@@ -20671,7 +20664,7 @@
       <c r="H28" s="36"/>
       <c r="I28" s="41"/>
     </row>
-    <row r="29" spans="1:1027" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1027" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="87"/>
       <c r="B29" s="88" t="s">
         <v>162</v>
@@ -20692,7 +20685,7 @@
       <c r="H29" s="36"/>
       <c r="I29" s="41"/>
     </row>
-    <row r="30" spans="1:1027" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1027" ht="195" x14ac:dyDescent="0.25">
       <c r="A30" s="87">
         <v>9</v>
       </c>
@@ -20711,13 +20704,13 @@
       <c r="F30" s="88"/>
       <c r="G30" s="36"/>
       <c r="H30" s="36" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="I30" s="36" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="31" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="87">
         <v>10</v>
       </c>
@@ -20742,7 +20735,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="32" spans="1:1027" s="99" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1027" s="99" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="87">
         <v>11</v>
       </c>
@@ -21802,20 +21795,20 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="29.5546875" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="29.5703125" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="120" t="s">
         <v>140</v>
       </c>
@@ -21828,7 +21821,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:9" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -21857,7 +21850,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -21874,7 +21867,7 @@
       <c r="H3" s="41"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -21891,7 +21884,7 @@
       <c r="H4" s="41"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -21908,7 +21901,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -21925,7 +21918,7 @@
       <c r="H6" s="41"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -21942,7 +21935,7 @@
       <c r="H7" s="41"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -21959,7 +21952,7 @@
       <c r="H8" s="41"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -21976,7 +21969,7 @@
       <c r="H9" s="41"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -22008,21 +22001,21 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="41.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.21875" style="3" customWidth="1"/>
-    <col min="10" max="1025" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="84.28515625" style="3" customWidth="1"/>
+    <col min="10" max="1025" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="121" t="s">
         <v>194</v>
       </c>
@@ -22035,7 +22028,7 @@
       <c r="H1" s="122"/>
       <c r="I1" s="122"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -22064,7 +22057,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -22106,7 +22099,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f>A3+1</f>
         <v>2</v>
@@ -22149,7 +22142,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" ref="A5:A41" si="0">A4+1</f>
         <v>3</v>
@@ -22192,7 +22185,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -22233,7 +22226,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f>A9+1</f>
         <v>7</v>
@@ -22276,7 +22269,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f>A6+1</f>
         <v>5</v>
@@ -22317,7 +22310,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -22358,7 +22351,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -22384,7 +22377,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f>A7+1</f>
         <v>8</v>
@@ -22427,7 +22420,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -22470,7 +22463,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="9" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f>A12+1</f>
         <v>10</v>
@@ -22511,7 +22504,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" s="9" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" s="9" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f>A13+1</f>
         <v>11</v>
@@ -22554,7 +22547,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <f t="shared" ref="A15:A22" si="1">A14+1</f>
         <v>12</v>
@@ -22595,7 +22588,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -22636,7 +22629,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:1025" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1025" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -22677,7 +22670,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="71">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -23713,7 +23706,7 @@
       <c r="AMJ18" s="74"/>
       <c r="AMK18" s="74"/>
     </row>
-    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="71">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -24749,7 +24742,7 @@
       <c r="AMJ19" s="74"/>
       <c r="AMK19" s="74"/>
     </row>
-    <row r="20" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -24775,7 +24768,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="21" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -24801,7 +24794,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="22" spans="1:1025" s="75" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1025" s="75" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="71">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -25839,7 +25832,7 @@
       <c r="AMJ22" s="74"/>
       <c r="AMK22" s="74"/>
     </row>
-    <row r="23" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -25865,7 +25858,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="24" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -25889,7 +25882,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="25" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -25913,7 +25906,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="26" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -25937,7 +25930,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="27" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -25961,7 +25954,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -25985,7 +25978,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="29" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -26009,7 +26002,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="30" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -26033,7 +26026,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="31" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -26057,7 +26050,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="32" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -26081,7 +26074,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -26105,7 +26098,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -27139,7 +27132,7 @@
       <c r="AMJ34" s="74"/>
       <c r="AMK34" s="74"/>
     </row>
-    <row r="35" spans="1:1025" ht="184.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1025" ht="210" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -27163,7 +27156,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="132" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1025" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -27187,7 +27180,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1025" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -27211,7 +27204,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -27235,7 +27228,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -27257,7 +27250,7 @@
       </c>
       <c r="I39" s="41"/>
     </row>
-    <row r="40" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -27281,7 +27274,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1025" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -27305,7 +27298,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>39</v>
       </c>
@@ -27328,7 +27321,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>40</v>
       </c>
@@ -27351,7 +27344,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>41</v>
       </c>
@@ -27374,7 +27367,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="45" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>42</v>
       </c>
@@ -27397,7 +27390,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>43</v>
       </c>
@@ -27420,7 +27413,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>44</v>
       </c>
@@ -27443,7 +27436,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="48" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>45</v>
       </c>
@@ -27464,7 +27457,7 @@
       </c>
       <c r="I48" s="36"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>46</v>
       </c>
@@ -27485,7 +27478,7 @@
       </c>
       <c r="I49" s="36"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>47</v>
       </c>
@@ -27506,7 +27499,7 @@
       </c>
       <c r="I50" s="36"/>
     </row>
-    <row r="51" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>48</v>
       </c>
@@ -27529,7 +27522,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Updated VID config for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B9293D92-711F-4B94-A2AA-C8114B7D80A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F4ED499F-DB12-4D3D-85F5-6A7D379F82A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6465" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3290,9 +3290,6 @@
     <t>Setup PDF template for e-KYC</t>
   </si>
   <si>
-    <t>Configure the idtype to be supported for Authentication</t>
-  </si>
-  <si>
     <t>UIN/VIN</t>
   </si>
   <si>
@@ -3300,6 +3297,9 @@
   </si>
   <si>
     <t>To be added</t>
+  </si>
+  <si>
+    <t>Configure the idtype to be supported for Authentication/KYC/OTP Request</t>
   </si>
   <si>
     <r>
@@ -3325,7 +3325,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> he authentication,eKYC and OTP requests will be supported for the id Type Changed
+      <t xml:space="preserve"> The authentication,eKYC and OTP requests will be supported for the id Type Changed
 In general this is an one-time setup activity. However the country might decide to change the config as per the scenario and the business need in the country</t>
     </r>
   </si>
@@ -3528,6 +3528,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
+      <family val="1"/>
     </font>
     <font>
       <strike/>
@@ -4083,21 +4084,6 @@
     <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4114,6 +4100,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5418,17 +5419,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -6006,17 +6007,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -10612,17 +10613,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="127" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -10991,10 +10992,10 @@
   <dimension ref="A1:AMM33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -11012,17 +11013,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1027" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
     </row>
     <row r="2" spans="1:1027" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -20782,1040 +20783,1040 @@
       <c r="H27" s="36"/>
       <c r="I27" s="41"/>
     </row>
-    <row r="28" spans="1:1027" s="129" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
-      <c r="B28" s="126" t="s">
+    <row r="28" spans="1:1027" s="124" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="120"/>
+      <c r="B28" s="121" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="127" t="s">
+      <c r="C28" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="124"/>
-      <c r="E28" s="124"/>
-      <c r="F28" s="126" t="s">
+      <c r="D28" s="119"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="121" t="s">
         <v>348</v>
       </c>
-      <c r="G28" s="126"/>
-      <c r="H28" s="126"/>
-      <c r="I28" s="124"/>
-      <c r="J28" s="128"/>
-      <c r="K28" s="128"/>
-      <c r="L28" s="128"/>
-      <c r="M28" s="128"/>
-      <c r="N28" s="128"/>
-      <c r="O28" s="128"/>
-      <c r="P28" s="128"/>
-      <c r="Q28" s="128"/>
-      <c r="R28" s="128"/>
-      <c r="S28" s="128"/>
-      <c r="T28" s="128"/>
-      <c r="U28" s="128"/>
-      <c r="V28" s="128"/>
-      <c r="W28" s="128"/>
-      <c r="X28" s="128"/>
-      <c r="Y28" s="128"/>
-      <c r="Z28" s="128"/>
-      <c r="AA28" s="128"/>
-      <c r="AB28" s="128"/>
-      <c r="AC28" s="128"/>
-      <c r="AD28" s="128"/>
-      <c r="AE28" s="128"/>
-      <c r="AF28" s="128"/>
-      <c r="AG28" s="128"/>
-      <c r="AH28" s="128"/>
-      <c r="AI28" s="128"/>
-      <c r="AJ28" s="128"/>
-      <c r="AK28" s="128"/>
-      <c r="AL28" s="128"/>
-      <c r="AM28" s="128"/>
-      <c r="AN28" s="128"/>
-      <c r="AO28" s="128"/>
-      <c r="AP28" s="128"/>
-      <c r="AQ28" s="128"/>
-      <c r="AR28" s="128"/>
-      <c r="AS28" s="128"/>
-      <c r="AT28" s="128"/>
-      <c r="AU28" s="128"/>
-      <c r="AV28" s="128"/>
-      <c r="AW28" s="128"/>
-      <c r="AX28" s="128"/>
-      <c r="AY28" s="128"/>
-      <c r="AZ28" s="128"/>
-      <c r="BA28" s="128"/>
-      <c r="BB28" s="128"/>
-      <c r="BC28" s="128"/>
-      <c r="BD28" s="128"/>
-      <c r="BE28" s="128"/>
-      <c r="BF28" s="128"/>
-      <c r="BG28" s="128"/>
-      <c r="BH28" s="128"/>
-      <c r="BI28" s="128"/>
-      <c r="BJ28" s="128"/>
-      <c r="BK28" s="128"/>
-      <c r="BL28" s="128"/>
-      <c r="BM28" s="128"/>
-      <c r="BN28" s="128"/>
-      <c r="BO28" s="128"/>
-      <c r="BP28" s="128"/>
-      <c r="BQ28" s="128"/>
-      <c r="BR28" s="128"/>
-      <c r="BS28" s="128"/>
-      <c r="BT28" s="128"/>
-      <c r="BU28" s="128"/>
-      <c r="BV28" s="128"/>
-      <c r="BW28" s="128"/>
-      <c r="BX28" s="128"/>
-      <c r="BY28" s="128"/>
-      <c r="BZ28" s="128"/>
-      <c r="CA28" s="128"/>
-      <c r="CB28" s="128"/>
-      <c r="CC28" s="128"/>
-      <c r="CD28" s="128"/>
-      <c r="CE28" s="128"/>
-      <c r="CF28" s="128"/>
-      <c r="CG28" s="128"/>
-      <c r="CH28" s="128"/>
-      <c r="CI28" s="128"/>
-      <c r="CJ28" s="128"/>
-      <c r="CK28" s="128"/>
-      <c r="CL28" s="128"/>
-      <c r="CM28" s="128"/>
-      <c r="CN28" s="128"/>
-      <c r="CO28" s="128"/>
-      <c r="CP28" s="128"/>
-      <c r="CQ28" s="128"/>
-      <c r="CR28" s="128"/>
-      <c r="CS28" s="128"/>
-      <c r="CT28" s="128"/>
-      <c r="CU28" s="128"/>
-      <c r="CV28" s="128"/>
-      <c r="CW28" s="128"/>
-      <c r="CX28" s="128"/>
-      <c r="CY28" s="128"/>
-      <c r="CZ28" s="128"/>
-      <c r="DA28" s="128"/>
-      <c r="DB28" s="128"/>
-      <c r="DC28" s="128"/>
-      <c r="DD28" s="128"/>
-      <c r="DE28" s="128"/>
-      <c r="DF28" s="128"/>
-      <c r="DG28" s="128"/>
-      <c r="DH28" s="128"/>
-      <c r="DI28" s="128"/>
-      <c r="DJ28" s="128"/>
-      <c r="DK28" s="128"/>
-      <c r="DL28" s="128"/>
-      <c r="DM28" s="128"/>
-      <c r="DN28" s="128"/>
-      <c r="DO28" s="128"/>
-      <c r="DP28" s="128"/>
-      <c r="DQ28" s="128"/>
-      <c r="DR28" s="128"/>
-      <c r="DS28" s="128"/>
-      <c r="DT28" s="128"/>
-      <c r="DU28" s="128"/>
-      <c r="DV28" s="128"/>
-      <c r="DW28" s="128"/>
-      <c r="DX28" s="128"/>
-      <c r="DY28" s="128"/>
-      <c r="DZ28" s="128"/>
-      <c r="EA28" s="128"/>
-      <c r="EB28" s="128"/>
-      <c r="EC28" s="128"/>
-      <c r="ED28" s="128"/>
-      <c r="EE28" s="128"/>
-      <c r="EF28" s="128"/>
-      <c r="EG28" s="128"/>
-      <c r="EH28" s="128"/>
-      <c r="EI28" s="128"/>
-      <c r="EJ28" s="128"/>
-      <c r="EK28" s="128"/>
-      <c r="EL28" s="128"/>
-      <c r="EM28" s="128"/>
-      <c r="EN28" s="128"/>
-      <c r="EO28" s="128"/>
-      <c r="EP28" s="128"/>
-      <c r="EQ28" s="128"/>
-      <c r="ER28" s="128"/>
-      <c r="ES28" s="128"/>
-      <c r="ET28" s="128"/>
-      <c r="EU28" s="128"/>
-      <c r="EV28" s="128"/>
-      <c r="EW28" s="128"/>
-      <c r="EX28" s="128"/>
-      <c r="EY28" s="128"/>
-      <c r="EZ28" s="128"/>
-      <c r="FA28" s="128"/>
-      <c r="FB28" s="128"/>
-      <c r="FC28" s="128"/>
-      <c r="FD28" s="128"/>
-      <c r="FE28" s="128"/>
-      <c r="FF28" s="128"/>
-      <c r="FG28" s="128"/>
-      <c r="FH28" s="128"/>
-      <c r="FI28" s="128"/>
-      <c r="FJ28" s="128"/>
-      <c r="FK28" s="128"/>
-      <c r="FL28" s="128"/>
-      <c r="FM28" s="128"/>
-      <c r="FN28" s="128"/>
-      <c r="FO28" s="128"/>
-      <c r="FP28" s="128"/>
-      <c r="FQ28" s="128"/>
-      <c r="FR28" s="128"/>
-      <c r="FS28" s="128"/>
-      <c r="FT28" s="128"/>
-      <c r="FU28" s="128"/>
-      <c r="FV28" s="128"/>
-      <c r="FW28" s="128"/>
-      <c r="FX28" s="128"/>
-      <c r="FY28" s="128"/>
-      <c r="FZ28" s="128"/>
-      <c r="GA28" s="128"/>
-      <c r="GB28" s="128"/>
-      <c r="GC28" s="128"/>
-      <c r="GD28" s="128"/>
-      <c r="GE28" s="128"/>
-      <c r="GF28" s="128"/>
-      <c r="GG28" s="128"/>
-      <c r="GH28" s="128"/>
-      <c r="GI28" s="128"/>
-      <c r="GJ28" s="128"/>
-      <c r="GK28" s="128"/>
-      <c r="GL28" s="128"/>
-      <c r="GM28" s="128"/>
-      <c r="GN28" s="128"/>
-      <c r="GO28" s="128"/>
-      <c r="GP28" s="128"/>
-      <c r="GQ28" s="128"/>
-      <c r="GR28" s="128"/>
-      <c r="GS28" s="128"/>
-      <c r="GT28" s="128"/>
-      <c r="GU28" s="128"/>
-      <c r="GV28" s="128"/>
-      <c r="GW28" s="128"/>
-      <c r="GX28" s="128"/>
-      <c r="GY28" s="128"/>
-      <c r="GZ28" s="128"/>
-      <c r="HA28" s="128"/>
-      <c r="HB28" s="128"/>
-      <c r="HC28" s="128"/>
-      <c r="HD28" s="128"/>
-      <c r="HE28" s="128"/>
-      <c r="HF28" s="128"/>
-      <c r="HG28" s="128"/>
-      <c r="HH28" s="128"/>
-      <c r="HI28" s="128"/>
-      <c r="HJ28" s="128"/>
-      <c r="HK28" s="128"/>
-      <c r="HL28" s="128"/>
-      <c r="HM28" s="128"/>
-      <c r="HN28" s="128"/>
-      <c r="HO28" s="128"/>
-      <c r="HP28" s="128"/>
-      <c r="HQ28" s="128"/>
-      <c r="HR28" s="128"/>
-      <c r="HS28" s="128"/>
-      <c r="HT28" s="128"/>
-      <c r="HU28" s="128"/>
-      <c r="HV28" s="128"/>
-      <c r="HW28" s="128"/>
-      <c r="HX28" s="128"/>
-      <c r="HY28" s="128"/>
-      <c r="HZ28" s="128"/>
-      <c r="IA28" s="128"/>
-      <c r="IB28" s="128"/>
-      <c r="IC28" s="128"/>
-      <c r="ID28" s="128"/>
-      <c r="IE28" s="128"/>
-      <c r="IF28" s="128"/>
-      <c r="IG28" s="128"/>
-      <c r="IH28" s="128"/>
-      <c r="II28" s="128"/>
-      <c r="IJ28" s="128"/>
-      <c r="IK28" s="128"/>
-      <c r="IL28" s="128"/>
-      <c r="IM28" s="128"/>
-      <c r="IN28" s="128"/>
-      <c r="IO28" s="128"/>
-      <c r="IP28" s="128"/>
-      <c r="IQ28" s="128"/>
-      <c r="IR28" s="128"/>
-      <c r="IS28" s="128"/>
-      <c r="IT28" s="128"/>
-      <c r="IU28" s="128"/>
-      <c r="IV28" s="128"/>
-      <c r="IW28" s="128"/>
-      <c r="IX28" s="128"/>
-      <c r="IY28" s="128"/>
-      <c r="IZ28" s="128"/>
-      <c r="JA28" s="128"/>
-      <c r="JB28" s="128"/>
-      <c r="JC28" s="128"/>
-      <c r="JD28" s="128"/>
-      <c r="JE28" s="128"/>
-      <c r="JF28" s="128"/>
-      <c r="JG28" s="128"/>
-      <c r="JH28" s="128"/>
-      <c r="JI28" s="128"/>
-      <c r="JJ28" s="128"/>
-      <c r="JK28" s="128"/>
-      <c r="JL28" s="128"/>
-      <c r="JM28" s="128"/>
-      <c r="JN28" s="128"/>
-      <c r="JO28" s="128"/>
-      <c r="JP28" s="128"/>
-      <c r="JQ28" s="128"/>
-      <c r="JR28" s="128"/>
-      <c r="JS28" s="128"/>
-      <c r="JT28" s="128"/>
-      <c r="JU28" s="128"/>
-      <c r="JV28" s="128"/>
-      <c r="JW28" s="128"/>
-      <c r="JX28" s="128"/>
-      <c r="JY28" s="128"/>
-      <c r="JZ28" s="128"/>
-      <c r="KA28" s="128"/>
-      <c r="KB28" s="128"/>
-      <c r="KC28" s="128"/>
-      <c r="KD28" s="128"/>
-      <c r="KE28" s="128"/>
-      <c r="KF28" s="128"/>
-      <c r="KG28" s="128"/>
-      <c r="KH28" s="128"/>
-      <c r="KI28" s="128"/>
-      <c r="KJ28" s="128"/>
-      <c r="KK28" s="128"/>
-      <c r="KL28" s="128"/>
-      <c r="KM28" s="128"/>
-      <c r="KN28" s="128"/>
-      <c r="KO28" s="128"/>
-      <c r="KP28" s="128"/>
-      <c r="KQ28" s="128"/>
-      <c r="KR28" s="128"/>
-      <c r="KS28" s="128"/>
-      <c r="KT28" s="128"/>
-      <c r="KU28" s="128"/>
-      <c r="KV28" s="128"/>
-      <c r="KW28" s="128"/>
-      <c r="KX28" s="128"/>
-      <c r="KY28" s="128"/>
-      <c r="KZ28" s="128"/>
-      <c r="LA28" s="128"/>
-      <c r="LB28" s="128"/>
-      <c r="LC28" s="128"/>
-      <c r="LD28" s="128"/>
-      <c r="LE28" s="128"/>
-      <c r="LF28" s="128"/>
-      <c r="LG28" s="128"/>
-      <c r="LH28" s="128"/>
-      <c r="LI28" s="128"/>
-      <c r="LJ28" s="128"/>
-      <c r="LK28" s="128"/>
-      <c r="LL28" s="128"/>
-      <c r="LM28" s="128"/>
-      <c r="LN28" s="128"/>
-      <c r="LO28" s="128"/>
-      <c r="LP28" s="128"/>
-      <c r="LQ28" s="128"/>
-      <c r="LR28" s="128"/>
-      <c r="LS28" s="128"/>
-      <c r="LT28" s="128"/>
-      <c r="LU28" s="128"/>
-      <c r="LV28" s="128"/>
-      <c r="LW28" s="128"/>
-      <c r="LX28" s="128"/>
-      <c r="LY28" s="128"/>
-      <c r="LZ28" s="128"/>
-      <c r="MA28" s="128"/>
-      <c r="MB28" s="128"/>
-      <c r="MC28" s="128"/>
-      <c r="MD28" s="128"/>
-      <c r="ME28" s="128"/>
-      <c r="MF28" s="128"/>
-      <c r="MG28" s="128"/>
-      <c r="MH28" s="128"/>
-      <c r="MI28" s="128"/>
-      <c r="MJ28" s="128"/>
-      <c r="MK28" s="128"/>
-      <c r="ML28" s="128"/>
-      <c r="MM28" s="128"/>
-      <c r="MN28" s="128"/>
-      <c r="MO28" s="128"/>
-      <c r="MP28" s="128"/>
-      <c r="MQ28" s="128"/>
-      <c r="MR28" s="128"/>
-      <c r="MS28" s="128"/>
-      <c r="MT28" s="128"/>
-      <c r="MU28" s="128"/>
-      <c r="MV28" s="128"/>
-      <c r="MW28" s="128"/>
-      <c r="MX28" s="128"/>
-      <c r="MY28" s="128"/>
-      <c r="MZ28" s="128"/>
-      <c r="NA28" s="128"/>
-      <c r="NB28" s="128"/>
-      <c r="NC28" s="128"/>
-      <c r="ND28" s="128"/>
-      <c r="NE28" s="128"/>
-      <c r="NF28" s="128"/>
-      <c r="NG28" s="128"/>
-      <c r="NH28" s="128"/>
-      <c r="NI28" s="128"/>
-      <c r="NJ28" s="128"/>
-      <c r="NK28" s="128"/>
-      <c r="NL28" s="128"/>
-      <c r="NM28" s="128"/>
-      <c r="NN28" s="128"/>
-      <c r="NO28" s="128"/>
-      <c r="NP28" s="128"/>
-      <c r="NQ28" s="128"/>
-      <c r="NR28" s="128"/>
-      <c r="NS28" s="128"/>
-      <c r="NT28" s="128"/>
-      <c r="NU28" s="128"/>
-      <c r="NV28" s="128"/>
-      <c r="NW28" s="128"/>
-      <c r="NX28" s="128"/>
-      <c r="NY28" s="128"/>
-      <c r="NZ28" s="128"/>
-      <c r="OA28" s="128"/>
-      <c r="OB28" s="128"/>
-      <c r="OC28" s="128"/>
-      <c r="OD28" s="128"/>
-      <c r="OE28" s="128"/>
-      <c r="OF28" s="128"/>
-      <c r="OG28" s="128"/>
-      <c r="OH28" s="128"/>
-      <c r="OI28" s="128"/>
-      <c r="OJ28" s="128"/>
-      <c r="OK28" s="128"/>
-      <c r="OL28" s="128"/>
-      <c r="OM28" s="128"/>
-      <c r="ON28" s="128"/>
-      <c r="OO28" s="128"/>
-      <c r="OP28" s="128"/>
-      <c r="OQ28" s="128"/>
-      <c r="OR28" s="128"/>
-      <c r="OS28" s="128"/>
-      <c r="OT28" s="128"/>
-      <c r="OU28" s="128"/>
-      <c r="OV28" s="128"/>
-      <c r="OW28" s="128"/>
-      <c r="OX28" s="128"/>
-      <c r="OY28" s="128"/>
-      <c r="OZ28" s="128"/>
-      <c r="PA28" s="128"/>
-      <c r="PB28" s="128"/>
-      <c r="PC28" s="128"/>
-      <c r="PD28" s="128"/>
-      <c r="PE28" s="128"/>
-      <c r="PF28" s="128"/>
-      <c r="PG28" s="128"/>
-      <c r="PH28" s="128"/>
-      <c r="PI28" s="128"/>
-      <c r="PJ28" s="128"/>
-      <c r="PK28" s="128"/>
-      <c r="PL28" s="128"/>
-      <c r="PM28" s="128"/>
-      <c r="PN28" s="128"/>
-      <c r="PO28" s="128"/>
-      <c r="PP28" s="128"/>
-      <c r="PQ28" s="128"/>
-      <c r="PR28" s="128"/>
-      <c r="PS28" s="128"/>
-      <c r="PT28" s="128"/>
-      <c r="PU28" s="128"/>
-      <c r="PV28" s="128"/>
-      <c r="PW28" s="128"/>
-      <c r="PX28" s="128"/>
-      <c r="PY28" s="128"/>
-      <c r="PZ28" s="128"/>
-      <c r="QA28" s="128"/>
-      <c r="QB28" s="128"/>
-      <c r="QC28" s="128"/>
-      <c r="QD28" s="128"/>
-      <c r="QE28" s="128"/>
-      <c r="QF28" s="128"/>
-      <c r="QG28" s="128"/>
-      <c r="QH28" s="128"/>
-      <c r="QI28" s="128"/>
-      <c r="QJ28" s="128"/>
-      <c r="QK28" s="128"/>
-      <c r="QL28" s="128"/>
-      <c r="QM28" s="128"/>
-      <c r="QN28" s="128"/>
-      <c r="QO28" s="128"/>
-      <c r="QP28" s="128"/>
-      <c r="QQ28" s="128"/>
-      <c r="QR28" s="128"/>
-      <c r="QS28" s="128"/>
-      <c r="QT28" s="128"/>
-      <c r="QU28" s="128"/>
-      <c r="QV28" s="128"/>
-      <c r="QW28" s="128"/>
-      <c r="QX28" s="128"/>
-      <c r="QY28" s="128"/>
-      <c r="QZ28" s="128"/>
-      <c r="RA28" s="128"/>
-      <c r="RB28" s="128"/>
-      <c r="RC28" s="128"/>
-      <c r="RD28" s="128"/>
-      <c r="RE28" s="128"/>
-      <c r="RF28" s="128"/>
-      <c r="RG28" s="128"/>
-      <c r="RH28" s="128"/>
-      <c r="RI28" s="128"/>
-      <c r="RJ28" s="128"/>
-      <c r="RK28" s="128"/>
-      <c r="RL28" s="128"/>
-      <c r="RM28" s="128"/>
-      <c r="RN28" s="128"/>
-      <c r="RO28" s="128"/>
-      <c r="RP28" s="128"/>
-      <c r="RQ28" s="128"/>
-      <c r="RR28" s="128"/>
-      <c r="RS28" s="128"/>
-      <c r="RT28" s="128"/>
-      <c r="RU28" s="128"/>
-      <c r="RV28" s="128"/>
-      <c r="RW28" s="128"/>
-      <c r="RX28" s="128"/>
-      <c r="RY28" s="128"/>
-      <c r="RZ28" s="128"/>
-      <c r="SA28" s="128"/>
-      <c r="SB28" s="128"/>
-      <c r="SC28" s="128"/>
-      <c r="SD28" s="128"/>
-      <c r="SE28" s="128"/>
-      <c r="SF28" s="128"/>
-      <c r="SG28" s="128"/>
-      <c r="SH28" s="128"/>
-      <c r="SI28" s="128"/>
-      <c r="SJ28" s="128"/>
-      <c r="SK28" s="128"/>
-      <c r="SL28" s="128"/>
-      <c r="SM28" s="128"/>
-      <c r="SN28" s="128"/>
-      <c r="SO28" s="128"/>
-      <c r="SP28" s="128"/>
-      <c r="SQ28" s="128"/>
-      <c r="SR28" s="128"/>
-      <c r="SS28" s="128"/>
-      <c r="ST28" s="128"/>
-      <c r="SU28" s="128"/>
-      <c r="SV28" s="128"/>
-      <c r="SW28" s="128"/>
-      <c r="SX28" s="128"/>
-      <c r="SY28" s="128"/>
-      <c r="SZ28" s="128"/>
-      <c r="TA28" s="128"/>
-      <c r="TB28" s="128"/>
-      <c r="TC28" s="128"/>
-      <c r="TD28" s="128"/>
-      <c r="TE28" s="128"/>
-      <c r="TF28" s="128"/>
-      <c r="TG28" s="128"/>
-      <c r="TH28" s="128"/>
-      <c r="TI28" s="128"/>
-      <c r="TJ28" s="128"/>
-      <c r="TK28" s="128"/>
-      <c r="TL28" s="128"/>
-      <c r="TM28" s="128"/>
-      <c r="TN28" s="128"/>
-      <c r="TO28" s="128"/>
-      <c r="TP28" s="128"/>
-      <c r="TQ28" s="128"/>
-      <c r="TR28" s="128"/>
-      <c r="TS28" s="128"/>
-      <c r="TT28" s="128"/>
-      <c r="TU28" s="128"/>
-      <c r="TV28" s="128"/>
-      <c r="TW28" s="128"/>
-      <c r="TX28" s="128"/>
-      <c r="TY28" s="128"/>
-      <c r="TZ28" s="128"/>
-      <c r="UA28" s="128"/>
-      <c r="UB28" s="128"/>
-      <c r="UC28" s="128"/>
-      <c r="UD28" s="128"/>
-      <c r="UE28" s="128"/>
-      <c r="UF28" s="128"/>
-      <c r="UG28" s="128"/>
-      <c r="UH28" s="128"/>
-      <c r="UI28" s="128"/>
-      <c r="UJ28" s="128"/>
-      <c r="UK28" s="128"/>
-      <c r="UL28" s="128"/>
-      <c r="UM28" s="128"/>
-      <c r="UN28" s="128"/>
-      <c r="UO28" s="128"/>
-      <c r="UP28" s="128"/>
-      <c r="UQ28" s="128"/>
-      <c r="UR28" s="128"/>
-      <c r="US28" s="128"/>
-      <c r="UT28" s="128"/>
-      <c r="UU28" s="128"/>
-      <c r="UV28" s="128"/>
-      <c r="UW28" s="128"/>
-      <c r="UX28" s="128"/>
-      <c r="UY28" s="128"/>
-      <c r="UZ28" s="128"/>
-      <c r="VA28" s="128"/>
-      <c r="VB28" s="128"/>
-      <c r="VC28" s="128"/>
-      <c r="VD28" s="128"/>
-      <c r="VE28" s="128"/>
-      <c r="VF28" s="128"/>
-      <c r="VG28" s="128"/>
-      <c r="VH28" s="128"/>
-      <c r="VI28" s="128"/>
-      <c r="VJ28" s="128"/>
-      <c r="VK28" s="128"/>
-      <c r="VL28" s="128"/>
-      <c r="VM28" s="128"/>
-      <c r="VN28" s="128"/>
-      <c r="VO28" s="128"/>
-      <c r="VP28" s="128"/>
-      <c r="VQ28" s="128"/>
-      <c r="VR28" s="128"/>
-      <c r="VS28" s="128"/>
-      <c r="VT28" s="128"/>
-      <c r="VU28" s="128"/>
-      <c r="VV28" s="128"/>
-      <c r="VW28" s="128"/>
-      <c r="VX28" s="128"/>
-      <c r="VY28" s="128"/>
-      <c r="VZ28" s="128"/>
-      <c r="WA28" s="128"/>
-      <c r="WB28" s="128"/>
-      <c r="WC28" s="128"/>
-      <c r="WD28" s="128"/>
-      <c r="WE28" s="128"/>
-      <c r="WF28" s="128"/>
-      <c r="WG28" s="128"/>
-      <c r="WH28" s="128"/>
-      <c r="WI28" s="128"/>
-      <c r="WJ28" s="128"/>
-      <c r="WK28" s="128"/>
-      <c r="WL28" s="128"/>
-      <c r="WM28" s="128"/>
-      <c r="WN28" s="128"/>
-      <c r="WO28" s="128"/>
-      <c r="WP28" s="128"/>
-      <c r="WQ28" s="128"/>
-      <c r="WR28" s="128"/>
-      <c r="WS28" s="128"/>
-      <c r="WT28" s="128"/>
-      <c r="WU28" s="128"/>
-      <c r="WV28" s="128"/>
-      <c r="WW28" s="128"/>
-      <c r="WX28" s="128"/>
-      <c r="WY28" s="128"/>
-      <c r="WZ28" s="128"/>
-      <c r="XA28" s="128"/>
-      <c r="XB28" s="128"/>
-      <c r="XC28" s="128"/>
-      <c r="XD28" s="128"/>
-      <c r="XE28" s="128"/>
-      <c r="XF28" s="128"/>
-      <c r="XG28" s="128"/>
-      <c r="XH28" s="128"/>
-      <c r="XI28" s="128"/>
-      <c r="XJ28" s="128"/>
-      <c r="XK28" s="128"/>
-      <c r="XL28" s="128"/>
-      <c r="XM28" s="128"/>
-      <c r="XN28" s="128"/>
-      <c r="XO28" s="128"/>
-      <c r="XP28" s="128"/>
-      <c r="XQ28" s="128"/>
-      <c r="XR28" s="128"/>
-      <c r="XS28" s="128"/>
-      <c r="XT28" s="128"/>
-      <c r="XU28" s="128"/>
-      <c r="XV28" s="128"/>
-      <c r="XW28" s="128"/>
-      <c r="XX28" s="128"/>
-      <c r="XY28" s="128"/>
-      <c r="XZ28" s="128"/>
-      <c r="YA28" s="128"/>
-      <c r="YB28" s="128"/>
-      <c r="YC28" s="128"/>
-      <c r="YD28" s="128"/>
-      <c r="YE28" s="128"/>
-      <c r="YF28" s="128"/>
-      <c r="YG28" s="128"/>
-      <c r="YH28" s="128"/>
-      <c r="YI28" s="128"/>
-      <c r="YJ28" s="128"/>
-      <c r="YK28" s="128"/>
-      <c r="YL28" s="128"/>
-      <c r="YM28" s="128"/>
-      <c r="YN28" s="128"/>
-      <c r="YO28" s="128"/>
-      <c r="YP28" s="128"/>
-      <c r="YQ28" s="128"/>
-      <c r="YR28" s="128"/>
-      <c r="YS28" s="128"/>
-      <c r="YT28" s="128"/>
-      <c r="YU28" s="128"/>
-      <c r="YV28" s="128"/>
-      <c r="YW28" s="128"/>
-      <c r="YX28" s="128"/>
-      <c r="YY28" s="128"/>
-      <c r="YZ28" s="128"/>
-      <c r="ZA28" s="128"/>
-      <c r="ZB28" s="128"/>
-      <c r="ZC28" s="128"/>
-      <c r="ZD28" s="128"/>
-      <c r="ZE28" s="128"/>
-      <c r="ZF28" s="128"/>
-      <c r="ZG28" s="128"/>
-      <c r="ZH28" s="128"/>
-      <c r="ZI28" s="128"/>
-      <c r="ZJ28" s="128"/>
-      <c r="ZK28" s="128"/>
-      <c r="ZL28" s="128"/>
-      <c r="ZM28" s="128"/>
-      <c r="ZN28" s="128"/>
-      <c r="ZO28" s="128"/>
-      <c r="ZP28" s="128"/>
-      <c r="ZQ28" s="128"/>
-      <c r="ZR28" s="128"/>
-      <c r="ZS28" s="128"/>
-      <c r="ZT28" s="128"/>
-      <c r="ZU28" s="128"/>
-      <c r="ZV28" s="128"/>
-      <c r="ZW28" s="128"/>
-      <c r="ZX28" s="128"/>
-      <c r="ZY28" s="128"/>
-      <c r="ZZ28" s="128"/>
-      <c r="AAA28" s="128"/>
-      <c r="AAB28" s="128"/>
-      <c r="AAC28" s="128"/>
-      <c r="AAD28" s="128"/>
-      <c r="AAE28" s="128"/>
-      <c r="AAF28" s="128"/>
-      <c r="AAG28" s="128"/>
-      <c r="AAH28" s="128"/>
-      <c r="AAI28" s="128"/>
-      <c r="AAJ28" s="128"/>
-      <c r="AAK28" s="128"/>
-      <c r="AAL28" s="128"/>
-      <c r="AAM28" s="128"/>
-      <c r="AAN28" s="128"/>
-      <c r="AAO28" s="128"/>
-      <c r="AAP28" s="128"/>
-      <c r="AAQ28" s="128"/>
-      <c r="AAR28" s="128"/>
-      <c r="AAS28" s="128"/>
-      <c r="AAT28" s="128"/>
-      <c r="AAU28" s="128"/>
-      <c r="AAV28" s="128"/>
-      <c r="AAW28" s="128"/>
-      <c r="AAX28" s="128"/>
-      <c r="AAY28" s="128"/>
-      <c r="AAZ28" s="128"/>
-      <c r="ABA28" s="128"/>
-      <c r="ABB28" s="128"/>
-      <c r="ABC28" s="128"/>
-      <c r="ABD28" s="128"/>
-      <c r="ABE28" s="128"/>
-      <c r="ABF28" s="128"/>
-      <c r="ABG28" s="128"/>
-      <c r="ABH28" s="128"/>
-      <c r="ABI28" s="128"/>
-      <c r="ABJ28" s="128"/>
-      <c r="ABK28" s="128"/>
-      <c r="ABL28" s="128"/>
-      <c r="ABM28" s="128"/>
-      <c r="ABN28" s="128"/>
-      <c r="ABO28" s="128"/>
-      <c r="ABP28" s="128"/>
-      <c r="ABQ28" s="128"/>
-      <c r="ABR28" s="128"/>
-      <c r="ABS28" s="128"/>
-      <c r="ABT28" s="128"/>
-      <c r="ABU28" s="128"/>
-      <c r="ABV28" s="128"/>
-      <c r="ABW28" s="128"/>
-      <c r="ABX28" s="128"/>
-      <c r="ABY28" s="128"/>
-      <c r="ABZ28" s="128"/>
-      <c r="ACA28" s="128"/>
-      <c r="ACB28" s="128"/>
-      <c r="ACC28" s="128"/>
-      <c r="ACD28" s="128"/>
-      <c r="ACE28" s="128"/>
-      <c r="ACF28" s="128"/>
-      <c r="ACG28" s="128"/>
-      <c r="ACH28" s="128"/>
-      <c r="ACI28" s="128"/>
-      <c r="ACJ28" s="128"/>
-      <c r="ACK28" s="128"/>
-      <c r="ACL28" s="128"/>
-      <c r="ACM28" s="128"/>
-      <c r="ACN28" s="128"/>
-      <c r="ACO28" s="128"/>
-      <c r="ACP28" s="128"/>
-      <c r="ACQ28" s="128"/>
-      <c r="ACR28" s="128"/>
-      <c r="ACS28" s="128"/>
-      <c r="ACT28" s="128"/>
-      <c r="ACU28" s="128"/>
-      <c r="ACV28" s="128"/>
-      <c r="ACW28" s="128"/>
-      <c r="ACX28" s="128"/>
-      <c r="ACY28" s="128"/>
-      <c r="ACZ28" s="128"/>
-      <c r="ADA28" s="128"/>
-      <c r="ADB28" s="128"/>
-      <c r="ADC28" s="128"/>
-      <c r="ADD28" s="128"/>
-      <c r="ADE28" s="128"/>
-      <c r="ADF28" s="128"/>
-      <c r="ADG28" s="128"/>
-      <c r="ADH28" s="128"/>
-      <c r="ADI28" s="128"/>
-      <c r="ADJ28" s="128"/>
-      <c r="ADK28" s="128"/>
-      <c r="ADL28" s="128"/>
-      <c r="ADM28" s="128"/>
-      <c r="ADN28" s="128"/>
-      <c r="ADO28" s="128"/>
-      <c r="ADP28" s="128"/>
-      <c r="ADQ28" s="128"/>
-      <c r="ADR28" s="128"/>
-      <c r="ADS28" s="128"/>
-      <c r="ADT28" s="128"/>
-      <c r="ADU28" s="128"/>
-      <c r="ADV28" s="128"/>
-      <c r="ADW28" s="128"/>
-      <c r="ADX28" s="128"/>
-      <c r="ADY28" s="128"/>
-      <c r="ADZ28" s="128"/>
-      <c r="AEA28" s="128"/>
-      <c r="AEB28" s="128"/>
-      <c r="AEC28" s="128"/>
-      <c r="AED28" s="128"/>
-      <c r="AEE28" s="128"/>
-      <c r="AEF28" s="128"/>
-      <c r="AEG28" s="128"/>
-      <c r="AEH28" s="128"/>
-      <c r="AEI28" s="128"/>
-      <c r="AEJ28" s="128"/>
-      <c r="AEK28" s="128"/>
-      <c r="AEL28" s="128"/>
-      <c r="AEM28" s="128"/>
-      <c r="AEN28" s="128"/>
-      <c r="AEO28" s="128"/>
-      <c r="AEP28" s="128"/>
-      <c r="AEQ28" s="128"/>
-      <c r="AER28" s="128"/>
-      <c r="AES28" s="128"/>
-      <c r="AET28" s="128"/>
-      <c r="AEU28" s="128"/>
-      <c r="AEV28" s="128"/>
-      <c r="AEW28" s="128"/>
-      <c r="AEX28" s="128"/>
-      <c r="AEY28" s="128"/>
-      <c r="AEZ28" s="128"/>
-      <c r="AFA28" s="128"/>
-      <c r="AFB28" s="128"/>
-      <c r="AFC28" s="128"/>
-      <c r="AFD28" s="128"/>
-      <c r="AFE28" s="128"/>
-      <c r="AFF28" s="128"/>
-      <c r="AFG28" s="128"/>
-      <c r="AFH28" s="128"/>
-      <c r="AFI28" s="128"/>
-      <c r="AFJ28" s="128"/>
-      <c r="AFK28" s="128"/>
-      <c r="AFL28" s="128"/>
-      <c r="AFM28" s="128"/>
-      <c r="AFN28" s="128"/>
-      <c r="AFO28" s="128"/>
-      <c r="AFP28" s="128"/>
-      <c r="AFQ28" s="128"/>
-      <c r="AFR28" s="128"/>
-      <c r="AFS28" s="128"/>
-      <c r="AFT28" s="128"/>
-      <c r="AFU28" s="128"/>
-      <c r="AFV28" s="128"/>
-      <c r="AFW28" s="128"/>
-      <c r="AFX28" s="128"/>
-      <c r="AFY28" s="128"/>
-      <c r="AFZ28" s="128"/>
-      <c r="AGA28" s="128"/>
-      <c r="AGB28" s="128"/>
-      <c r="AGC28" s="128"/>
-      <c r="AGD28" s="128"/>
-      <c r="AGE28" s="128"/>
-      <c r="AGF28" s="128"/>
-      <c r="AGG28" s="128"/>
-      <c r="AGH28" s="128"/>
-      <c r="AGI28" s="128"/>
-      <c r="AGJ28" s="128"/>
-      <c r="AGK28" s="128"/>
-      <c r="AGL28" s="128"/>
-      <c r="AGM28" s="128"/>
-      <c r="AGN28" s="128"/>
-      <c r="AGO28" s="128"/>
-      <c r="AGP28" s="128"/>
-      <c r="AGQ28" s="128"/>
-      <c r="AGR28" s="128"/>
-      <c r="AGS28" s="128"/>
-      <c r="AGT28" s="128"/>
-      <c r="AGU28" s="128"/>
-      <c r="AGV28" s="128"/>
-      <c r="AGW28" s="128"/>
-      <c r="AGX28" s="128"/>
-      <c r="AGY28" s="128"/>
-      <c r="AGZ28" s="128"/>
-      <c r="AHA28" s="128"/>
-      <c r="AHB28" s="128"/>
-      <c r="AHC28" s="128"/>
-      <c r="AHD28" s="128"/>
-      <c r="AHE28" s="128"/>
-      <c r="AHF28" s="128"/>
-      <c r="AHG28" s="128"/>
-      <c r="AHH28" s="128"/>
-      <c r="AHI28" s="128"/>
-      <c r="AHJ28" s="128"/>
-      <c r="AHK28" s="128"/>
-      <c r="AHL28" s="128"/>
-      <c r="AHM28" s="128"/>
-      <c r="AHN28" s="128"/>
-      <c r="AHO28" s="128"/>
-      <c r="AHP28" s="128"/>
-      <c r="AHQ28" s="128"/>
-      <c r="AHR28" s="128"/>
-      <c r="AHS28" s="128"/>
-      <c r="AHT28" s="128"/>
-      <c r="AHU28" s="128"/>
-      <c r="AHV28" s="128"/>
-      <c r="AHW28" s="128"/>
-      <c r="AHX28" s="128"/>
-      <c r="AHY28" s="128"/>
-      <c r="AHZ28" s="128"/>
-      <c r="AIA28" s="128"/>
-      <c r="AIB28" s="128"/>
-      <c r="AIC28" s="128"/>
-      <c r="AID28" s="128"/>
-      <c r="AIE28" s="128"/>
-      <c r="AIF28" s="128"/>
-      <c r="AIG28" s="128"/>
-      <c r="AIH28" s="128"/>
-      <c r="AII28" s="128"/>
-      <c r="AIJ28" s="128"/>
-      <c r="AIK28" s="128"/>
-      <c r="AIL28" s="128"/>
-      <c r="AIM28" s="128"/>
-      <c r="AIN28" s="128"/>
-      <c r="AIO28" s="128"/>
-      <c r="AIP28" s="128"/>
-      <c r="AIQ28" s="128"/>
-      <c r="AIR28" s="128"/>
-      <c r="AIS28" s="128"/>
-      <c r="AIT28" s="128"/>
-      <c r="AIU28" s="128"/>
-      <c r="AIV28" s="128"/>
-      <c r="AIW28" s="128"/>
-      <c r="AIX28" s="128"/>
-      <c r="AIY28" s="128"/>
-      <c r="AIZ28" s="128"/>
-      <c r="AJA28" s="128"/>
-      <c r="AJB28" s="128"/>
-      <c r="AJC28" s="128"/>
-      <c r="AJD28" s="128"/>
-      <c r="AJE28" s="128"/>
-      <c r="AJF28" s="128"/>
-      <c r="AJG28" s="128"/>
-      <c r="AJH28" s="128"/>
-      <c r="AJI28" s="128"/>
-      <c r="AJJ28" s="128"/>
-      <c r="AJK28" s="128"/>
-      <c r="AJL28" s="128"/>
-      <c r="AJM28" s="128"/>
-      <c r="AJN28" s="128"/>
-      <c r="AJO28" s="128"/>
-      <c r="AJP28" s="128"/>
-      <c r="AJQ28" s="128"/>
-      <c r="AJR28" s="128"/>
-      <c r="AJS28" s="128"/>
-      <c r="AJT28" s="128"/>
-      <c r="AJU28" s="128"/>
-      <c r="AJV28" s="128"/>
-      <c r="AJW28" s="128"/>
-      <c r="AJX28" s="128"/>
-      <c r="AJY28" s="128"/>
-      <c r="AJZ28" s="128"/>
-      <c r="AKA28" s="128"/>
-      <c r="AKB28" s="128"/>
-      <c r="AKC28" s="128"/>
-      <c r="AKD28" s="128"/>
-      <c r="AKE28" s="128"/>
-      <c r="AKF28" s="128"/>
-      <c r="AKG28" s="128"/>
-      <c r="AKH28" s="128"/>
-      <c r="AKI28" s="128"/>
-      <c r="AKJ28" s="128"/>
-      <c r="AKK28" s="128"/>
-      <c r="AKL28" s="128"/>
-      <c r="AKM28" s="128"/>
-      <c r="AKN28" s="128"/>
-      <c r="AKO28" s="128"/>
-      <c r="AKP28" s="128"/>
-      <c r="AKQ28" s="128"/>
-      <c r="AKR28" s="128"/>
-      <c r="AKS28" s="128"/>
-      <c r="AKT28" s="128"/>
-      <c r="AKU28" s="128"/>
-      <c r="AKV28" s="128"/>
-      <c r="AKW28" s="128"/>
-      <c r="AKX28" s="128"/>
-      <c r="AKY28" s="128"/>
-      <c r="AKZ28" s="128"/>
-      <c r="ALA28" s="128"/>
-      <c r="ALB28" s="128"/>
-      <c r="ALC28" s="128"/>
-      <c r="ALD28" s="128"/>
-      <c r="ALE28" s="128"/>
-      <c r="ALF28" s="128"/>
-      <c r="ALG28" s="128"/>
-      <c r="ALH28" s="128"/>
-      <c r="ALI28" s="128"/>
-      <c r="ALJ28" s="128"/>
-      <c r="ALK28" s="128"/>
-      <c r="ALL28" s="128"/>
-      <c r="ALM28" s="128"/>
-      <c r="ALN28" s="128"/>
-      <c r="ALO28" s="128"/>
-      <c r="ALP28" s="128"/>
-      <c r="ALQ28" s="128"/>
-      <c r="ALR28" s="128"/>
-      <c r="ALS28" s="128"/>
-      <c r="ALT28" s="128"/>
-      <c r="ALU28" s="128"/>
-      <c r="ALV28" s="128"/>
-      <c r="ALW28" s="128"/>
-      <c r="ALX28" s="128"/>
-      <c r="ALY28" s="128"/>
-      <c r="ALZ28" s="128"/>
-      <c r="AMA28" s="128"/>
-      <c r="AMB28" s="128"/>
-      <c r="AMC28" s="128"/>
-      <c r="AMD28" s="128"/>
-      <c r="AME28" s="128"/>
-      <c r="AMF28" s="128"/>
-      <c r="AMG28" s="128"/>
-      <c r="AMH28" s="128"/>
-      <c r="AMI28" s="128"/>
-      <c r="AMJ28" s="128"/>
-      <c r="AMK28" s="128"/>
-      <c r="AML28" s="128"/>
-      <c r="AMM28" s="128"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="119"/>
+      <c r="J28" s="123"/>
+      <c r="K28" s="123"/>
+      <c r="L28" s="123"/>
+      <c r="M28" s="123"/>
+      <c r="N28" s="123"/>
+      <c r="O28" s="123"/>
+      <c r="P28" s="123"/>
+      <c r="Q28" s="123"/>
+      <c r="R28" s="123"/>
+      <c r="S28" s="123"/>
+      <c r="T28" s="123"/>
+      <c r="U28" s="123"/>
+      <c r="V28" s="123"/>
+      <c r="W28" s="123"/>
+      <c r="X28" s="123"/>
+      <c r="Y28" s="123"/>
+      <c r="Z28" s="123"/>
+      <c r="AA28" s="123"/>
+      <c r="AB28" s="123"/>
+      <c r="AC28" s="123"/>
+      <c r="AD28" s="123"/>
+      <c r="AE28" s="123"/>
+      <c r="AF28" s="123"/>
+      <c r="AG28" s="123"/>
+      <c r="AH28" s="123"/>
+      <c r="AI28" s="123"/>
+      <c r="AJ28" s="123"/>
+      <c r="AK28" s="123"/>
+      <c r="AL28" s="123"/>
+      <c r="AM28" s="123"/>
+      <c r="AN28" s="123"/>
+      <c r="AO28" s="123"/>
+      <c r="AP28" s="123"/>
+      <c r="AQ28" s="123"/>
+      <c r="AR28" s="123"/>
+      <c r="AS28" s="123"/>
+      <c r="AT28" s="123"/>
+      <c r="AU28" s="123"/>
+      <c r="AV28" s="123"/>
+      <c r="AW28" s="123"/>
+      <c r="AX28" s="123"/>
+      <c r="AY28" s="123"/>
+      <c r="AZ28" s="123"/>
+      <c r="BA28" s="123"/>
+      <c r="BB28" s="123"/>
+      <c r="BC28" s="123"/>
+      <c r="BD28" s="123"/>
+      <c r="BE28" s="123"/>
+      <c r="BF28" s="123"/>
+      <c r="BG28" s="123"/>
+      <c r="BH28" s="123"/>
+      <c r="BI28" s="123"/>
+      <c r="BJ28" s="123"/>
+      <c r="BK28" s="123"/>
+      <c r="BL28" s="123"/>
+      <c r="BM28" s="123"/>
+      <c r="BN28" s="123"/>
+      <c r="BO28" s="123"/>
+      <c r="BP28" s="123"/>
+      <c r="BQ28" s="123"/>
+      <c r="BR28" s="123"/>
+      <c r="BS28" s="123"/>
+      <c r="BT28" s="123"/>
+      <c r="BU28" s="123"/>
+      <c r="BV28" s="123"/>
+      <c r="BW28" s="123"/>
+      <c r="BX28" s="123"/>
+      <c r="BY28" s="123"/>
+      <c r="BZ28" s="123"/>
+      <c r="CA28" s="123"/>
+      <c r="CB28" s="123"/>
+      <c r="CC28" s="123"/>
+      <c r="CD28" s="123"/>
+      <c r="CE28" s="123"/>
+      <c r="CF28" s="123"/>
+      <c r="CG28" s="123"/>
+      <c r="CH28" s="123"/>
+      <c r="CI28" s="123"/>
+      <c r="CJ28" s="123"/>
+      <c r="CK28" s="123"/>
+      <c r="CL28" s="123"/>
+      <c r="CM28" s="123"/>
+      <c r="CN28" s="123"/>
+      <c r="CO28" s="123"/>
+      <c r="CP28" s="123"/>
+      <c r="CQ28" s="123"/>
+      <c r="CR28" s="123"/>
+      <c r="CS28" s="123"/>
+      <c r="CT28" s="123"/>
+      <c r="CU28" s="123"/>
+      <c r="CV28" s="123"/>
+      <c r="CW28" s="123"/>
+      <c r="CX28" s="123"/>
+      <c r="CY28" s="123"/>
+      <c r="CZ28" s="123"/>
+      <c r="DA28" s="123"/>
+      <c r="DB28" s="123"/>
+      <c r="DC28" s="123"/>
+      <c r="DD28" s="123"/>
+      <c r="DE28" s="123"/>
+      <c r="DF28" s="123"/>
+      <c r="DG28" s="123"/>
+      <c r="DH28" s="123"/>
+      <c r="DI28" s="123"/>
+      <c r="DJ28" s="123"/>
+      <c r="DK28" s="123"/>
+      <c r="DL28" s="123"/>
+      <c r="DM28" s="123"/>
+      <c r="DN28" s="123"/>
+      <c r="DO28" s="123"/>
+      <c r="DP28" s="123"/>
+      <c r="DQ28" s="123"/>
+      <c r="DR28" s="123"/>
+      <c r="DS28" s="123"/>
+      <c r="DT28" s="123"/>
+      <c r="DU28" s="123"/>
+      <c r="DV28" s="123"/>
+      <c r="DW28" s="123"/>
+      <c r="DX28" s="123"/>
+      <c r="DY28" s="123"/>
+      <c r="DZ28" s="123"/>
+      <c r="EA28" s="123"/>
+      <c r="EB28" s="123"/>
+      <c r="EC28" s="123"/>
+      <c r="ED28" s="123"/>
+      <c r="EE28" s="123"/>
+      <c r="EF28" s="123"/>
+      <c r="EG28" s="123"/>
+      <c r="EH28" s="123"/>
+      <c r="EI28" s="123"/>
+      <c r="EJ28" s="123"/>
+      <c r="EK28" s="123"/>
+      <c r="EL28" s="123"/>
+      <c r="EM28" s="123"/>
+      <c r="EN28" s="123"/>
+      <c r="EO28" s="123"/>
+      <c r="EP28" s="123"/>
+      <c r="EQ28" s="123"/>
+      <c r="ER28" s="123"/>
+      <c r="ES28" s="123"/>
+      <c r="ET28" s="123"/>
+      <c r="EU28" s="123"/>
+      <c r="EV28" s="123"/>
+      <c r="EW28" s="123"/>
+      <c r="EX28" s="123"/>
+      <c r="EY28" s="123"/>
+      <c r="EZ28" s="123"/>
+      <c r="FA28" s="123"/>
+      <c r="FB28" s="123"/>
+      <c r="FC28" s="123"/>
+      <c r="FD28" s="123"/>
+      <c r="FE28" s="123"/>
+      <c r="FF28" s="123"/>
+      <c r="FG28" s="123"/>
+      <c r="FH28" s="123"/>
+      <c r="FI28" s="123"/>
+      <c r="FJ28" s="123"/>
+      <c r="FK28" s="123"/>
+      <c r="FL28" s="123"/>
+      <c r="FM28" s="123"/>
+      <c r="FN28" s="123"/>
+      <c r="FO28" s="123"/>
+      <c r="FP28" s="123"/>
+      <c r="FQ28" s="123"/>
+      <c r="FR28" s="123"/>
+      <c r="FS28" s="123"/>
+      <c r="FT28" s="123"/>
+      <c r="FU28" s="123"/>
+      <c r="FV28" s="123"/>
+      <c r="FW28" s="123"/>
+      <c r="FX28" s="123"/>
+      <c r="FY28" s="123"/>
+      <c r="FZ28" s="123"/>
+      <c r="GA28" s="123"/>
+      <c r="GB28" s="123"/>
+      <c r="GC28" s="123"/>
+      <c r="GD28" s="123"/>
+      <c r="GE28" s="123"/>
+      <c r="GF28" s="123"/>
+      <c r="GG28" s="123"/>
+      <c r="GH28" s="123"/>
+      <c r="GI28" s="123"/>
+      <c r="GJ28" s="123"/>
+      <c r="GK28" s="123"/>
+      <c r="GL28" s="123"/>
+      <c r="GM28" s="123"/>
+      <c r="GN28" s="123"/>
+      <c r="GO28" s="123"/>
+      <c r="GP28" s="123"/>
+      <c r="GQ28" s="123"/>
+      <c r="GR28" s="123"/>
+      <c r="GS28" s="123"/>
+      <c r="GT28" s="123"/>
+      <c r="GU28" s="123"/>
+      <c r="GV28" s="123"/>
+      <c r="GW28" s="123"/>
+      <c r="GX28" s="123"/>
+      <c r="GY28" s="123"/>
+      <c r="GZ28" s="123"/>
+      <c r="HA28" s="123"/>
+      <c r="HB28" s="123"/>
+      <c r="HC28" s="123"/>
+      <c r="HD28" s="123"/>
+      <c r="HE28" s="123"/>
+      <c r="HF28" s="123"/>
+      <c r="HG28" s="123"/>
+      <c r="HH28" s="123"/>
+      <c r="HI28" s="123"/>
+      <c r="HJ28" s="123"/>
+      <c r="HK28" s="123"/>
+      <c r="HL28" s="123"/>
+      <c r="HM28" s="123"/>
+      <c r="HN28" s="123"/>
+      <c r="HO28" s="123"/>
+      <c r="HP28" s="123"/>
+      <c r="HQ28" s="123"/>
+      <c r="HR28" s="123"/>
+      <c r="HS28" s="123"/>
+      <c r="HT28" s="123"/>
+      <c r="HU28" s="123"/>
+      <c r="HV28" s="123"/>
+      <c r="HW28" s="123"/>
+      <c r="HX28" s="123"/>
+      <c r="HY28" s="123"/>
+      <c r="HZ28" s="123"/>
+      <c r="IA28" s="123"/>
+      <c r="IB28" s="123"/>
+      <c r="IC28" s="123"/>
+      <c r="ID28" s="123"/>
+      <c r="IE28" s="123"/>
+      <c r="IF28" s="123"/>
+      <c r="IG28" s="123"/>
+      <c r="IH28" s="123"/>
+      <c r="II28" s="123"/>
+      <c r="IJ28" s="123"/>
+      <c r="IK28" s="123"/>
+      <c r="IL28" s="123"/>
+      <c r="IM28" s="123"/>
+      <c r="IN28" s="123"/>
+      <c r="IO28" s="123"/>
+      <c r="IP28" s="123"/>
+      <c r="IQ28" s="123"/>
+      <c r="IR28" s="123"/>
+      <c r="IS28" s="123"/>
+      <c r="IT28" s="123"/>
+      <c r="IU28" s="123"/>
+      <c r="IV28" s="123"/>
+      <c r="IW28" s="123"/>
+      <c r="IX28" s="123"/>
+      <c r="IY28" s="123"/>
+      <c r="IZ28" s="123"/>
+      <c r="JA28" s="123"/>
+      <c r="JB28" s="123"/>
+      <c r="JC28" s="123"/>
+      <c r="JD28" s="123"/>
+      <c r="JE28" s="123"/>
+      <c r="JF28" s="123"/>
+      <c r="JG28" s="123"/>
+      <c r="JH28" s="123"/>
+      <c r="JI28" s="123"/>
+      <c r="JJ28" s="123"/>
+      <c r="JK28" s="123"/>
+      <c r="JL28" s="123"/>
+      <c r="JM28" s="123"/>
+      <c r="JN28" s="123"/>
+      <c r="JO28" s="123"/>
+      <c r="JP28" s="123"/>
+      <c r="JQ28" s="123"/>
+      <c r="JR28" s="123"/>
+      <c r="JS28" s="123"/>
+      <c r="JT28" s="123"/>
+      <c r="JU28" s="123"/>
+      <c r="JV28" s="123"/>
+      <c r="JW28" s="123"/>
+      <c r="JX28" s="123"/>
+      <c r="JY28" s="123"/>
+      <c r="JZ28" s="123"/>
+      <c r="KA28" s="123"/>
+      <c r="KB28" s="123"/>
+      <c r="KC28" s="123"/>
+      <c r="KD28" s="123"/>
+      <c r="KE28" s="123"/>
+      <c r="KF28" s="123"/>
+      <c r="KG28" s="123"/>
+      <c r="KH28" s="123"/>
+      <c r="KI28" s="123"/>
+      <c r="KJ28" s="123"/>
+      <c r="KK28" s="123"/>
+      <c r="KL28" s="123"/>
+      <c r="KM28" s="123"/>
+      <c r="KN28" s="123"/>
+      <c r="KO28" s="123"/>
+      <c r="KP28" s="123"/>
+      <c r="KQ28" s="123"/>
+      <c r="KR28" s="123"/>
+      <c r="KS28" s="123"/>
+      <c r="KT28" s="123"/>
+      <c r="KU28" s="123"/>
+      <c r="KV28" s="123"/>
+      <c r="KW28" s="123"/>
+      <c r="KX28" s="123"/>
+      <c r="KY28" s="123"/>
+      <c r="KZ28" s="123"/>
+      <c r="LA28" s="123"/>
+      <c r="LB28" s="123"/>
+      <c r="LC28" s="123"/>
+      <c r="LD28" s="123"/>
+      <c r="LE28" s="123"/>
+      <c r="LF28" s="123"/>
+      <c r="LG28" s="123"/>
+      <c r="LH28" s="123"/>
+      <c r="LI28" s="123"/>
+      <c r="LJ28" s="123"/>
+      <c r="LK28" s="123"/>
+      <c r="LL28" s="123"/>
+      <c r="LM28" s="123"/>
+      <c r="LN28" s="123"/>
+      <c r="LO28" s="123"/>
+      <c r="LP28" s="123"/>
+      <c r="LQ28" s="123"/>
+      <c r="LR28" s="123"/>
+      <c r="LS28" s="123"/>
+      <c r="LT28" s="123"/>
+      <c r="LU28" s="123"/>
+      <c r="LV28" s="123"/>
+      <c r="LW28" s="123"/>
+      <c r="LX28" s="123"/>
+      <c r="LY28" s="123"/>
+      <c r="LZ28" s="123"/>
+      <c r="MA28" s="123"/>
+      <c r="MB28" s="123"/>
+      <c r="MC28" s="123"/>
+      <c r="MD28" s="123"/>
+      <c r="ME28" s="123"/>
+      <c r="MF28" s="123"/>
+      <c r="MG28" s="123"/>
+      <c r="MH28" s="123"/>
+      <c r="MI28" s="123"/>
+      <c r="MJ28" s="123"/>
+      <c r="MK28" s="123"/>
+      <c r="ML28" s="123"/>
+      <c r="MM28" s="123"/>
+      <c r="MN28" s="123"/>
+      <c r="MO28" s="123"/>
+      <c r="MP28" s="123"/>
+      <c r="MQ28" s="123"/>
+      <c r="MR28" s="123"/>
+      <c r="MS28" s="123"/>
+      <c r="MT28" s="123"/>
+      <c r="MU28" s="123"/>
+      <c r="MV28" s="123"/>
+      <c r="MW28" s="123"/>
+      <c r="MX28" s="123"/>
+      <c r="MY28" s="123"/>
+      <c r="MZ28" s="123"/>
+      <c r="NA28" s="123"/>
+      <c r="NB28" s="123"/>
+      <c r="NC28" s="123"/>
+      <c r="ND28" s="123"/>
+      <c r="NE28" s="123"/>
+      <c r="NF28" s="123"/>
+      <c r="NG28" s="123"/>
+      <c r="NH28" s="123"/>
+      <c r="NI28" s="123"/>
+      <c r="NJ28" s="123"/>
+      <c r="NK28" s="123"/>
+      <c r="NL28" s="123"/>
+      <c r="NM28" s="123"/>
+      <c r="NN28" s="123"/>
+      <c r="NO28" s="123"/>
+      <c r="NP28" s="123"/>
+      <c r="NQ28" s="123"/>
+      <c r="NR28" s="123"/>
+      <c r="NS28" s="123"/>
+      <c r="NT28" s="123"/>
+      <c r="NU28" s="123"/>
+      <c r="NV28" s="123"/>
+      <c r="NW28" s="123"/>
+      <c r="NX28" s="123"/>
+      <c r="NY28" s="123"/>
+      <c r="NZ28" s="123"/>
+      <c r="OA28" s="123"/>
+      <c r="OB28" s="123"/>
+      <c r="OC28" s="123"/>
+      <c r="OD28" s="123"/>
+      <c r="OE28" s="123"/>
+      <c r="OF28" s="123"/>
+      <c r="OG28" s="123"/>
+      <c r="OH28" s="123"/>
+      <c r="OI28" s="123"/>
+      <c r="OJ28" s="123"/>
+      <c r="OK28" s="123"/>
+      <c r="OL28" s="123"/>
+      <c r="OM28" s="123"/>
+      <c r="ON28" s="123"/>
+      <c r="OO28" s="123"/>
+      <c r="OP28" s="123"/>
+      <c r="OQ28" s="123"/>
+      <c r="OR28" s="123"/>
+      <c r="OS28" s="123"/>
+      <c r="OT28" s="123"/>
+      <c r="OU28" s="123"/>
+      <c r="OV28" s="123"/>
+      <c r="OW28" s="123"/>
+      <c r="OX28" s="123"/>
+      <c r="OY28" s="123"/>
+      <c r="OZ28" s="123"/>
+      <c r="PA28" s="123"/>
+      <c r="PB28" s="123"/>
+      <c r="PC28" s="123"/>
+      <c r="PD28" s="123"/>
+      <c r="PE28" s="123"/>
+      <c r="PF28" s="123"/>
+      <c r="PG28" s="123"/>
+      <c r="PH28" s="123"/>
+      <c r="PI28" s="123"/>
+      <c r="PJ28" s="123"/>
+      <c r="PK28" s="123"/>
+      <c r="PL28" s="123"/>
+      <c r="PM28" s="123"/>
+      <c r="PN28" s="123"/>
+      <c r="PO28" s="123"/>
+      <c r="PP28" s="123"/>
+      <c r="PQ28" s="123"/>
+      <c r="PR28" s="123"/>
+      <c r="PS28" s="123"/>
+      <c r="PT28" s="123"/>
+      <c r="PU28" s="123"/>
+      <c r="PV28" s="123"/>
+      <c r="PW28" s="123"/>
+      <c r="PX28" s="123"/>
+      <c r="PY28" s="123"/>
+      <c r="PZ28" s="123"/>
+      <c r="QA28" s="123"/>
+      <c r="QB28" s="123"/>
+      <c r="QC28" s="123"/>
+      <c r="QD28" s="123"/>
+      <c r="QE28" s="123"/>
+      <c r="QF28" s="123"/>
+      <c r="QG28" s="123"/>
+      <c r="QH28" s="123"/>
+      <c r="QI28" s="123"/>
+      <c r="QJ28" s="123"/>
+      <c r="QK28" s="123"/>
+      <c r="QL28" s="123"/>
+      <c r="QM28" s="123"/>
+      <c r="QN28" s="123"/>
+      <c r="QO28" s="123"/>
+      <c r="QP28" s="123"/>
+      <c r="QQ28" s="123"/>
+      <c r="QR28" s="123"/>
+      <c r="QS28" s="123"/>
+      <c r="QT28" s="123"/>
+      <c r="QU28" s="123"/>
+      <c r="QV28" s="123"/>
+      <c r="QW28" s="123"/>
+      <c r="QX28" s="123"/>
+      <c r="QY28" s="123"/>
+      <c r="QZ28" s="123"/>
+      <c r="RA28" s="123"/>
+      <c r="RB28" s="123"/>
+      <c r="RC28" s="123"/>
+      <c r="RD28" s="123"/>
+      <c r="RE28" s="123"/>
+      <c r="RF28" s="123"/>
+      <c r="RG28" s="123"/>
+      <c r="RH28" s="123"/>
+      <c r="RI28" s="123"/>
+      <c r="RJ28" s="123"/>
+      <c r="RK28" s="123"/>
+      <c r="RL28" s="123"/>
+      <c r="RM28" s="123"/>
+      <c r="RN28" s="123"/>
+      <c r="RO28" s="123"/>
+      <c r="RP28" s="123"/>
+      <c r="RQ28" s="123"/>
+      <c r="RR28" s="123"/>
+      <c r="RS28" s="123"/>
+      <c r="RT28" s="123"/>
+      <c r="RU28" s="123"/>
+      <c r="RV28" s="123"/>
+      <c r="RW28" s="123"/>
+      <c r="RX28" s="123"/>
+      <c r="RY28" s="123"/>
+      <c r="RZ28" s="123"/>
+      <c r="SA28" s="123"/>
+      <c r="SB28" s="123"/>
+      <c r="SC28" s="123"/>
+      <c r="SD28" s="123"/>
+      <c r="SE28" s="123"/>
+      <c r="SF28" s="123"/>
+      <c r="SG28" s="123"/>
+      <c r="SH28" s="123"/>
+      <c r="SI28" s="123"/>
+      <c r="SJ28" s="123"/>
+      <c r="SK28" s="123"/>
+      <c r="SL28" s="123"/>
+      <c r="SM28" s="123"/>
+      <c r="SN28" s="123"/>
+      <c r="SO28" s="123"/>
+      <c r="SP28" s="123"/>
+      <c r="SQ28" s="123"/>
+      <c r="SR28" s="123"/>
+      <c r="SS28" s="123"/>
+      <c r="ST28" s="123"/>
+      <c r="SU28" s="123"/>
+      <c r="SV28" s="123"/>
+      <c r="SW28" s="123"/>
+      <c r="SX28" s="123"/>
+      <c r="SY28" s="123"/>
+      <c r="SZ28" s="123"/>
+      <c r="TA28" s="123"/>
+      <c r="TB28" s="123"/>
+      <c r="TC28" s="123"/>
+      <c r="TD28" s="123"/>
+      <c r="TE28" s="123"/>
+      <c r="TF28" s="123"/>
+      <c r="TG28" s="123"/>
+      <c r="TH28" s="123"/>
+      <c r="TI28" s="123"/>
+      <c r="TJ28" s="123"/>
+      <c r="TK28" s="123"/>
+      <c r="TL28" s="123"/>
+      <c r="TM28" s="123"/>
+      <c r="TN28" s="123"/>
+      <c r="TO28" s="123"/>
+      <c r="TP28" s="123"/>
+      <c r="TQ28" s="123"/>
+      <c r="TR28" s="123"/>
+      <c r="TS28" s="123"/>
+      <c r="TT28" s="123"/>
+      <c r="TU28" s="123"/>
+      <c r="TV28" s="123"/>
+      <c r="TW28" s="123"/>
+      <c r="TX28" s="123"/>
+      <c r="TY28" s="123"/>
+      <c r="TZ28" s="123"/>
+      <c r="UA28" s="123"/>
+      <c r="UB28" s="123"/>
+      <c r="UC28" s="123"/>
+      <c r="UD28" s="123"/>
+      <c r="UE28" s="123"/>
+      <c r="UF28" s="123"/>
+      <c r="UG28" s="123"/>
+      <c r="UH28" s="123"/>
+      <c r="UI28" s="123"/>
+      <c r="UJ28" s="123"/>
+      <c r="UK28" s="123"/>
+      <c r="UL28" s="123"/>
+      <c r="UM28" s="123"/>
+      <c r="UN28" s="123"/>
+      <c r="UO28" s="123"/>
+      <c r="UP28" s="123"/>
+      <c r="UQ28" s="123"/>
+      <c r="UR28" s="123"/>
+      <c r="US28" s="123"/>
+      <c r="UT28" s="123"/>
+      <c r="UU28" s="123"/>
+      <c r="UV28" s="123"/>
+      <c r="UW28" s="123"/>
+      <c r="UX28" s="123"/>
+      <c r="UY28" s="123"/>
+      <c r="UZ28" s="123"/>
+      <c r="VA28" s="123"/>
+      <c r="VB28" s="123"/>
+      <c r="VC28" s="123"/>
+      <c r="VD28" s="123"/>
+      <c r="VE28" s="123"/>
+      <c r="VF28" s="123"/>
+      <c r="VG28" s="123"/>
+      <c r="VH28" s="123"/>
+      <c r="VI28" s="123"/>
+      <c r="VJ28" s="123"/>
+      <c r="VK28" s="123"/>
+      <c r="VL28" s="123"/>
+      <c r="VM28" s="123"/>
+      <c r="VN28" s="123"/>
+      <c r="VO28" s="123"/>
+      <c r="VP28" s="123"/>
+      <c r="VQ28" s="123"/>
+      <c r="VR28" s="123"/>
+      <c r="VS28" s="123"/>
+      <c r="VT28" s="123"/>
+      <c r="VU28" s="123"/>
+      <c r="VV28" s="123"/>
+      <c r="VW28" s="123"/>
+      <c r="VX28" s="123"/>
+      <c r="VY28" s="123"/>
+      <c r="VZ28" s="123"/>
+      <c r="WA28" s="123"/>
+      <c r="WB28" s="123"/>
+      <c r="WC28" s="123"/>
+      <c r="WD28" s="123"/>
+      <c r="WE28" s="123"/>
+      <c r="WF28" s="123"/>
+      <c r="WG28" s="123"/>
+      <c r="WH28" s="123"/>
+      <c r="WI28" s="123"/>
+      <c r="WJ28" s="123"/>
+      <c r="WK28" s="123"/>
+      <c r="WL28" s="123"/>
+      <c r="WM28" s="123"/>
+      <c r="WN28" s="123"/>
+      <c r="WO28" s="123"/>
+      <c r="WP28" s="123"/>
+      <c r="WQ28" s="123"/>
+      <c r="WR28" s="123"/>
+      <c r="WS28" s="123"/>
+      <c r="WT28" s="123"/>
+      <c r="WU28" s="123"/>
+      <c r="WV28" s="123"/>
+      <c r="WW28" s="123"/>
+      <c r="WX28" s="123"/>
+      <c r="WY28" s="123"/>
+      <c r="WZ28" s="123"/>
+      <c r="XA28" s="123"/>
+      <c r="XB28" s="123"/>
+      <c r="XC28" s="123"/>
+      <c r="XD28" s="123"/>
+      <c r="XE28" s="123"/>
+      <c r="XF28" s="123"/>
+      <c r="XG28" s="123"/>
+      <c r="XH28" s="123"/>
+      <c r="XI28" s="123"/>
+      <c r="XJ28" s="123"/>
+      <c r="XK28" s="123"/>
+      <c r="XL28" s="123"/>
+      <c r="XM28" s="123"/>
+      <c r="XN28" s="123"/>
+      <c r="XO28" s="123"/>
+      <c r="XP28" s="123"/>
+      <c r="XQ28" s="123"/>
+      <c r="XR28" s="123"/>
+      <c r="XS28" s="123"/>
+      <c r="XT28" s="123"/>
+      <c r="XU28" s="123"/>
+      <c r="XV28" s="123"/>
+      <c r="XW28" s="123"/>
+      <c r="XX28" s="123"/>
+      <c r="XY28" s="123"/>
+      <c r="XZ28" s="123"/>
+      <c r="YA28" s="123"/>
+      <c r="YB28" s="123"/>
+      <c r="YC28" s="123"/>
+      <c r="YD28" s="123"/>
+      <c r="YE28" s="123"/>
+      <c r="YF28" s="123"/>
+      <c r="YG28" s="123"/>
+      <c r="YH28" s="123"/>
+      <c r="YI28" s="123"/>
+      <c r="YJ28" s="123"/>
+      <c r="YK28" s="123"/>
+      <c r="YL28" s="123"/>
+      <c r="YM28" s="123"/>
+      <c r="YN28" s="123"/>
+      <c r="YO28" s="123"/>
+      <c r="YP28" s="123"/>
+      <c r="YQ28" s="123"/>
+      <c r="YR28" s="123"/>
+      <c r="YS28" s="123"/>
+      <c r="YT28" s="123"/>
+      <c r="YU28" s="123"/>
+      <c r="YV28" s="123"/>
+      <c r="YW28" s="123"/>
+      <c r="YX28" s="123"/>
+      <c r="YY28" s="123"/>
+      <c r="YZ28" s="123"/>
+      <c r="ZA28" s="123"/>
+      <c r="ZB28" s="123"/>
+      <c r="ZC28" s="123"/>
+      <c r="ZD28" s="123"/>
+      <c r="ZE28" s="123"/>
+      <c r="ZF28" s="123"/>
+      <c r="ZG28" s="123"/>
+      <c r="ZH28" s="123"/>
+      <c r="ZI28" s="123"/>
+      <c r="ZJ28" s="123"/>
+      <c r="ZK28" s="123"/>
+      <c r="ZL28" s="123"/>
+      <c r="ZM28" s="123"/>
+      <c r="ZN28" s="123"/>
+      <c r="ZO28" s="123"/>
+      <c r="ZP28" s="123"/>
+      <c r="ZQ28" s="123"/>
+      <c r="ZR28" s="123"/>
+      <c r="ZS28" s="123"/>
+      <c r="ZT28" s="123"/>
+      <c r="ZU28" s="123"/>
+      <c r="ZV28" s="123"/>
+      <c r="ZW28" s="123"/>
+      <c r="ZX28" s="123"/>
+      <c r="ZY28" s="123"/>
+      <c r="ZZ28" s="123"/>
+      <c r="AAA28" s="123"/>
+      <c r="AAB28" s="123"/>
+      <c r="AAC28" s="123"/>
+      <c r="AAD28" s="123"/>
+      <c r="AAE28" s="123"/>
+      <c r="AAF28" s="123"/>
+      <c r="AAG28" s="123"/>
+      <c r="AAH28" s="123"/>
+      <c r="AAI28" s="123"/>
+      <c r="AAJ28" s="123"/>
+      <c r="AAK28" s="123"/>
+      <c r="AAL28" s="123"/>
+      <c r="AAM28" s="123"/>
+      <c r="AAN28" s="123"/>
+      <c r="AAO28" s="123"/>
+      <c r="AAP28" s="123"/>
+      <c r="AAQ28" s="123"/>
+      <c r="AAR28" s="123"/>
+      <c r="AAS28" s="123"/>
+      <c r="AAT28" s="123"/>
+      <c r="AAU28" s="123"/>
+      <c r="AAV28" s="123"/>
+      <c r="AAW28" s="123"/>
+      <c r="AAX28" s="123"/>
+      <c r="AAY28" s="123"/>
+      <c r="AAZ28" s="123"/>
+      <c r="ABA28" s="123"/>
+      <c r="ABB28" s="123"/>
+      <c r="ABC28" s="123"/>
+      <c r="ABD28" s="123"/>
+      <c r="ABE28" s="123"/>
+      <c r="ABF28" s="123"/>
+      <c r="ABG28" s="123"/>
+      <c r="ABH28" s="123"/>
+      <c r="ABI28" s="123"/>
+      <c r="ABJ28" s="123"/>
+      <c r="ABK28" s="123"/>
+      <c r="ABL28" s="123"/>
+      <c r="ABM28" s="123"/>
+      <c r="ABN28" s="123"/>
+      <c r="ABO28" s="123"/>
+      <c r="ABP28" s="123"/>
+      <c r="ABQ28" s="123"/>
+      <c r="ABR28" s="123"/>
+      <c r="ABS28" s="123"/>
+      <c r="ABT28" s="123"/>
+      <c r="ABU28" s="123"/>
+      <c r="ABV28" s="123"/>
+      <c r="ABW28" s="123"/>
+      <c r="ABX28" s="123"/>
+      <c r="ABY28" s="123"/>
+      <c r="ABZ28" s="123"/>
+      <c r="ACA28" s="123"/>
+      <c r="ACB28" s="123"/>
+      <c r="ACC28" s="123"/>
+      <c r="ACD28" s="123"/>
+      <c r="ACE28" s="123"/>
+      <c r="ACF28" s="123"/>
+      <c r="ACG28" s="123"/>
+      <c r="ACH28" s="123"/>
+      <c r="ACI28" s="123"/>
+      <c r="ACJ28" s="123"/>
+      <c r="ACK28" s="123"/>
+      <c r="ACL28" s="123"/>
+      <c r="ACM28" s="123"/>
+      <c r="ACN28" s="123"/>
+      <c r="ACO28" s="123"/>
+      <c r="ACP28" s="123"/>
+      <c r="ACQ28" s="123"/>
+      <c r="ACR28" s="123"/>
+      <c r="ACS28" s="123"/>
+      <c r="ACT28" s="123"/>
+      <c r="ACU28" s="123"/>
+      <c r="ACV28" s="123"/>
+      <c r="ACW28" s="123"/>
+      <c r="ACX28" s="123"/>
+      <c r="ACY28" s="123"/>
+      <c r="ACZ28" s="123"/>
+      <c r="ADA28" s="123"/>
+      <c r="ADB28" s="123"/>
+      <c r="ADC28" s="123"/>
+      <c r="ADD28" s="123"/>
+      <c r="ADE28" s="123"/>
+      <c r="ADF28" s="123"/>
+      <c r="ADG28" s="123"/>
+      <c r="ADH28" s="123"/>
+      <c r="ADI28" s="123"/>
+      <c r="ADJ28" s="123"/>
+      <c r="ADK28" s="123"/>
+      <c r="ADL28" s="123"/>
+      <c r="ADM28" s="123"/>
+      <c r="ADN28" s="123"/>
+      <c r="ADO28" s="123"/>
+      <c r="ADP28" s="123"/>
+      <c r="ADQ28" s="123"/>
+      <c r="ADR28" s="123"/>
+      <c r="ADS28" s="123"/>
+      <c r="ADT28" s="123"/>
+      <c r="ADU28" s="123"/>
+      <c r="ADV28" s="123"/>
+      <c r="ADW28" s="123"/>
+      <c r="ADX28" s="123"/>
+      <c r="ADY28" s="123"/>
+      <c r="ADZ28" s="123"/>
+      <c r="AEA28" s="123"/>
+      <c r="AEB28" s="123"/>
+      <c r="AEC28" s="123"/>
+      <c r="AED28" s="123"/>
+      <c r="AEE28" s="123"/>
+      <c r="AEF28" s="123"/>
+      <c r="AEG28" s="123"/>
+      <c r="AEH28" s="123"/>
+      <c r="AEI28" s="123"/>
+      <c r="AEJ28" s="123"/>
+      <c r="AEK28" s="123"/>
+      <c r="AEL28" s="123"/>
+      <c r="AEM28" s="123"/>
+      <c r="AEN28" s="123"/>
+      <c r="AEO28" s="123"/>
+      <c r="AEP28" s="123"/>
+      <c r="AEQ28" s="123"/>
+      <c r="AER28" s="123"/>
+      <c r="AES28" s="123"/>
+      <c r="AET28" s="123"/>
+      <c r="AEU28" s="123"/>
+      <c r="AEV28" s="123"/>
+      <c r="AEW28" s="123"/>
+      <c r="AEX28" s="123"/>
+      <c r="AEY28" s="123"/>
+      <c r="AEZ28" s="123"/>
+      <c r="AFA28" s="123"/>
+      <c r="AFB28" s="123"/>
+      <c r="AFC28" s="123"/>
+      <c r="AFD28" s="123"/>
+      <c r="AFE28" s="123"/>
+      <c r="AFF28" s="123"/>
+      <c r="AFG28" s="123"/>
+      <c r="AFH28" s="123"/>
+      <c r="AFI28" s="123"/>
+      <c r="AFJ28" s="123"/>
+      <c r="AFK28" s="123"/>
+      <c r="AFL28" s="123"/>
+      <c r="AFM28" s="123"/>
+      <c r="AFN28" s="123"/>
+      <c r="AFO28" s="123"/>
+      <c r="AFP28" s="123"/>
+      <c r="AFQ28" s="123"/>
+      <c r="AFR28" s="123"/>
+      <c r="AFS28" s="123"/>
+      <c r="AFT28" s="123"/>
+      <c r="AFU28" s="123"/>
+      <c r="AFV28" s="123"/>
+      <c r="AFW28" s="123"/>
+      <c r="AFX28" s="123"/>
+      <c r="AFY28" s="123"/>
+      <c r="AFZ28" s="123"/>
+      <c r="AGA28" s="123"/>
+      <c r="AGB28" s="123"/>
+      <c r="AGC28" s="123"/>
+      <c r="AGD28" s="123"/>
+      <c r="AGE28" s="123"/>
+      <c r="AGF28" s="123"/>
+      <c r="AGG28" s="123"/>
+      <c r="AGH28" s="123"/>
+      <c r="AGI28" s="123"/>
+      <c r="AGJ28" s="123"/>
+      <c r="AGK28" s="123"/>
+      <c r="AGL28" s="123"/>
+      <c r="AGM28" s="123"/>
+      <c r="AGN28" s="123"/>
+      <c r="AGO28" s="123"/>
+      <c r="AGP28" s="123"/>
+      <c r="AGQ28" s="123"/>
+      <c r="AGR28" s="123"/>
+      <c r="AGS28" s="123"/>
+      <c r="AGT28" s="123"/>
+      <c r="AGU28" s="123"/>
+      <c r="AGV28" s="123"/>
+      <c r="AGW28" s="123"/>
+      <c r="AGX28" s="123"/>
+      <c r="AGY28" s="123"/>
+      <c r="AGZ28" s="123"/>
+      <c r="AHA28" s="123"/>
+      <c r="AHB28" s="123"/>
+      <c r="AHC28" s="123"/>
+      <c r="AHD28" s="123"/>
+      <c r="AHE28" s="123"/>
+      <c r="AHF28" s="123"/>
+      <c r="AHG28" s="123"/>
+      <c r="AHH28" s="123"/>
+      <c r="AHI28" s="123"/>
+      <c r="AHJ28" s="123"/>
+      <c r="AHK28" s="123"/>
+      <c r="AHL28" s="123"/>
+      <c r="AHM28" s="123"/>
+      <c r="AHN28" s="123"/>
+      <c r="AHO28" s="123"/>
+      <c r="AHP28" s="123"/>
+      <c r="AHQ28" s="123"/>
+      <c r="AHR28" s="123"/>
+      <c r="AHS28" s="123"/>
+      <c r="AHT28" s="123"/>
+      <c r="AHU28" s="123"/>
+      <c r="AHV28" s="123"/>
+      <c r="AHW28" s="123"/>
+      <c r="AHX28" s="123"/>
+      <c r="AHY28" s="123"/>
+      <c r="AHZ28" s="123"/>
+      <c r="AIA28" s="123"/>
+      <c r="AIB28" s="123"/>
+      <c r="AIC28" s="123"/>
+      <c r="AID28" s="123"/>
+      <c r="AIE28" s="123"/>
+      <c r="AIF28" s="123"/>
+      <c r="AIG28" s="123"/>
+      <c r="AIH28" s="123"/>
+      <c r="AII28" s="123"/>
+      <c r="AIJ28" s="123"/>
+      <c r="AIK28" s="123"/>
+      <c r="AIL28" s="123"/>
+      <c r="AIM28" s="123"/>
+      <c r="AIN28" s="123"/>
+      <c r="AIO28" s="123"/>
+      <c r="AIP28" s="123"/>
+      <c r="AIQ28" s="123"/>
+      <c r="AIR28" s="123"/>
+      <c r="AIS28" s="123"/>
+      <c r="AIT28" s="123"/>
+      <c r="AIU28" s="123"/>
+      <c r="AIV28" s="123"/>
+      <c r="AIW28" s="123"/>
+      <c r="AIX28" s="123"/>
+      <c r="AIY28" s="123"/>
+      <c r="AIZ28" s="123"/>
+      <c r="AJA28" s="123"/>
+      <c r="AJB28" s="123"/>
+      <c r="AJC28" s="123"/>
+      <c r="AJD28" s="123"/>
+      <c r="AJE28" s="123"/>
+      <c r="AJF28" s="123"/>
+      <c r="AJG28" s="123"/>
+      <c r="AJH28" s="123"/>
+      <c r="AJI28" s="123"/>
+      <c r="AJJ28" s="123"/>
+      <c r="AJK28" s="123"/>
+      <c r="AJL28" s="123"/>
+      <c r="AJM28" s="123"/>
+      <c r="AJN28" s="123"/>
+      <c r="AJO28" s="123"/>
+      <c r="AJP28" s="123"/>
+      <c r="AJQ28" s="123"/>
+      <c r="AJR28" s="123"/>
+      <c r="AJS28" s="123"/>
+      <c r="AJT28" s="123"/>
+      <c r="AJU28" s="123"/>
+      <c r="AJV28" s="123"/>
+      <c r="AJW28" s="123"/>
+      <c r="AJX28" s="123"/>
+      <c r="AJY28" s="123"/>
+      <c r="AJZ28" s="123"/>
+      <c r="AKA28" s="123"/>
+      <c r="AKB28" s="123"/>
+      <c r="AKC28" s="123"/>
+      <c r="AKD28" s="123"/>
+      <c r="AKE28" s="123"/>
+      <c r="AKF28" s="123"/>
+      <c r="AKG28" s="123"/>
+      <c r="AKH28" s="123"/>
+      <c r="AKI28" s="123"/>
+      <c r="AKJ28" s="123"/>
+      <c r="AKK28" s="123"/>
+      <c r="AKL28" s="123"/>
+      <c r="AKM28" s="123"/>
+      <c r="AKN28" s="123"/>
+      <c r="AKO28" s="123"/>
+      <c r="AKP28" s="123"/>
+      <c r="AKQ28" s="123"/>
+      <c r="AKR28" s="123"/>
+      <c r="AKS28" s="123"/>
+      <c r="AKT28" s="123"/>
+      <c r="AKU28" s="123"/>
+      <c r="AKV28" s="123"/>
+      <c r="AKW28" s="123"/>
+      <c r="AKX28" s="123"/>
+      <c r="AKY28" s="123"/>
+      <c r="AKZ28" s="123"/>
+      <c r="ALA28" s="123"/>
+      <c r="ALB28" s="123"/>
+      <c r="ALC28" s="123"/>
+      <c r="ALD28" s="123"/>
+      <c r="ALE28" s="123"/>
+      <c r="ALF28" s="123"/>
+      <c r="ALG28" s="123"/>
+      <c r="ALH28" s="123"/>
+      <c r="ALI28" s="123"/>
+      <c r="ALJ28" s="123"/>
+      <c r="ALK28" s="123"/>
+      <c r="ALL28" s="123"/>
+      <c r="ALM28" s="123"/>
+      <c r="ALN28" s="123"/>
+      <c r="ALO28" s="123"/>
+      <c r="ALP28" s="123"/>
+      <c r="ALQ28" s="123"/>
+      <c r="ALR28" s="123"/>
+      <c r="ALS28" s="123"/>
+      <c r="ALT28" s="123"/>
+      <c r="ALU28" s="123"/>
+      <c r="ALV28" s="123"/>
+      <c r="ALW28" s="123"/>
+      <c r="ALX28" s="123"/>
+      <c r="ALY28" s="123"/>
+      <c r="ALZ28" s="123"/>
+      <c r="AMA28" s="123"/>
+      <c r="AMB28" s="123"/>
+      <c r="AMC28" s="123"/>
+      <c r="AMD28" s="123"/>
+      <c r="AME28" s="123"/>
+      <c r="AMF28" s="123"/>
+      <c r="AMG28" s="123"/>
+      <c r="AMH28" s="123"/>
+      <c r="AMI28" s="123"/>
+      <c r="AMJ28" s="123"/>
+      <c r="AMK28" s="123"/>
+      <c r="AML28" s="123"/>
+      <c r="AMM28" s="123"/>
     </row>
     <row r="29" spans="1:1027" ht="90" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="87"/>
@@ -21863,7 +21864,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="31" spans="1:1027" ht="180" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="87">
         <v>10</v>
       </c>
@@ -22936,21 +22937,21 @@
         <v>12</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="C33" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="96" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F33" s="36"/>
       <c r="G33" s="97"/>
       <c r="H33" s="97" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I33" s="36" t="s">
         <v>656</v>
@@ -24005,17 +24006,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="127" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
     </row>
     <row r="2" spans="1:9" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -24212,17 +24213,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="128" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
Updated Reg. Client #72
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{27C5C68B-C16A-4AC8-8C14-80DCAD376C0E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1175BF8A-0014-425E-B2C4-7B55B59D97B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6465" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,14 @@
     <sheet name="Resident Services" sheetId="6" r:id="rId6"/>
     <sheet name="Global Configurations" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3149,9 +3156,6 @@
     <t xml:space="preserve">Documents to be uploaded: Mapping of Process (New/UIN Update) + Adult/Child + Gender + Foreigner/Local + Field being updated in case of UIN Update to Document Category + Document Type </t>
   </si>
   <si>
-    <t>UIN Update - Mode of authentication of individual through Registration Client</t>
-  </si>
-  <si>
     <t>Biometric</t>
   </si>
   <si>
@@ -3309,6 +3313,22 @@
   <si>
     <t>Denotes if VIN as a concept if it is applicable for a country or not</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UIN Update - Mode of authentication of individual through Registration Client - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+      </rPr>
+      <t>applicable for v2 only</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -3317,7 +3337,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3529,6 +3549,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -5402,21 +5430,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="3" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="129" t="s">
         <v>0</v>
       </c>
@@ -5430,7 +5458,7 @@
       <c r="I1" s="129"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -5460,7 +5488,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A3" s="67">
         <v>1</v>
       </c>
@@ -5498,7 +5526,7 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>2</v>
@@ -5541,7 +5569,7 @@
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
     </row>
-    <row r="5" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5584,7 +5612,7 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
     </row>
-    <row r="6" spans="1:28" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5627,7 +5655,7 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5670,7 +5698,7 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
     </row>
-    <row r="8" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5713,7 +5741,7 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
     </row>
-    <row r="9" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5756,7 +5784,7 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
     </row>
-    <row r="10" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5799,7 +5827,7 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
     </row>
-    <row r="11" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5842,7 +5870,7 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
     </row>
-    <row r="12" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5885,7 +5913,7 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
     </row>
-    <row r="13" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5928,7 +5956,7 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5990,21 +6018,21 @@
       <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="72" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="16" style="15" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" style="16" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="35.28515625" style="16" customWidth="1"/>
-    <col min="10" max="1025" width="9.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" style="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" style="16" customWidth="1"/>
+    <col min="10" max="1025" width="9.33203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="130" t="s">
         <v>26</v>
       </c>
@@ -6017,7 +6045,7 @@
       <c r="H1" s="130"/>
       <c r="I1" s="130"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -6046,7 +6074,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -6073,7 +6101,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="20" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -6098,7 +6126,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -6125,7 +6153,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -6152,7 +6180,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -6179,7 +6207,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -6206,7 +6234,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>7</v>
       </c>
@@ -6233,7 +6261,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>8</v>
       </c>
@@ -6260,7 +6288,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>9</v>
       </c>
@@ -6287,7 +6315,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>10</v>
       </c>
@@ -6314,7 +6342,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>11</v>
       </c>
@@ -6341,7 +6369,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>12</v>
       </c>
@@ -6366,7 +6394,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>13</v>
       </c>
@@ -6388,21 +6416,21 @@
         <v>622</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>32</v>
@@ -6410,24 +6438,24 @@
       <c r="F16" s="50"/>
       <c r="G16" s="118"/>
       <c r="H16" s="118" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>32</v>
@@ -6435,13 +6463,13 @@
       <c r="F17" s="50"/>
       <c r="G17" s="118"/>
       <c r="H17" s="118" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>15</v>
       </c>
@@ -6462,7 +6490,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>16</v>
       </c>
@@ -6481,7 +6509,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -6500,7 +6528,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>18</v>
       </c>
@@ -6519,7 +6547,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>19</v>
       </c>
@@ -6538,7 +6566,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>20</v>
       </c>
@@ -6557,7 +6585,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>21</v>
       </c>
@@ -6576,7 +6604,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>22</v>
       </c>
@@ -6595,7 +6623,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A26" s="18">
         <v>23</v>
       </c>
@@ -6614,7 +6642,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <v>24</v>
       </c>
@@ -6637,7 +6665,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
         <v>25</v>
       </c>
@@ -6656,7 +6684,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>26</v>
       </c>
@@ -6675,7 +6703,7 @@
       <c r="H29" s="7"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <v>27</v>
       </c>
@@ -6696,7 +6724,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="62"/>
     </row>
-    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <v>28</v>
       </c>
@@ -6733,25 +6761,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AML75"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="46.5703125" style="15" customWidth="1"/>
-    <col min="9" max="1026" width="9.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="46.5546875" style="15" customWidth="1"/>
+    <col min="9" max="1026" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="109" t="s">
         <v>53</v>
       </c>
@@ -6763,7 +6791,7 @@
       <c r="G1" s="109"/>
       <c r="H1" s="109"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -6789,7 +6817,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -6815,7 +6843,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A59" si="0">A3+1</f>
         <v>2</v>
@@ -6842,7 +6870,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6865,7 +6893,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6888,7 +6916,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6915,7 +6943,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6942,7 +6970,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6969,7 +6997,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6996,7 +7024,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7023,7 +7051,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7050,7 +7078,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7077,7 +7105,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7104,7 +7132,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7127,7 +7155,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7150,7 +7178,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7173,7 +7201,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7196,7 +7224,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7217,7 +7245,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7238,7 +7266,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7261,7 +7289,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7284,7 +7312,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -7305,7 +7333,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -7326,7 +7354,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7351,7 +7379,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -7374,7 +7402,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -7399,7 +7427,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -7424,7 +7452,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -7449,7 +7477,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="198" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7476,7 +7504,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="132" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7503,7 +7531,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7530,7 +7558,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="33" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7557,7 +7585,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="34" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7584,7 +7612,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="35" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7611,7 +7639,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="36" spans="1:1026" ht="195" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1026" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7638,7 +7666,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="37" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7659,7 +7687,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="38" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7684,7 +7712,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="39" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7709,7 +7737,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="40" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7736,7 +7764,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="41" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7763,7 +7791,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="42" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -8808,7 +8836,7 @@
       <c r="AMK42" s="15"/>
       <c r="AML42" s="15"/>
     </row>
-    <row r="43" spans="1:1026" ht="120" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1026" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -9851,7 +9879,7 @@
       <c r="AMK43" s="15"/>
       <c r="AML43" s="15"/>
     </row>
-    <row r="44" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9874,7 +9902,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="45" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -9897,7 +9925,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="46" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9920,7 +9948,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="47" spans="1:1026" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1026" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9943,7 +9971,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="48" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9968,7 +9996,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9993,7 +10021,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -10018,7 +10046,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="132" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -10043,7 +10071,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -10066,7 +10094,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -10089,7 +10117,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -10112,7 +10140,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -10135,7 +10163,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -10156,7 +10184,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="375" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -10168,7 +10196,7 @@
         <v>9</v>
       </c>
       <c r="D57" s="36" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E57" s="41"/>
       <c r="F57" s="49"/>
@@ -10179,7 +10207,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="132" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -10204,7 +10232,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -10229,7 +10257,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -10253,7 +10281,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -10277,7 +10305,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -10299,7 +10327,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -10323,7 +10351,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -10347,7 +10375,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -10371,7 +10399,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -10395,7 +10423,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -10417,7 +10445,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -10437,7 +10465,7 @@
       </c>
       <c r="H68" s="36"/>
     </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -10457,7 +10485,7 @@
       </c>
       <c r="H69" s="36"/>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -10477,7 +10505,7 @@
       </c>
       <c r="H70" s="36"/>
     </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -10497,7 +10525,7 @@
       </c>
       <c r="H71" s="36"/>
     </row>
-    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -10517,18 +10545,18 @@
       </c>
       <c r="H72" s="36"/>
     </row>
-    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>72</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>629</v>
+        <v>660</v>
       </c>
       <c r="C73" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E73" s="36" t="s">
         <v>589</v>
@@ -10536,15 +10564,15 @@
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>9</v>
@@ -10554,16 +10582,16 @@
       <c r="F74" s="8"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <f t="shared" ref="A75" si="1">A74+1</f>
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>9</v>
@@ -10573,7 +10601,7 @@
       <c r="F75" s="8"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -10596,21 +10624,21 @@
       <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5703125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="24" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="40.28515625" style="24" customWidth="1"/>
-    <col min="9" max="9" width="62.7109375" style="24" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5546875" style="24" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" style="24" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="62.6640625" style="24" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="131" t="s">
         <v>154</v>
       </c>
@@ -10623,7 +10651,7 @@
       <c r="H1" s="131"/>
       <c r="I1" s="131"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -10652,7 +10680,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -10673,7 +10701,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -10694,7 +10722,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>3</v>
       </c>
@@ -10715,7 +10743,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>4</v>
       </c>
@@ -10736,7 +10764,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>5</v>
       </c>
@@ -10757,7 +10785,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -10778,7 +10806,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -10801,7 +10829,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>8</v>
       </c>
@@ -10824,7 +10852,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -10845,7 +10873,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
         <v>10</v>
       </c>
@@ -10866,7 +10894,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>11</v>
       </c>
@@ -10887,7 +10915,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
         <v>12</v>
       </c>
@@ -10908,7 +10936,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
         <v>13</v>
       </c>
@@ -10929,7 +10957,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="132" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -10952,7 +10980,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -10996,21 +11024,21 @@
       <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="74.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="44.5546875" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1027" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="131" t="s">
         <v>101</v>
       </c>
@@ -11023,7 +11051,7 @@
       <c r="H1" s="131"/>
       <c r="I1" s="131"/>
     </row>
-    <row r="2" spans="1:1027" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1027" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -11052,7 +11080,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:1027" s="84" customFormat="1" ht="315" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" s="84" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
       <c r="A3" s="78">
         <v>1</v>
       </c>
@@ -12093,7 +12121,7 @@
       <c r="AML3" s="83"/>
       <c r="AMM3" s="83"/>
     </row>
-    <row r="4" spans="1:1027" s="84" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1027" s="84" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="78">
         <v>2</v>
       </c>
@@ -13134,7 +13162,7 @@
       <c r="AML4" s="83"/>
       <c r="AMM4" s="83"/>
     </row>
-    <row r="5" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1027" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -13157,7 +13185,7 @@
       <c r="H5" s="57"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -13178,7 +13206,7 @@
       <c r="H6" s="53"/>
       <c r="I6" s="41"/>
     </row>
-    <row r="7" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -13199,7 +13227,7 @@
       <c r="H7" s="53"/>
       <c r="I7" s="41"/>
     </row>
-    <row r="8" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -13222,7 +13250,7 @@
       <c r="H8" s="53"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -13243,7 +13271,7 @@
       <c r="H9" s="53"/>
       <c r="I9" s="41"/>
     </row>
-    <row r="10" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -13264,7 +13292,7 @@
       <c r="H10" s="53"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="85">
         <v>9</v>
       </c>
@@ -14301,7 +14329,7 @@
       <c r="AML11" s="74"/>
       <c r="AMM11" s="74"/>
     </row>
-    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="85">
         <v>10</v>
       </c>
@@ -15338,7 +15366,7 @@
       <c r="AML12" s="74"/>
       <c r="AMM12" s="74"/>
     </row>
-    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="85">
         <v>11</v>
       </c>
@@ -16375,7 +16403,7 @@
       <c r="AML13" s="74"/>
       <c r="AMM13" s="74"/>
     </row>
-    <row r="14" spans="1:1027" s="75" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1027" s="75" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="85">
         <v>12</v>
       </c>
@@ -17412,7 +17440,7 @@
       <c r="AML14" s="74"/>
       <c r="AMM14" s="74"/>
     </row>
-    <row r="15" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>1</v>
       </c>
@@ -17437,7 +17465,7 @@
       </c>
       <c r="I15" s="73"/>
     </row>
-    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>2</v>
       </c>
@@ -17458,13 +17486,13 @@
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I16" s="36" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="17" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1027" ht="224.4" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>3</v>
       </c>
@@ -17485,13 +17513,13 @@
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I17" s="36" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="18" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>4</v>
       </c>
@@ -17518,7 +17546,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="19" spans="1:1027" s="84" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="78">
         <v>17</v>
       </c>
@@ -18555,7 +18583,7 @@
       <c r="AML19" s="83"/>
       <c r="AMM19" s="83"/>
     </row>
-    <row r="20" spans="1:1027" s="84" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="78">
         <v>18</v>
       </c>
@@ -19592,7 +19620,7 @@
       <c r="AML20" s="83"/>
       <c r="AMM20" s="83"/>
     </row>
-    <row r="21" spans="1:1027" s="94" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1027" s="94" customFormat="1" ht="39.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="87"/>
       <c r="B21" s="88" t="s">
         <v>130</v>
@@ -20631,7 +20659,7 @@
       <c r="AML21" s="93"/>
       <c r="AMM21" s="93"/>
     </row>
-    <row r="22" spans="1:1027" ht="210" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1027" ht="184.8" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A22" s="87">
         <v>5</v>
       </c>
@@ -20658,7 +20686,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="23" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="87">
         <v>6</v>
       </c>
@@ -20677,13 +20705,13 @@
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="36" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I23" s="36" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="24" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="87">
         <v>7</v>
       </c>
@@ -20708,7 +20736,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="25" spans="1:1027" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1027" ht="138" x14ac:dyDescent="0.3">
       <c r="A25" s="111">
         <v>19</v>
       </c>
@@ -20735,7 +20763,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="26" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A26" s="87">
         <v>8</v>
       </c>
@@ -20762,10 +20790,10 @@
         <v>591</v>
       </c>
     </row>
-    <row r="27" spans="1:1027" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1027" ht="26.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" s="87"/>
       <c r="B27" s="88" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C27" s="89" t="s">
         <v>9</v>
@@ -20779,7 +20807,7 @@
       <c r="H27" s="36"/>
       <c r="I27" s="41"/>
     </row>
-    <row r="28" spans="1:1027" s="124" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1027" s="124" customFormat="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A28" s="120"/>
       <c r="B28" s="121" t="s">
         <v>138</v>
@@ -21814,7 +21842,7 @@
       <c r="AML28" s="123"/>
       <c r="AMM28" s="123"/>
     </row>
-    <row r="29" spans="1:1027" ht="90" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1027" ht="79.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A29" s="87"/>
       <c r="B29" s="88" t="s">
         <v>161</v>
@@ -21835,7 +21863,7 @@
       <c r="H29" s="36"/>
       <c r="I29" s="41"/>
     </row>
-    <row r="30" spans="1:1027" ht="195" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1027" ht="171.6" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A30" s="87">
         <v>9</v>
       </c>
@@ -21860,7 +21888,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="31" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="87">
         <v>10</v>
       </c>
@@ -21885,7 +21913,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="32" spans="1:1027" s="128" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1027" s="128" customFormat="1" ht="138" x14ac:dyDescent="0.3">
       <c r="A32" s="85">
         <v>11</v>
       </c>
@@ -21902,14 +21930,14 @@
         <v>5</v>
       </c>
       <c r="F32" s="72" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G32" s="126"/>
       <c r="H32" s="126" t="s">
         <v>356</v>
       </c>
       <c r="I32" s="72" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J32" s="127"/>
       <c r="K32" s="127"/>
@@ -22930,29 +22958,29 @@
       <c r="AML32" s="127"/>
       <c r="AMM32" s="127"/>
     </row>
-    <row r="33" spans="1:1027" s="99" customFormat="1" ht="162.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1027" s="99" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="87">
         <v>11</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C33" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="96" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F33" s="36"/>
       <c r="G33" s="97"/>
       <c r="H33" s="97" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I33" s="36" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J33" s="98"/>
       <c r="K33" s="98"/>
@@ -23990,20 +24018,20 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="29.5703125" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="29.5546875" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="131" t="s">
         <v>139</v>
       </c>
@@ -24016,7 +24044,7 @@
       <c r="H1" s="131"/>
       <c r="I1" s="131"/>
     </row>
-    <row r="2" spans="1:9" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -24045,7 +24073,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -24062,7 +24090,7 @@
       <c r="H3" s="41"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -24079,7 +24107,7 @@
       <c r="H4" s="41"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -24096,7 +24124,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -24113,7 +24141,7 @@
       <c r="H6" s="41"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -24130,7 +24158,7 @@
       <c r="H7" s="41"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -24147,7 +24175,7 @@
       <c r="H8" s="41"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -24164,7 +24192,7 @@
       <c r="H9" s="41"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -24192,25 +24220,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMK53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C49" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView topLeftCell="A45" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.28515625" style="3" customWidth="1"/>
-    <col min="10" max="1025" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="84.33203125" style="3" customWidth="1"/>
+    <col min="10" max="1025" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="132" t="s">
         <v>193</v>
       </c>
@@ -24223,7 +24251,7 @@
       <c r="H1" s="133"/>
       <c r="I1" s="133"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -24252,7 +24280,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -24294,7 +24322,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f>A3+1</f>
         <v>2</v>
@@ -24337,7 +24365,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" ref="A5:A41" si="0">A4+1</f>
         <v>3</v>
@@ -24380,7 +24408,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -24421,7 +24449,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f>A9+1</f>
         <v>7</v>
@@ -24464,7 +24492,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f>A6+1</f>
         <v>5</v>
@@ -24505,7 +24533,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -24546,7 +24574,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -24572,7 +24600,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f>A7+1</f>
         <v>8</v>
@@ -24615,7 +24643,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -24658,7 +24686,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="9" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f>A12+1</f>
         <v>10</v>
@@ -24699,7 +24727,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" s="9" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="9" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f>A13+1</f>
         <v>11</v>
@@ -24742,7 +24770,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" ref="A15:A22" si="1">A14+1</f>
         <v>12</v>
@@ -24783,7 +24811,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -24824,7 +24852,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:1025" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1025" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -24865,7 +24893,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="71">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -25901,7 +25929,7 @@
       <c r="AMJ18" s="74"/>
       <c r="AMK18" s="74"/>
     </row>
-    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="71">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -26937,7 +26965,7 @@
       <c r="AMJ19" s="74"/>
       <c r="AMK19" s="74"/>
     </row>
-    <row r="20" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -26963,7 +26991,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="21" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -26989,7 +27017,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="22" spans="1:1025" s="75" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1025" s="75" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="71">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -28027,7 +28055,7 @@
       <c r="AMJ22" s="74"/>
       <c r="AMK22" s="74"/>
     </row>
-    <row r="23" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -28053,7 +28081,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -28077,7 +28105,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="25" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -28101,7 +28129,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="26" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -28125,7 +28153,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="27" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -28149,7 +28177,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="28" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -28173,7 +28201,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="29" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -28197,7 +28225,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -28221,7 +28249,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="31" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -28245,7 +28273,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="32" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -28269,7 +28297,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -28293,7 +28321,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -29327,7 +29355,7 @@
       <c r="AMJ34" s="74"/>
       <c r="AMK34" s="74"/>
     </row>
-    <row r="35" spans="1:1025" ht="210" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1025" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -29351,7 +29379,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1025" ht="132" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -29375,7 +29403,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1025" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -29399,7 +29427,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -29423,7 +29451,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -29445,7 +29473,7 @@
       </c>
       <c r="I39" s="41"/>
     </row>
-    <row r="40" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -29469,7 +29497,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1025" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -29493,7 +29521,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>39</v>
       </c>
@@ -29516,7 +29544,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>40</v>
       </c>
@@ -29539,7 +29567,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1025" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>41</v>
       </c>
@@ -29562,7 +29590,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>42</v>
       </c>
@@ -29585,7 +29613,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>43</v>
       </c>
@@ -29608,7 +29636,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>44</v>
       </c>
@@ -29631,7 +29659,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="48" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>45</v>
       </c>
@@ -29652,7 +29680,7 @@
       </c>
       <c r="I48" s="36"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>46</v>
       </c>
@@ -29673,7 +29701,7 @@
       </c>
       <c r="I49" s="36"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>47</v>
       </c>
@@ -29694,7 +29722,7 @@
       </c>
       <c r="I50" s="36"/>
     </row>
-    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>48</v>
       </c>
@@ -29717,7 +29745,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>49</v>
       </c>
@@ -29740,29 +29768,29 @@
         <v>596</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>50</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="13" t="s">
+        <v>657</v>
+      </c>
+      <c r="E53" s="36" t="s">
         <v>658</v>
-      </c>
-      <c r="E53" s="36" t="s">
-        <v>659</v>
       </c>
       <c r="F53" s="41"/>
       <c r="G53" s="41"/>
       <c r="H53" s="104" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I53" s="36" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated reg. client #16
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{70C4B283-822D-42B8-827D-A72E1AD9618B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD20A33-D0B7-4227-B68D-F83483759E97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8535" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,19 @@
     <sheet name="Resident Services" sheetId="6" r:id="rId6"/>
     <sheet name="Global Configurations" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="644">
   <si>
     <r>
       <rPr>
@@ -3261,6 +3268,9 @@
   </si>
   <si>
     <t>auth.types.allowed</t>
+  </si>
+  <si>
+    <t>“Dear [Individual full name], Thank you for registering with Digital Identity platform. Your registration id is [Registration ID]."</t>
   </si>
 </sst>
 </file>
@@ -5320,21 +5330,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="3" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
@@ -5348,7 +5358,7 @@
       <c r="I1" s="118"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -5378,7 +5388,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A3" s="67">
         <v>1</v>
       </c>
@@ -5416,7 +5426,7 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>2</v>
@@ -5459,7 +5469,7 @@
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
     </row>
-    <row r="5" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5502,7 +5512,7 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
     </row>
-    <row r="6" spans="1:28" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5545,7 +5555,7 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5588,7 +5598,7 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
     </row>
-    <row r="8" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5631,7 +5641,7 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
     </row>
-    <row r="9" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5674,7 +5684,7 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
     </row>
-    <row r="10" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5717,7 +5727,7 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
     </row>
-    <row r="11" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5760,7 +5770,7 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
     </row>
-    <row r="12" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5803,7 +5813,7 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
     </row>
-    <row r="13" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5846,7 +5856,7 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5908,21 +5918,21 @@
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="72" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="16" style="15" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" style="16" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="35.28515625" style="16" customWidth="1"/>
-    <col min="10" max="1025" width="9.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" style="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" style="16" customWidth="1"/>
+    <col min="10" max="1025" width="9.33203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="119" t="s">
         <v>26</v>
       </c>
@@ -5935,7 +5945,7 @@
       <c r="H1" s="119"/>
       <c r="I1" s="119"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -5964,7 +5974,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -5991,7 +6001,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="20" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -6016,7 +6026,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -6043,7 +6053,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -6070,7 +6080,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -6097,7 +6107,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -6124,7 +6134,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>7</v>
       </c>
@@ -6151,7 +6161,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>8</v>
       </c>
@@ -6178,7 +6188,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>9</v>
       </c>
@@ -6205,7 +6215,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>10</v>
       </c>
@@ -6232,7 +6242,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>11</v>
       </c>
@@ -6259,7 +6269,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>12</v>
       </c>
@@ -6284,7 +6294,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>13</v>
       </c>
@@ -6307,7 +6317,7 @@
       </c>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>14</v>
       </c>
@@ -6328,7 +6338,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -6347,7 +6357,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>16</v>
       </c>
@@ -6366,7 +6376,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>17</v>
       </c>
@@ -6385,7 +6395,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>18</v>
       </c>
@@ -6404,7 +6414,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>19</v>
       </c>
@@ -6423,7 +6433,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>20</v>
       </c>
@@ -6442,7 +6452,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>21</v>
       </c>
@@ -6461,7 +6471,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>22</v>
       </c>
@@ -6480,7 +6490,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>23</v>
       </c>
@@ -6503,7 +6513,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A26" s="18">
         <v>24</v>
       </c>
@@ -6522,7 +6532,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <v>25</v>
       </c>
@@ -6541,7 +6551,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
         <v>26</v>
       </c>
@@ -6562,7 +6572,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="62"/>
     </row>
-    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>27</v>
       </c>
@@ -6599,25 +6609,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AML75"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="46.5703125" style="15" customWidth="1"/>
-    <col min="9" max="1026" width="9.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="46.5546875" style="15" customWidth="1"/>
+    <col min="9" max="1026" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="109" t="s">
         <v>53</v>
       </c>
@@ -6629,7 +6639,7 @@
       <c r="G1" s="109"/>
       <c r="H1" s="109"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -6655,7 +6665,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -6681,7 +6691,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A59" si="0">A3+1</f>
         <v>2</v>
@@ -6708,7 +6718,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6731,7 +6741,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6754,7 +6764,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6781,7 +6791,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6808,7 +6818,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6835,7 +6845,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6862,7 +6872,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6889,7 +6899,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6916,7 +6926,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6943,7 +6953,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6970,7 +6980,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6993,7 +7003,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7016,7 +7026,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7039,7 +7049,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7050,7 +7060,9 @@
       <c r="C18" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="7" t="s">
+        <v>643</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
         <v>11</v>
@@ -7062,7 +7074,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7083,7 +7095,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7104,7 +7116,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7127,7 +7139,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7150,7 +7162,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -7171,7 +7183,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -7192,7 +7204,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7217,7 +7229,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -7240,7 +7252,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -7265,7 +7277,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -7290,7 +7302,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -7315,7 +7327,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="198" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7342,7 +7354,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="132" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7369,7 +7381,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7396,7 +7408,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="33" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7423,7 +7435,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="34" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7450,7 +7462,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="35" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7477,7 +7489,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="36" spans="1:1026" ht="195" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1026" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7504,7 +7516,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="37" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7525,7 +7537,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7550,7 +7562,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="39" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7575,7 +7587,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="40" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7602,7 +7614,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="41" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7629,7 +7641,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="42" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -8674,7 +8686,7 @@
       <c r="AMK42" s="15"/>
       <c r="AML42" s="15"/>
     </row>
-    <row r="43" spans="1:1026" ht="120" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1026" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -9717,7 +9729,7 @@
       <c r="AMK43" s="15"/>
       <c r="AML43" s="15"/>
     </row>
-    <row r="44" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9740,7 +9752,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="45" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -9763,7 +9775,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="46" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9786,7 +9798,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="47" spans="1:1026" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1026" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9809,7 +9821,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="48" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9834,7 +9846,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9859,7 +9871,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9884,7 +9896,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="132" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9909,7 +9921,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9932,7 +9944,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -9955,7 +9967,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -9978,7 +9990,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -10001,7 +10013,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -10022,7 +10034,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="375" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -10045,7 +10057,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="132" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -10070,7 +10082,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -10095,7 +10107,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -10119,7 +10131,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -10143,7 +10155,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -10165,7 +10177,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -10189,7 +10201,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -10213,7 +10225,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -10237,7 +10249,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -10261,7 +10273,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -10283,7 +10295,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -10303,7 +10315,7 @@
       </c>
       <c r="H68" s="36"/>
     </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -10323,7 +10335,7 @@
       </c>
       <c r="H69" s="36"/>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -10343,7 +10355,7 @@
       </c>
       <c r="H70" s="36"/>
     </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -10363,7 +10375,7 @@
       </c>
       <c r="H71" s="36"/>
     </row>
-    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -10383,7 +10395,7 @@
       </c>
       <c r="H72" s="36"/>
     </row>
-    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -10405,7 +10417,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -10423,7 +10435,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <f t="shared" ref="A75" si="1">A74+1</f>
         <v>74</v>
@@ -10462,21 +10474,21 @@
       <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5703125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="24" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="40.28515625" style="24" customWidth="1"/>
-    <col min="9" max="9" width="62.7109375" style="24" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5546875" style="24" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" style="24" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="62.6640625" style="24" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="120" t="s">
         <v>155</v>
       </c>
@@ -10489,7 +10501,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -10518,7 +10530,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -10539,7 +10551,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -10560,7 +10572,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>3</v>
       </c>
@@ -10581,7 +10593,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>4</v>
       </c>
@@ -10602,7 +10614,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>5</v>
       </c>
@@ -10623,7 +10635,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -10644,7 +10656,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -10667,7 +10679,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>8</v>
       </c>
@@ -10690,7 +10702,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -10711,7 +10723,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
         <v>10</v>
       </c>
@@ -10732,7 +10744,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>11</v>
       </c>
@@ -10753,7 +10765,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
         <v>12</v>
       </c>
@@ -10774,7 +10786,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
         <v>13</v>
       </c>
@@ -10795,7 +10807,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="132" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -10818,7 +10830,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -10855,28 +10867,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMM32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="74.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="44.5546875" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1027" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="120" t="s">
         <v>101</v>
       </c>
@@ -10889,7 +10901,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:1027" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1027" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -10918,7 +10930,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:1027" s="84" customFormat="1" ht="330" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" s="84" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
       <c r="A3" s="78">
         <v>1</v>
       </c>
@@ -11959,7 +11971,7 @@
       <c r="AML3" s="83"/>
       <c r="AMM3" s="83"/>
     </row>
-    <row r="4" spans="1:1027" s="84" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1027" s="84" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="78">
         <v>2</v>
       </c>
@@ -13000,7 +13012,7 @@
       <c r="AML4" s="83"/>
       <c r="AMM4" s="83"/>
     </row>
-    <row r="5" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1027" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -13023,7 +13035,7 @@
       <c r="H5" s="57"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -13044,7 +13056,7 @@
       <c r="H6" s="53"/>
       <c r="I6" s="41"/>
     </row>
-    <row r="7" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -13065,7 +13077,7 @@
       <c r="H7" s="53"/>
       <c r="I7" s="41"/>
     </row>
-    <row r="8" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -13088,7 +13100,7 @@
       <c r="H8" s="53"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -13109,7 +13121,7 @@
       <c r="H9" s="53"/>
       <c r="I9" s="41"/>
     </row>
-    <row r="10" spans="1:1027" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1027" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -13130,7 +13142,7 @@
       <c r="H10" s="53"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="85">
         <v>9</v>
       </c>
@@ -14167,7 +14179,7 @@
       <c r="AML11" s="74"/>
       <c r="AMM11" s="74"/>
     </row>
-    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="85">
         <v>10</v>
       </c>
@@ -15204,7 +15216,7 @@
       <c r="AML12" s="74"/>
       <c r="AMM12" s="74"/>
     </row>
-    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="85">
         <v>11</v>
       </c>
@@ -16241,7 +16253,7 @@
       <c r="AML13" s="74"/>
       <c r="AMM13" s="74"/>
     </row>
-    <row r="14" spans="1:1027" s="75" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1027" s="75" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="85">
         <v>12</v>
       </c>
@@ -17278,7 +17290,7 @@
       <c r="AML14" s="74"/>
       <c r="AMM14" s="74"/>
     </row>
-    <row r="15" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1027" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>1</v>
       </c>
@@ -17305,7 +17317,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>2</v>
       </c>
@@ -17332,7 +17344,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="17" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1027" ht="224.4" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>3</v>
       </c>
@@ -17359,7 +17371,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="18" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>4</v>
       </c>
@@ -17386,7 +17398,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="19" spans="1:1027" s="84" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="78">
         <v>17</v>
       </c>
@@ -18423,7 +18435,7 @@
       <c r="AML19" s="83"/>
       <c r="AMM19" s="83"/>
     </row>
-    <row r="20" spans="1:1027" s="84" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="78">
         <v>18</v>
       </c>
@@ -19460,7 +19472,7 @@
       <c r="AML20" s="83"/>
       <c r="AMM20" s="83"/>
     </row>
-    <row r="21" spans="1:1027" s="94" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1027" s="94" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A21" s="87"/>
       <c r="B21" s="88" t="s">
         <v>130</v>
@@ -20499,7 +20511,7 @@
       <c r="AML21" s="93"/>
       <c r="AMM21" s="93"/>
     </row>
-    <row r="22" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A22" s="87">
         <v>5</v>
       </c>
@@ -20526,7 +20538,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="23" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="87">
         <v>6</v>
       </c>
@@ -20551,7 +20563,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="24" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="87">
         <v>7</v>
       </c>
@@ -20576,7 +20588,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="25" spans="1:1027" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1027" ht="138" x14ac:dyDescent="0.3">
       <c r="A25" s="111">
         <v>19</v>
       </c>
@@ -20603,7 +20615,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A26" s="87">
         <v>8</v>
       </c>
@@ -20630,7 +20642,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="27" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="87"/>
       <c r="B27" s="88" t="s">
         <v>138</v>
@@ -20647,7 +20659,7 @@
       <c r="H27" s="36"/>
       <c r="I27" s="41"/>
     </row>
-    <row r="28" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A28" s="87"/>
       <c r="B28" s="88" t="s">
         <v>139</v>
@@ -20664,7 +20676,7 @@
       <c r="H28" s="36"/>
       <c r="I28" s="41"/>
     </row>
-    <row r="29" spans="1:1027" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1027" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A29" s="87"/>
       <c r="B29" s="88" t="s">
         <v>162</v>
@@ -20685,7 +20697,7 @@
       <c r="H29" s="36"/>
       <c r="I29" s="41"/>
     </row>
-    <row r="30" spans="1:1027" ht="195" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1027" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A30" s="87">
         <v>9</v>
       </c>
@@ -20710,7 +20722,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="31" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="87">
         <v>10</v>
       </c>
@@ -20735,7 +20747,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="32" spans="1:1027" s="99" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1027" s="99" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="87">
         <v>11</v>
       </c>
@@ -21795,20 +21807,20 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="29.5703125" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="29.5546875" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="120" t="s">
         <v>140</v>
       </c>
@@ -21821,7 +21833,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:9" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -21850,7 +21862,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -21867,7 +21879,7 @@
       <c r="H3" s="41"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -21884,7 +21896,7 @@
       <c r="H4" s="41"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -21901,7 +21913,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -21918,7 +21930,7 @@
       <c r="H6" s="41"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -21935,7 +21947,7 @@
       <c r="H7" s="41"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -21952,7 +21964,7 @@
       <c r="H8" s="41"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -21969,7 +21981,7 @@
       <c r="H9" s="41"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -21997,25 +22009,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMK52"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A49" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.28515625" style="3" customWidth="1"/>
-    <col min="10" max="1025" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="84.33203125" style="3" customWidth="1"/>
+    <col min="10" max="1025" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="121" t="s">
         <v>194</v>
       </c>
@@ -22028,7 +22040,7 @@
       <c r="H1" s="122"/>
       <c r="I1" s="122"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -22057,7 +22069,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -22099,7 +22111,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f>A3+1</f>
         <v>2</v>
@@ -22142,7 +22154,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" ref="A5:A41" si="0">A4+1</f>
         <v>3</v>
@@ -22185,7 +22197,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -22226,7 +22238,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f>A9+1</f>
         <v>7</v>
@@ -22269,7 +22281,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f>A6+1</f>
         <v>5</v>
@@ -22310,7 +22322,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -22351,7 +22363,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -22377,7 +22389,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f>A7+1</f>
         <v>8</v>
@@ -22420,7 +22432,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -22463,7 +22475,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="9" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f>A12+1</f>
         <v>10</v>
@@ -22504,7 +22516,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" s="9" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="9" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f>A13+1</f>
         <v>11</v>
@@ -22547,7 +22559,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" ref="A15:A22" si="1">A14+1</f>
         <v>12</v>
@@ -22588,7 +22600,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -22629,7 +22641,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:1025" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1025" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -22670,7 +22682,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="71">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -23706,7 +23718,7 @@
       <c r="AMJ18" s="74"/>
       <c r="AMK18" s="74"/>
     </row>
-    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="71">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -24742,7 +24754,7 @@
       <c r="AMJ19" s="74"/>
       <c r="AMK19" s="74"/>
     </row>
-    <row r="20" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -24768,7 +24780,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="21" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -24794,7 +24806,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="22" spans="1:1025" s="75" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1025" s="75" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="71">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -25832,7 +25844,7 @@
       <c r="AMJ22" s="74"/>
       <c r="AMK22" s="74"/>
     </row>
-    <row r="23" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -25858,7 +25870,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="24" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -25882,7 +25894,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="25" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -25906,7 +25918,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="26" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -25930,7 +25942,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="27" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -25954,7 +25966,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -25978,7 +25990,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="29" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -26002,7 +26014,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="30" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -26026,7 +26038,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="31" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -26050,7 +26062,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="32" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -26074,7 +26086,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -26098,7 +26110,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -27132,7 +27144,7 @@
       <c r="AMJ34" s="74"/>
       <c r="AMK34" s="74"/>
     </row>
-    <row r="35" spans="1:1025" ht="210" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1025" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -27156,7 +27168,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1025" ht="132" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -27180,7 +27192,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1025" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -27204,7 +27216,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -27228,7 +27240,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -27250,7 +27262,7 @@
       </c>
       <c r="I39" s="41"/>
     </row>
-    <row r="40" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -27274,7 +27286,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1025" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -27298,7 +27310,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>39</v>
       </c>
@@ -27321,7 +27333,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>40</v>
       </c>
@@ -27344,7 +27356,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1025" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>41</v>
       </c>
@@ -27367,7 +27379,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="45" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>42</v>
       </c>
@@ -27390,7 +27402,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>43</v>
       </c>
@@ -27413,7 +27425,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>44</v>
       </c>
@@ -27436,7 +27448,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="48" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>45</v>
       </c>
@@ -27457,7 +27469,7 @@
       </c>
       <c r="I48" s="36"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>46</v>
       </c>
@@ -27478,7 +27490,7 @@
       </c>
       <c r="I49" s="36"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>47</v>
       </c>
@@ -27499,7 +27511,7 @@
       </c>
       <c r="I50" s="36"/>
     </row>
-    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>48</v>
       </c>
@@ -27522,7 +27534,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Updated a global config
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD20A33-D0B7-4227-B68D-F83483759E97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4ECD28D1-711A-428F-A2F5-5EC4071A0C1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8535" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,12 @@
     <sheet name="Resident Services" sheetId="6" r:id="rId6"/>
     <sheet name="Global Configurations" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="648">
   <si>
     <r>
       <rPr>
@@ -2454,10 +2447,6 @@
 Registration: Validate that the email entered in demographic details does not exceed the maximum length.</t>
   </si>
   <si>
-    <t>IDA: The auth and OTP notifications will be sent both in primary and secondary  language. The eKYC response will be sent both in primary and secondary language
-Registration: All static content will display in the primary language. For demographic details, preview and acknowledgement pages: display static content and user entry in left hand side in primary and right hand side in secondary language.</t>
-  </si>
-  <si>
     <t>This configuration will impact both the Pre-Registration and Registration Client.
 This will validate the size of the document being uploaded
 Registration: Validates that the document uploaded does not exceed the maximum size configured.</t>
@@ -3038,11 +3027,6 @@
 </t>
   </si>
   <si>
-    <t>IDA: The auth and OTP notifications will be sent in the primary language configured. The eKYC response will be sent in primary language configured.  
-Registration: All static content will display in the primary language. For demographic details, preview and acknowledgement pages: display static content and user entry in left hand side in primary and right hand side in secondary language.
-Registration Processor: If Primary Language is Updated the Master Data and Notification will be fetched using New Primary Language but if Data is not present in the New Primary Language then the System will throw an error.</t>
-  </si>
-  <si>
     <t>Registration Processor: If Notification type is Changed and for the change implementation is done then, Notification will be sent based on the New Notification Type but if implementation is not done then system will throw an error.
 IDA: The auth notifications will be triggered based on this configuration</t>
   </si>
@@ -3271,6 +3255,27 @@
   </si>
   <si>
     <t>“Dear [Individual full name], Thank you for registering with Digital Identity platform. Your registration id is [Registration ID]."</t>
+  </si>
+  <si>
+    <t>Language to trigger Notification</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>IDA: The primary language to trigger auth and OTP notification and eKYC response  is set using this configuration
+Registration: All static content will display in the primary language. For demographic details, preview and acknowledgement pages: display static content and user entry in left hand side in primary and right hand side in secondary language.
+Registration Processor: If Primary Language is Updated the Master Data and Notification will be fetched using New Primary Language but if Data is not present in the New Primary Language then the System will throw an error.</t>
+  </si>
+  <si>
+    <t>IDA: The secondary language to trigger auth and OTP notification and eKYC response  is set using this configuration
+Registration: All static content will display in the primary language. For demographic details, preview and acknowledgement pages: display static content and user entry in left hand side in primary and right hand side in secondary language.</t>
+  </si>
+  <si>
+    <t>IDA: The language "primary" or "both" in which the notification/eKYC response has to be triggered is set by this configuration</t>
   </si>
 </sst>
 </file>
@@ -5330,21 +5335,21 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="3" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
@@ -5358,7 +5363,7 @@
       <c r="I1" s="118"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -5388,7 +5393,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="67">
         <v>1</v>
       </c>
@@ -5426,7 +5431,7 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>2</v>
@@ -5469,7 +5474,7 @@
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
     </row>
-    <row r="5" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5512,7 +5517,7 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
     </row>
-    <row r="6" spans="1:28" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5555,7 +5560,7 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5598,7 +5603,7 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
     </row>
-    <row r="8" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5641,7 +5646,7 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
     </row>
-    <row r="9" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5684,7 +5689,7 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
     </row>
-    <row r="10" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5727,7 +5732,7 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
     </row>
-    <row r="11" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5770,7 +5775,7 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
     </row>
-    <row r="12" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5813,7 +5818,7 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
     </row>
-    <row r="13" spans="1:28" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5856,7 +5861,7 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5918,21 +5923,21 @@
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="14" customWidth="1"/>
     <col min="2" max="2" width="72" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="15" customWidth="1"/>
     <col min="5" max="5" width="16" style="15" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" style="16" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="35.33203125" style="16" customWidth="1"/>
-    <col min="10" max="1025" width="9.33203125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="35.28515625" style="16" customWidth="1"/>
+    <col min="10" max="1025" width="9.28515625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="119" t="s">
         <v>26</v>
       </c>
@@ -5945,7 +5950,7 @@
       <c r="H1" s="119"/>
       <c r="I1" s="119"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -5974,7 +5979,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -5995,13 +6000,13 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="20" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -6020,18 +6025,18 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>9</v>
@@ -6053,7 +6058,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -6074,13 +6079,13 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -6101,13 +6106,13 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -6128,40 +6133,40 @@
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="101" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>8</v>
       </c>
@@ -6188,7 +6193,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>9</v>
       </c>
@@ -6215,7 +6220,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>10</v>
       </c>
@@ -6236,13 +6241,13 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="115" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>11</v>
       </c>
@@ -6259,7 +6264,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
@@ -6269,7 +6274,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>12</v>
       </c>
@@ -6294,18 +6299,18 @@
         <v>366</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>32</v>
@@ -6313,11 +6318,11 @@
       <c r="F15" s="50"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>14</v>
       </c>
@@ -6338,7 +6343,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -6357,7 +6362,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>16</v>
       </c>
@@ -6376,7 +6381,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>17</v>
       </c>
@@ -6395,7 +6400,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>18</v>
       </c>
@@ -6414,7 +6419,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>19</v>
       </c>
@@ -6433,7 +6438,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>20</v>
       </c>
@@ -6452,7 +6457,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>21</v>
       </c>
@@ -6471,7 +6476,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>22</v>
       </c>
@@ -6490,7 +6495,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>23</v>
       </c>
@@ -6513,7 +6518,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>24</v>
       </c>
@@ -6532,7 +6537,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>25</v>
       </c>
@@ -6551,7 +6556,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>26</v>
       </c>
@@ -6572,7 +6577,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="62"/>
     </row>
-    <row r="29" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>27</v>
       </c>
@@ -6609,25 +6614,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AML75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="46.5546875" style="15" customWidth="1"/>
-    <col min="9" max="1026" width="9.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="46.5703125" style="15" customWidth="1"/>
+    <col min="9" max="1026" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="109" t="s">
         <v>53</v>
       </c>
@@ -6639,7 +6644,7 @@
       <c r="G1" s="109"/>
       <c r="H1" s="109"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -6665,7 +6670,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -6688,10 +6693,10 @@
         <v>427</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="211.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A59" si="0">A3+1</f>
         <v>2</v>
@@ -6715,10 +6720,10 @@
         <v>428</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6741,7 +6746,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6761,10 +6766,10 @@
         <v>279</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6788,10 +6793,10 @@
         <v>429</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6815,10 +6820,10 @@
         <v>430</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6842,10 +6847,10 @@
         <v>431</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6869,10 +6874,10 @@
         <v>432</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6896,10 +6901,10 @@
         <v>279</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6923,10 +6928,10 @@
         <v>279</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6950,10 +6955,10 @@
         <v>427</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6977,10 +6982,10 @@
         <v>427</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7000,10 +7005,10 @@
         <v>279</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7023,10 +7028,10 @@
         <v>279</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7046,10 +7051,10 @@
         <v>433</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7061,7 +7066,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
@@ -7071,10 +7076,10 @@
         <v>433</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7095,7 +7100,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7116,7 +7121,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7136,10 +7141,10 @@
         <v>434</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7159,10 +7164,10 @@
         <v>434</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -7183,7 +7188,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -7204,7 +7209,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="250.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7226,10 +7231,10 @@
         <v>435</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -7249,10 +7254,10 @@
         <v>436</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -7274,10 +7279,10 @@
         <v>437</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -7299,10 +7304,10 @@
         <v>279</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -7324,10 +7329,10 @@
         <v>438</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="198" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7351,10 +7356,10 @@
         <v>439</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7378,10 +7383,10 @@
         <v>440</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7405,10 +7410,10 @@
         <v>442</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
-    <row r="33" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7432,10 +7437,10 @@
         <v>444</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
-    <row r="34" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7459,10 +7464,10 @@
         <v>445</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
-    <row r="35" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7486,10 +7491,10 @@
         <v>446</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
-    <row r="36" spans="1:1026" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1026" ht="195" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7513,10 +7518,10 @@
         <v>446</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
-    <row r="37" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7537,7 +7542,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7559,10 +7564,10 @@
         <v>449</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
-    <row r="39" spans="1:1026" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1026" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7584,10 +7589,10 @@
         <v>450</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
-    <row r="40" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7611,10 +7616,10 @@
         <v>427</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
-    <row r="41" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7638,10 +7643,10 @@
         <v>427</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
-    <row r="42" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -7665,7 +7670,7 @@
         <v>451</v>
       </c>
       <c r="H42" s="45" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -8686,7 +8691,7 @@
       <c r="AMK42" s="15"/>
       <c r="AML42" s="15"/>
     </row>
-    <row r="43" spans="1:1026" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1026" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -8708,7 +8713,7 @@
         <v>452</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -9729,7 +9734,7 @@
       <c r="AMK43" s="15"/>
       <c r="AML43" s="15"/>
     </row>
-    <row r="44" spans="1:1026" ht="66" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9749,10 +9754,10 @@
         <v>453</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
-    <row r="45" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -9772,10 +9777,10 @@
         <v>142</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
-    <row r="46" spans="1:1026" ht="132" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1026" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9795,10 +9800,10 @@
         <v>440</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
-    <row r="47" spans="1:1026" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1026" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9818,10 +9823,10 @@
         <v>454</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
-    <row r="48" spans="1:1026" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9843,10 +9848,10 @@
         <v>455</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9868,10 +9873,10 @@
         <v>456</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9893,10 +9898,10 @@
         <v>457</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9918,10 +9923,10 @@
         <v>459</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9941,10 +9946,10 @@
         <v>460</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -9964,10 +9969,10 @@
         <v>461</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -9987,10 +9992,10 @@
         <v>444</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -10010,16 +10015,16 @@
         <v>461</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C56" s="37" t="s">
         <v>9</v>
@@ -10031,10 +10036,10 @@
         <v>461</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="375" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -10046,7 +10051,7 @@
         <v>9</v>
       </c>
       <c r="D57" s="36" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E57" s="41"/>
       <c r="F57" s="49"/>
@@ -10054,10 +10059,10 @@
         <v>462</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -10079,10 +10084,10 @@
         <v>463</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -10104,10 +10109,10 @@
         <v>464</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -10128,10 +10133,10 @@
         <v>468</v>
       </c>
       <c r="H60" s="36" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -10152,10 +10157,10 @@
         <v>470</v>
       </c>
       <c r="H61" s="36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -10174,10 +10179,10 @@
         <v>472</v>
       </c>
       <c r="H62" s="36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -10198,10 +10203,10 @@
         <v>474</v>
       </c>
       <c r="H63" s="36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -10222,10 +10227,10 @@
         <v>476</v>
       </c>
       <c r="H64" s="36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -10246,10 +10251,10 @@
         <v>478</v>
       </c>
       <c r="H65" s="36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -10270,10 +10275,10 @@
         <v>480</v>
       </c>
       <c r="H66" s="36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -10292,10 +10297,10 @@
         <v>482</v>
       </c>
       <c r="H67" s="36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -10315,7 +10320,7 @@
       </c>
       <c r="H68" s="36"/>
     </row>
-    <row r="69" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -10335,7 +10340,7 @@
       </c>
       <c r="H69" s="36"/>
     </row>
-    <row r="70" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -10355,7 +10360,7 @@
       </c>
       <c r="H70" s="36"/>
     </row>
-    <row r="71" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -10375,7 +10380,7 @@
       </c>
       <c r="H71" s="36"/>
     </row>
-    <row r="72" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -10395,34 +10400,34 @@
       </c>
       <c r="H72" s="36"/>
     </row>
-    <row r="73" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>72</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C73" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E73" s="36" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>9</v>
@@ -10432,16 +10437,16 @@
       <c r="F74" s="8"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <f t="shared" ref="A75" si="1">A74+1</f>
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>9</v>
@@ -10451,7 +10456,7 @@
       <c r="F75" s="8"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -10474,21 +10479,21 @@
       <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="62" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.5546875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="30.44140625" style="24" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="40.33203125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="62.6640625" style="24" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="24" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="62.7109375" style="24" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="120" t="s">
         <v>155</v>
       </c>
@@ -10501,7 +10506,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -10530,7 +10535,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -10551,7 +10556,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -10572,7 +10577,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>3</v>
       </c>
@@ -10593,7 +10598,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>4</v>
       </c>
@@ -10614,7 +10619,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>5</v>
       </c>
@@ -10635,7 +10640,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -10656,7 +10661,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -10679,7 +10684,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="28">
         <v>8</v>
       </c>
@@ -10702,7 +10707,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -10723,7 +10728,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>10</v>
       </c>
@@ -10744,7 +10749,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>11</v>
       </c>
@@ -10765,7 +10770,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="28">
         <v>12</v>
       </c>
@@ -10786,7 +10791,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <v>13</v>
       </c>
@@ -10807,7 +10812,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="132" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -10830,7 +10835,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -10874,21 +10879,21 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="44.5546875" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1027" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="120" t="s">
         <v>101</v>
       </c>
@@ -10901,7 +10906,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:1027" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1027" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -10930,7 +10935,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:1027" s="84" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" s="84" customFormat="1" ht="330" x14ac:dyDescent="0.25">
       <c r="A3" s="78">
         <v>1</v>
       </c>
@@ -11971,7 +11976,7 @@
       <c r="AML3" s="83"/>
       <c r="AMM3" s="83"/>
     </row>
-    <row r="4" spans="1:1027" s="84" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1027" s="84" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="78">
         <v>2</v>
       </c>
@@ -13012,7 +13017,7 @@
       <c r="AML4" s="83"/>
       <c r="AMM4" s="83"/>
     </row>
-    <row r="5" spans="1:1027" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -13035,7 +13040,7 @@
       <c r="H5" s="57"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -13056,7 +13061,7 @@
       <c r="H6" s="53"/>
       <c r="I6" s="41"/>
     </row>
-    <row r="7" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -13077,7 +13082,7 @@
       <c r="H7" s="53"/>
       <c r="I7" s="41"/>
     </row>
-    <row r="8" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -13100,7 +13105,7 @@
       <c r="H8" s="53"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -13121,7 +13126,7 @@
       <c r="H9" s="53"/>
       <c r="I9" s="41"/>
     </row>
-    <row r="10" spans="1:1027" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -13142,7 +13147,7 @@
       <c r="H10" s="53"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="85">
         <v>9</v>
       </c>
@@ -14179,7 +14184,7 @@
       <c r="AML11" s="74"/>
       <c r="AMM11" s="74"/>
     </row>
-    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="85">
         <v>10</v>
       </c>
@@ -15216,7 +15221,7 @@
       <c r="AML12" s="74"/>
       <c r="AMM12" s="74"/>
     </row>
-    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1027" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="85">
         <v>11</v>
       </c>
@@ -16253,7 +16258,7 @@
       <c r="AML13" s="74"/>
       <c r="AMM13" s="74"/>
     </row>
-    <row r="14" spans="1:1027" s="75" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1027" s="75" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="85">
         <v>12</v>
       </c>
@@ -17290,7 +17295,7 @@
       <c r="AML14" s="74"/>
       <c r="AMM14" s="74"/>
     </row>
-    <row r="15" spans="1:1027" ht="211.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>1</v>
       </c>
@@ -17311,13 +17316,13 @@
       </c>
       <c r="G15" s="36"/>
       <c r="H15" s="36" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
-    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1027" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>2</v>
       </c>
@@ -17338,13 +17343,13 @@
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
-    <row r="17" spans="1:1027" ht="224.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>3</v>
       </c>
@@ -17365,13 +17370,13 @@
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
-    <row r="18" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>4</v>
       </c>
@@ -17395,10 +17400,10 @@
         <v>345</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
-    <row r="19" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1027" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="78">
         <v>17</v>
       </c>
@@ -18435,7 +18440,7 @@
       <c r="AML19" s="83"/>
       <c r="AMM19" s="83"/>
     </row>
-    <row r="20" spans="1:1027" s="84" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1027" s="84" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="78">
         <v>18</v>
       </c>
@@ -19472,7 +19477,7 @@
       <c r="AML20" s="83"/>
       <c r="AMM20" s="83"/>
     </row>
-    <row r="21" spans="1:1027" s="94" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1027" s="94" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="87"/>
       <c r="B21" s="88" t="s">
         <v>130</v>
@@ -20511,12 +20516,12 @@
       <c r="AML21" s="93"/>
       <c r="AMM21" s="93"/>
     </row>
-    <row r="22" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
       <c r="A22" s="87">
         <v>5</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C22" s="37" t="s">
         <v>9</v>
@@ -20525,70 +20530,70 @@
         <v>131</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F22" s="36" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
-    <row r="23" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="87">
         <v>6</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="36" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
-    <row r="24" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="87">
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F24" s="36"/>
       <c r="G24" s="36"/>
       <c r="H24" s="36" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
-    <row r="25" spans="1:1027" ht="138" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1027" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A25" s="111">
         <v>19</v>
       </c>
@@ -20612,10 +20617,10 @@
         <v>347</v>
       </c>
       <c r="I25" s="112" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
-    <row r="26" spans="1:1027" ht="184.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="87">
         <v>8</v>
       </c>
@@ -20639,10 +20644,10 @@
         <v>348</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="27" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="87"/>
       <c r="B27" s="88" t="s">
         <v>138</v>
@@ -20659,7 +20664,7 @@
       <c r="H27" s="36"/>
       <c r="I27" s="41"/>
     </row>
-    <row r="28" spans="1:1027" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="87"/>
       <c r="B28" s="88" t="s">
         <v>139</v>
@@ -20676,7 +20681,7 @@
       <c r="H28" s="36"/>
       <c r="I28" s="41"/>
     </row>
-    <row r="29" spans="1:1027" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1027" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="87"/>
       <c r="B29" s="88" t="s">
         <v>162</v>
@@ -20697,7 +20702,7 @@
       <c r="H29" s="36"/>
       <c r="I29" s="41"/>
     </row>
-    <row r="30" spans="1:1027" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1027" ht="195" x14ac:dyDescent="0.25">
       <c r="A30" s="87">
         <v>9</v>
       </c>
@@ -20716,13 +20721,13 @@
       <c r="F30" s="88"/>
       <c r="G30" s="36"/>
       <c r="H30" s="36" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I30" s="36" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
-    <row r="31" spans="1:1027" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="87">
         <v>10</v>
       </c>
@@ -20744,10 +20749,10 @@
         <v>354</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
-    <row r="32" spans="1:1027" s="99" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1027" s="99" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="87">
         <v>11</v>
       </c>
@@ -20769,7 +20774,7 @@
         <v>357</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J32" s="98"/>
       <c r="K32" s="98"/>
@@ -21807,20 +21812,20 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="29.5546875" style="3" customWidth="1"/>
-    <col min="10" max="1027" width="9.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="29.5703125" style="3" customWidth="1"/>
+    <col min="10" max="1027" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="120" t="s">
         <v>140</v>
       </c>
@@ -21833,7 +21838,7 @@
       <c r="H1" s="120"/>
       <c r="I1" s="120"/>
     </row>
-    <row r="2" spans="1:9" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -21862,7 +21867,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -21879,7 +21884,7 @@
       <c r="H3" s="41"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -21896,7 +21901,7 @@
       <c r="H4" s="41"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -21913,7 +21918,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -21930,7 +21935,7 @@
       <c r="H6" s="41"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -21947,7 +21952,7 @@
       <c r="H7" s="41"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -21964,7 +21969,7 @@
       <c r="H8" s="41"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -21981,7 +21986,7 @@
       <c r="H9" s="41"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -22007,27 +22012,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK52"/>
+  <dimension ref="A1:AMK53"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.33203125" style="3" customWidth="1"/>
-    <col min="10" max="1025" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="84.28515625" style="3" customWidth="1"/>
+    <col min="10" max="1025" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="121" t="s">
         <v>194</v>
       </c>
@@ -22040,7 +22045,7 @@
       <c r="H1" s="122"/>
       <c r="I1" s="122"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -22069,7 +22074,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -22111,7 +22116,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f>A3+1</f>
         <v>2</v>
@@ -22154,7 +22159,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" ref="A5:A41" si="0">A4+1</f>
         <v>3</v>
@@ -22197,7 +22202,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" s="9" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -22238,7 +22243,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f>A9+1</f>
         <v>7</v>
@@ -22281,7 +22286,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <f>A6+1</f>
         <v>5</v>
@@ -22322,7 +22327,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -22363,7 +22368,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -22389,7 +22394,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f>A7+1</f>
         <v>8</v>
@@ -22432,7 +22437,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -22475,7 +22480,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="9" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f>A12+1</f>
         <v>10</v>
@@ -22516,7 +22521,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" s="9" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" s="9" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f>A13+1</f>
         <v>11</v>
@@ -22539,7 +22544,7 @@
         <v>339</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -22559,7 +22564,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <f t="shared" ref="A15:A22" si="1">A14+1</f>
         <v>12</v>
@@ -22600,7 +22605,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -22641,7 +22646,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:1025" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1025" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -22682,7 +22687,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="71">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -23718,7 +23723,7 @@
       <c r="AMJ18" s="74"/>
       <c r="AMK18" s="74"/>
     </row>
-    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="71">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -24754,7 +24759,7 @@
       <c r="AMJ19" s="74"/>
       <c r="AMK19" s="74"/>
     </row>
-    <row r="20" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -24780,7 +24785,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="21" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -24806,7 +24811,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="22" spans="1:1025" s="75" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1025" s="75" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="71">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -25844,7 +25849,7 @@
       <c r="AMJ22" s="74"/>
       <c r="AMK22" s="74"/>
     </row>
-    <row r="23" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -25870,7 +25875,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="24" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -25894,7 +25899,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="25" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -25918,7 +25923,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="26" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -25942,7 +25947,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="27" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -25966,7 +25971,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -25990,7 +25995,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="29" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -26014,7 +26019,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="30" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -26038,7 +26043,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="31" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -26062,7 +26067,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="32" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -26086,7 +26091,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -26110,7 +26115,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1025" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -27144,7 +27149,7 @@
       <c r="AMJ34" s="74"/>
       <c r="AMK34" s="74"/>
     </row>
-    <row r="35" spans="1:1025" ht="184.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1025" ht="210" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -27165,10 +27170,10 @@
         <v>293</v>
       </c>
       <c r="I35" s="36" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="132" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1025" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -27189,10 +27194,10 @@
         <v>294</v>
       </c>
       <c r="I36" s="36" t="s">
-        <v>598</v>
+        <v>645</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1025" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -27213,10 +27218,10 @@
         <v>295</v>
       </c>
       <c r="I37" s="36" t="s">
-        <v>523</v>
+        <v>646</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -27240,7 +27245,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -27262,7 +27267,7 @@
       </c>
       <c r="I39" s="41"/>
     </row>
-    <row r="40" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -27286,7 +27291,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1025" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -27310,7 +27315,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="66" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>39</v>
       </c>
@@ -27330,10 +27335,10 @@
         <v>376</v>
       </c>
       <c r="I42" s="36" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1025" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>40</v>
       </c>
@@ -27353,10 +27358,10 @@
         <v>375</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>41</v>
       </c>
@@ -27379,7 +27384,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="45" spans="1:1025" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>42</v>
       </c>
@@ -27399,10 +27404,10 @@
         <v>378</v>
       </c>
       <c r="I45" s="36" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>43</v>
       </c>
@@ -27425,7 +27430,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1025" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>44</v>
       </c>
@@ -27445,10 +27450,10 @@
         <v>515</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
-    <row r="48" spans="1:1025" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>45</v>
       </c>
@@ -27465,11 +27470,11 @@
       <c r="F48" s="41"/>
       <c r="G48" s="41"/>
       <c r="H48" s="104" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I48" s="36"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>46</v>
       </c>
@@ -27486,11 +27491,11 @@
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
       <c r="H49" s="104" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I49" s="36"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>47</v>
       </c>
@@ -27507,16 +27512,16 @@
       <c r="F50" s="41"/>
       <c r="G50" s="41"/>
       <c r="H50" s="104" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I50" s="36"/>
     </row>
-    <row r="51" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>48</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C51" s="41" t="s">
         <v>9</v>
@@ -27531,10 +27536,10 @@
         <v>404</v>
       </c>
       <c r="I51" s="36" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>49</v>
       </c>
@@ -27551,10 +27556,33 @@
       <c r="F52" s="41"/>
       <c r="G52" s="41"/>
       <c r="H52" s="104" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I52" s="36" t="s">
-        <v>599</v>
+        <v>597</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>50</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>642</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>643</v>
+      </c>
+      <c r="E53" s="41" t="s">
+        <v>644</v>
+      </c>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="104"/>
+      <c r="I53" s="36" t="s">
+        <v>647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated a config for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4ECD28D1-711A-428F-A2F5-5EC4071A0C1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A95C3CD-86F5-4BEF-80CC-017796BF2410}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8535" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8535" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="653">
   <si>
     <r>
       <rPr>
@@ -2984,42 +2984,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Masked UIN is one of the id field to be returned for an eKYC partner. The no of digits of the masked UIN will be configurable
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Bookman Old Style"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">On change: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Bookman Old Style"/>
-        <family val="1"/>
-      </rPr>
-      <t>The no of digits of the masked UIN will be as per the updated config</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Bookman Old Style"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-In general this is an one-time setup activity. However the country might decide to change the config as per the scenario and the business need in the country</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">This configuration will contain the List of Langauge codes corresponding to Languages that MOSIP will support for a particular Country.
 Kernel: While adding an additional Language Code for a country, Master data also needs to be stored for that language, else Master data services would respond with no data
 IDA: During demo authentication, the language in the authentication input is validated against the configuration list
@@ -3277,6 +3241,74 @@
   <si>
     <t>IDA: The language "primary" or "both" in which the notification/eKYC response has to be triggered is set by this configuration</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Masked UIN is one of the id field to be returned for an eKYC partner. The no of digits of the masked UIN will be configurable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">On change: </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>The no of digits of the masked UIN will be as per the updated config
+In general this is an one-time setup activity. However the country might decide to change the config as per the scenario and the business need in the country</t>
+    </r>
+  </si>
+  <si>
+    <t>Configure the idtype to be supported for Authentication/KYC/OTP Request</t>
+  </si>
+  <si>
+    <t>To be added</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The authentication,eKYC and OTP requests will be supported for the id Types configured.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+On change:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> The authentication,eKYC and OTP requests will be supported for the id Type Changed
+In general this is an one-time setup activity. However the country might decide to change the config as per the scenario and the business need in the country</t>
+    </r>
+  </si>
+  <si>
+    <t>UIN and VID</t>
+  </si>
+  <si>
+    <t>UIN/VID</t>
+  </si>
 </sst>
 </file>
 
@@ -3285,7 +3317,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3470,6 +3502,20 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3666,7 +3712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3947,12 +3993,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4025,6 +4065,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5350,17 +5423,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -5938,17 +6011,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -5975,7 +6048,7 @@
       <c r="H2" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="116" t="s">
+      <c r="I2" s="114" t="s">
         <v>233</v>
       </c>
     </row>
@@ -6000,7 +6073,7 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>285</v>
@@ -6025,7 +6098,7 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>585</v>
@@ -6036,7 +6109,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>9</v>
@@ -6079,7 +6152,7 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>361</v>
@@ -6106,7 +6179,7 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>362</v>
@@ -6132,8 +6205,8 @@
         <v>11</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="101" t="s">
-        <v>618</v>
+      <c r="H8" s="99" t="s">
+        <v>617</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>363</v>
@@ -6144,26 +6217,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6176,7 +6249,7 @@
       <c r="C10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="117">
+      <c r="D10" s="115">
         <v>0</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -6186,7 +6259,7 @@
         <v>275</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="115" t="s">
+      <c r="H10" s="113" t="s">
         <v>383</v>
       </c>
       <c r="I10" s="19" t="s">
@@ -6203,7 +6276,7 @@
       <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="117">
+      <c r="D11" s="115">
         <v>0</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -6213,7 +6286,7 @@
         <v>275</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="115" t="s">
+      <c r="H11" s="113" t="s">
         <v>382</v>
       </c>
       <c r="I11" s="19" t="s">
@@ -6230,7 +6303,7 @@
       <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="117">
+      <c r="D12" s="115">
         <v>0</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -6240,8 +6313,8 @@
         <v>275</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="115" t="s">
-        <v>619</v>
+      <c r="H12" s="113" t="s">
+        <v>618</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>364</v>
@@ -6264,7 +6337,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
@@ -6304,13 +6377,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>32</v>
@@ -6318,7 +6391,7 @@
       <c r="F15" s="50"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I15" s="19"/>
     </row>
@@ -6343,7 +6416,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -6633,22 +6706,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="108" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="25" t="s">
@@ -6746,7 +6819,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7054,7 +7127,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7066,7 +7139,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
@@ -7209,7 +7282,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7227,7 +7300,7 @@
       <c r="F25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="100" t="s">
+      <c r="G25" s="98" t="s">
         <v>435</v>
       </c>
       <c r="H25" s="7" t="s">
@@ -9734,7 +9807,7 @@
       <c r="AMK43" s="15"/>
       <c r="AML43" s="15"/>
     </row>
-    <row r="44" spans="1:1026" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1026" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -10018,13 +10091,13 @@
         <v>578</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C56" s="37" t="s">
         <v>9</v>
@@ -10036,7 +10109,7 @@
         <v>461</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="375" x14ac:dyDescent="0.25">
@@ -10051,7 +10124,7 @@
         <v>9</v>
       </c>
       <c r="D57" s="36" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E57" s="41"/>
       <c r="F57" s="49"/>
@@ -10278,7 +10351,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -10405,13 +10478,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C73" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E73" s="36" t="s">
         <v>590</v>
@@ -10419,7 +10492,7 @@
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -10427,7 +10500,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>9</v>
@@ -10437,7 +10510,7 @@
       <c r="F74" s="8"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -10446,7 +10519,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>9</v>
@@ -10456,7 +10529,7 @@
       <c r="F75" s="8"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -10494,17 +10567,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="118" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -10677,10 +10750,10 @@
       <c r="E9" s="28"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
-      <c r="H9" s="102" t="s">
+      <c r="H9" s="100" t="s">
         <v>232</v>
       </c>
-      <c r="I9" s="103" t="s">
+      <c r="I9" s="101" t="s">
         <v>398</v>
       </c>
     </row>
@@ -10700,10 +10773,10 @@
       <c r="E10" s="28"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="102" t="s">
+      <c r="H10" s="100" t="s">
         <v>401</v>
       </c>
-      <c r="I10" s="103" t="s">
+      <c r="I10" s="101" t="s">
         <v>402</v>
       </c>
     </row>
@@ -10870,13 +10943,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMM32"/>
+  <dimension ref="A1:AMM33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10894,17 +10967,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1027" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
     </row>
     <row r="2" spans="1:1027" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -10935,7 +11008,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:1027" s="84" customFormat="1" ht="330" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" s="84" customFormat="1" ht="315" x14ac:dyDescent="0.25">
       <c r="A3" s="78">
         <v>1</v>
       </c>
@@ -17295,7 +17368,7 @@
       <c r="AML14" s="74"/>
       <c r="AMM14" s="74"/>
     </row>
-    <row r="15" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1027" ht="240" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>1</v>
       </c>
@@ -17316,7 +17389,7 @@
       </c>
       <c r="G15" s="36"/>
       <c r="H15" s="36" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I15" s="36" t="s">
         <v>586</v>
@@ -17343,7 +17416,7 @@
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I16" s="36" t="s">
         <v>587</v>
@@ -17370,7 +17443,7 @@
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I17" s="36" t="s">
         <v>588</v>
@@ -20521,7 +20594,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C22" s="37" t="s">
         <v>9</v>
@@ -20537,7 +20610,7 @@
       </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I22" s="36" t="s">
         <v>591</v>
@@ -20548,24 +20621,24 @@
         <v>6</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="39" t="s">
+        <v>600</v>
+      </c>
+      <c r="E23" s="38" t="s">
         <v>601</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>602</v>
       </c>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="36" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="24" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
@@ -20573,51 +20646,51 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="39" t="s">
+        <v>604</v>
+      </c>
+      <c r="E24" s="38" t="s">
         <v>605</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>606</v>
       </c>
       <c r="F24" s="36"/>
       <c r="G24" s="36"/>
       <c r="H24" s="36" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="25" spans="1:1027" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="111">
+      <c r="A25" s="109">
         <v>19</v>
       </c>
-      <c r="B25" s="112" t="s">
+      <c r="B25" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="113" t="s">
+      <c r="C25" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="114" t="s">
+      <c r="D25" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="E25" s="114" t="s">
+      <c r="E25" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="112" t="s">
+      <c r="F25" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="112"/>
-      <c r="H25" s="112" t="s">
+      <c r="G25" s="110"/>
+      <c r="H25" s="110" t="s">
         <v>347</v>
       </c>
-      <c r="I25" s="112" t="s">
-        <v>608</v>
+      <c r="I25" s="110" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="26" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
@@ -20721,7 +20794,7 @@
       <c r="F30" s="88"/>
       <c r="G30" s="36"/>
       <c r="H30" s="36" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I30" s="36" t="s">
         <v>593</v>
@@ -20752,1048 +20825,1073 @@
         <v>594</v>
       </c>
     </row>
-    <row r="32" spans="1:1027" s="99" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="87">
+    <row r="32" spans="1:1027" s="97" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="85">
         <v>11</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="73" t="s">
         <v>355</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="96" t="s">
+      <c r="D32" s="122" t="s">
         <v>356</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97" t="s">
+      <c r="F32" s="72"/>
+      <c r="G32" s="124"/>
+      <c r="H32" s="124" t="s">
         <v>357</v>
       </c>
-      <c r="I32" s="36" t="s">
-        <v>595</v>
-      </c>
-      <c r="J32" s="98"/>
-      <c r="K32" s="98"/>
-      <c r="L32" s="98"/>
-      <c r="M32" s="98"/>
-      <c r="N32" s="98"/>
-      <c r="O32" s="98"/>
-      <c r="P32" s="98"/>
-      <c r="Q32" s="98"/>
-      <c r="R32" s="98"/>
-      <c r="S32" s="98"/>
-      <c r="T32" s="98"/>
-      <c r="U32" s="98"/>
-      <c r="V32" s="98"/>
-      <c r="W32" s="98"/>
-      <c r="X32" s="98"/>
-      <c r="Y32" s="98"/>
-      <c r="Z32" s="98"/>
-      <c r="AA32" s="98"/>
-      <c r="AB32" s="98"/>
-      <c r="AC32" s="98"/>
-      <c r="AD32" s="98"/>
-      <c r="AE32" s="98"/>
-      <c r="AF32" s="98"/>
-      <c r="AG32" s="98"/>
-      <c r="AH32" s="98"/>
-      <c r="AI32" s="98"/>
-      <c r="AJ32" s="98"/>
-      <c r="AK32" s="98"/>
-      <c r="AL32" s="98"/>
-      <c r="AM32" s="98"/>
-      <c r="AN32" s="98"/>
-      <c r="AO32" s="98"/>
-      <c r="AP32" s="98"/>
-      <c r="AQ32" s="98"/>
-      <c r="AR32" s="98"/>
-      <c r="AS32" s="98"/>
-      <c r="AT32" s="98"/>
-      <c r="AU32" s="98"/>
-      <c r="AV32" s="98"/>
-      <c r="AW32" s="98"/>
-      <c r="AX32" s="98"/>
-      <c r="AY32" s="98"/>
-      <c r="AZ32" s="98"/>
-      <c r="BA32" s="98"/>
-      <c r="BB32" s="98"/>
-      <c r="BC32" s="98"/>
-      <c r="BD32" s="98"/>
-      <c r="BE32" s="98"/>
-      <c r="BF32" s="98"/>
-      <c r="BG32" s="98"/>
-      <c r="BH32" s="98"/>
-      <c r="BI32" s="98"/>
-      <c r="BJ32" s="98"/>
-      <c r="BK32" s="98"/>
-      <c r="BL32" s="98"/>
-      <c r="BM32" s="98"/>
-      <c r="BN32" s="98"/>
-      <c r="BO32" s="98"/>
-      <c r="BP32" s="98"/>
-      <c r="BQ32" s="98"/>
-      <c r="BR32" s="98"/>
-      <c r="BS32" s="98"/>
-      <c r="BT32" s="98"/>
-      <c r="BU32" s="98"/>
-      <c r="BV32" s="98"/>
-      <c r="BW32" s="98"/>
-      <c r="BX32" s="98"/>
-      <c r="BY32" s="98"/>
-      <c r="BZ32" s="98"/>
-      <c r="CA32" s="98"/>
-      <c r="CB32" s="98"/>
-      <c r="CC32" s="98"/>
-      <c r="CD32" s="98"/>
-      <c r="CE32" s="98"/>
-      <c r="CF32" s="98"/>
-      <c r="CG32" s="98"/>
-      <c r="CH32" s="98"/>
-      <c r="CI32" s="98"/>
-      <c r="CJ32" s="98"/>
-      <c r="CK32" s="98"/>
-      <c r="CL32" s="98"/>
-      <c r="CM32" s="98"/>
-      <c r="CN32" s="98"/>
-      <c r="CO32" s="98"/>
-      <c r="CP32" s="98"/>
-      <c r="CQ32" s="98"/>
-      <c r="CR32" s="98"/>
-      <c r="CS32" s="98"/>
-      <c r="CT32" s="98"/>
-      <c r="CU32" s="98"/>
-      <c r="CV32" s="98"/>
-      <c r="CW32" s="98"/>
-      <c r="CX32" s="98"/>
-      <c r="CY32" s="98"/>
-      <c r="CZ32" s="98"/>
-      <c r="DA32" s="98"/>
-      <c r="DB32" s="98"/>
-      <c r="DC32" s="98"/>
-      <c r="DD32" s="98"/>
-      <c r="DE32" s="98"/>
-      <c r="DF32" s="98"/>
-      <c r="DG32" s="98"/>
-      <c r="DH32" s="98"/>
-      <c r="DI32" s="98"/>
-      <c r="DJ32" s="98"/>
-      <c r="DK32" s="98"/>
-      <c r="DL32" s="98"/>
-      <c r="DM32" s="98"/>
-      <c r="DN32" s="98"/>
-      <c r="DO32" s="98"/>
-      <c r="DP32" s="98"/>
-      <c r="DQ32" s="98"/>
-      <c r="DR32" s="98"/>
-      <c r="DS32" s="98"/>
-      <c r="DT32" s="98"/>
-      <c r="DU32" s="98"/>
-      <c r="DV32" s="98"/>
-      <c r="DW32" s="98"/>
-      <c r="DX32" s="98"/>
-      <c r="DY32" s="98"/>
-      <c r="DZ32" s="98"/>
-      <c r="EA32" s="98"/>
-      <c r="EB32" s="98"/>
-      <c r="EC32" s="98"/>
-      <c r="ED32" s="98"/>
-      <c r="EE32" s="98"/>
-      <c r="EF32" s="98"/>
-      <c r="EG32" s="98"/>
-      <c r="EH32" s="98"/>
-      <c r="EI32" s="98"/>
-      <c r="EJ32" s="98"/>
-      <c r="EK32" s="98"/>
-      <c r="EL32" s="98"/>
-      <c r="EM32" s="98"/>
-      <c r="EN32" s="98"/>
-      <c r="EO32" s="98"/>
-      <c r="EP32" s="98"/>
-      <c r="EQ32" s="98"/>
-      <c r="ER32" s="98"/>
-      <c r="ES32" s="98"/>
-      <c r="ET32" s="98"/>
-      <c r="EU32" s="98"/>
-      <c r="EV32" s="98"/>
-      <c r="EW32" s="98"/>
-      <c r="EX32" s="98"/>
-      <c r="EY32" s="98"/>
-      <c r="EZ32" s="98"/>
-      <c r="FA32" s="98"/>
-      <c r="FB32" s="98"/>
-      <c r="FC32" s="98"/>
-      <c r="FD32" s="98"/>
-      <c r="FE32" s="98"/>
-      <c r="FF32" s="98"/>
-      <c r="FG32" s="98"/>
-      <c r="FH32" s="98"/>
-      <c r="FI32" s="98"/>
-      <c r="FJ32" s="98"/>
-      <c r="FK32" s="98"/>
-      <c r="FL32" s="98"/>
-      <c r="FM32" s="98"/>
-      <c r="FN32" s="98"/>
-      <c r="FO32" s="98"/>
-      <c r="FP32" s="98"/>
-      <c r="FQ32" s="98"/>
-      <c r="FR32" s="98"/>
-      <c r="FS32" s="98"/>
-      <c r="FT32" s="98"/>
-      <c r="FU32" s="98"/>
-      <c r="FV32" s="98"/>
-      <c r="FW32" s="98"/>
-      <c r="FX32" s="98"/>
-      <c r="FY32" s="98"/>
-      <c r="FZ32" s="98"/>
-      <c r="GA32" s="98"/>
-      <c r="GB32" s="98"/>
-      <c r="GC32" s="98"/>
-      <c r="GD32" s="98"/>
-      <c r="GE32" s="98"/>
-      <c r="GF32" s="98"/>
-      <c r="GG32" s="98"/>
-      <c r="GH32" s="98"/>
-      <c r="GI32" s="98"/>
-      <c r="GJ32" s="98"/>
-      <c r="GK32" s="98"/>
-      <c r="GL32" s="98"/>
-      <c r="GM32" s="98"/>
-      <c r="GN32" s="98"/>
-      <c r="GO32" s="98"/>
-      <c r="GP32" s="98"/>
-      <c r="GQ32" s="98"/>
-      <c r="GR32" s="98"/>
-      <c r="GS32" s="98"/>
-      <c r="GT32" s="98"/>
-      <c r="GU32" s="98"/>
-      <c r="GV32" s="98"/>
-      <c r="GW32" s="98"/>
-      <c r="GX32" s="98"/>
-      <c r="GY32" s="98"/>
-      <c r="GZ32" s="98"/>
-      <c r="HA32" s="98"/>
-      <c r="HB32" s="98"/>
-      <c r="HC32" s="98"/>
-      <c r="HD32" s="98"/>
-      <c r="HE32" s="98"/>
-      <c r="HF32" s="98"/>
-      <c r="HG32" s="98"/>
-      <c r="HH32" s="98"/>
-      <c r="HI32" s="98"/>
-      <c r="HJ32" s="98"/>
-      <c r="HK32" s="98"/>
-      <c r="HL32" s="98"/>
-      <c r="HM32" s="98"/>
-      <c r="HN32" s="98"/>
-      <c r="HO32" s="98"/>
-      <c r="HP32" s="98"/>
-      <c r="HQ32" s="98"/>
-      <c r="HR32" s="98"/>
-      <c r="HS32" s="98"/>
-      <c r="HT32" s="98"/>
-      <c r="HU32" s="98"/>
-      <c r="HV32" s="98"/>
-      <c r="HW32" s="98"/>
-      <c r="HX32" s="98"/>
-      <c r="HY32" s="98"/>
-      <c r="HZ32" s="98"/>
-      <c r="IA32" s="98"/>
-      <c r="IB32" s="98"/>
-      <c r="IC32" s="98"/>
-      <c r="ID32" s="98"/>
-      <c r="IE32" s="98"/>
-      <c r="IF32" s="98"/>
-      <c r="IG32" s="98"/>
-      <c r="IH32" s="98"/>
-      <c r="II32" s="98"/>
-      <c r="IJ32" s="98"/>
-      <c r="IK32" s="98"/>
-      <c r="IL32" s="98"/>
-      <c r="IM32" s="98"/>
-      <c r="IN32" s="98"/>
-      <c r="IO32" s="98"/>
-      <c r="IP32" s="98"/>
-      <c r="IQ32" s="98"/>
-      <c r="IR32" s="98"/>
-      <c r="IS32" s="98"/>
-      <c r="IT32" s="98"/>
-      <c r="IU32" s="98"/>
-      <c r="IV32" s="98"/>
-      <c r="IW32" s="98"/>
-      <c r="IX32" s="98"/>
-      <c r="IY32" s="98"/>
-      <c r="IZ32" s="98"/>
-      <c r="JA32" s="98"/>
-      <c r="JB32" s="98"/>
-      <c r="JC32" s="98"/>
-      <c r="JD32" s="98"/>
-      <c r="JE32" s="98"/>
-      <c r="JF32" s="98"/>
-      <c r="JG32" s="98"/>
-      <c r="JH32" s="98"/>
-      <c r="JI32" s="98"/>
-      <c r="JJ32" s="98"/>
-      <c r="JK32" s="98"/>
-      <c r="JL32" s="98"/>
-      <c r="JM32" s="98"/>
-      <c r="JN32" s="98"/>
-      <c r="JO32" s="98"/>
-      <c r="JP32" s="98"/>
-      <c r="JQ32" s="98"/>
-      <c r="JR32" s="98"/>
-      <c r="JS32" s="98"/>
-      <c r="JT32" s="98"/>
-      <c r="JU32" s="98"/>
-      <c r="JV32" s="98"/>
-      <c r="JW32" s="98"/>
-      <c r="JX32" s="98"/>
-      <c r="JY32" s="98"/>
-      <c r="JZ32" s="98"/>
-      <c r="KA32" s="98"/>
-      <c r="KB32" s="98"/>
-      <c r="KC32" s="98"/>
-      <c r="KD32" s="98"/>
-      <c r="KE32" s="98"/>
-      <c r="KF32" s="98"/>
-      <c r="KG32" s="98"/>
-      <c r="KH32" s="98"/>
-      <c r="KI32" s="98"/>
-      <c r="KJ32" s="98"/>
-      <c r="KK32" s="98"/>
-      <c r="KL32" s="98"/>
-      <c r="KM32" s="98"/>
-      <c r="KN32" s="98"/>
-      <c r="KO32" s="98"/>
-      <c r="KP32" s="98"/>
-      <c r="KQ32" s="98"/>
-      <c r="KR32" s="98"/>
-      <c r="KS32" s="98"/>
-      <c r="KT32" s="98"/>
-      <c r="KU32" s="98"/>
-      <c r="KV32" s="98"/>
-      <c r="KW32" s="98"/>
-      <c r="KX32" s="98"/>
-      <c r="KY32" s="98"/>
-      <c r="KZ32" s="98"/>
-      <c r="LA32" s="98"/>
-      <c r="LB32" s="98"/>
-      <c r="LC32" s="98"/>
-      <c r="LD32" s="98"/>
-      <c r="LE32" s="98"/>
-      <c r="LF32" s="98"/>
-      <c r="LG32" s="98"/>
-      <c r="LH32" s="98"/>
-      <c r="LI32" s="98"/>
-      <c r="LJ32" s="98"/>
-      <c r="LK32" s="98"/>
-      <c r="LL32" s="98"/>
-      <c r="LM32" s="98"/>
-      <c r="LN32" s="98"/>
-      <c r="LO32" s="98"/>
-      <c r="LP32" s="98"/>
-      <c r="LQ32" s="98"/>
-      <c r="LR32" s="98"/>
-      <c r="LS32" s="98"/>
-      <c r="LT32" s="98"/>
-      <c r="LU32" s="98"/>
-      <c r="LV32" s="98"/>
-      <c r="LW32" s="98"/>
-      <c r="LX32" s="98"/>
-      <c r="LY32" s="98"/>
-      <c r="LZ32" s="98"/>
-      <c r="MA32" s="98"/>
-      <c r="MB32" s="98"/>
-      <c r="MC32" s="98"/>
-      <c r="MD32" s="98"/>
-      <c r="ME32" s="98"/>
-      <c r="MF32" s="98"/>
-      <c r="MG32" s="98"/>
-      <c r="MH32" s="98"/>
-      <c r="MI32" s="98"/>
-      <c r="MJ32" s="98"/>
-      <c r="MK32" s="98"/>
-      <c r="ML32" s="98"/>
-      <c r="MM32" s="98"/>
-      <c r="MN32" s="98"/>
-      <c r="MO32" s="98"/>
-      <c r="MP32" s="98"/>
-      <c r="MQ32" s="98"/>
-      <c r="MR32" s="98"/>
-      <c r="MS32" s="98"/>
-      <c r="MT32" s="98"/>
-      <c r="MU32" s="98"/>
-      <c r="MV32" s="98"/>
-      <c r="MW32" s="98"/>
-      <c r="MX32" s="98"/>
-      <c r="MY32" s="98"/>
-      <c r="MZ32" s="98"/>
-      <c r="NA32" s="98"/>
-      <c r="NB32" s="98"/>
-      <c r="NC32" s="98"/>
-      <c r="ND32" s="98"/>
-      <c r="NE32" s="98"/>
-      <c r="NF32" s="98"/>
-      <c r="NG32" s="98"/>
-      <c r="NH32" s="98"/>
-      <c r="NI32" s="98"/>
-      <c r="NJ32" s="98"/>
-      <c r="NK32" s="98"/>
-      <c r="NL32" s="98"/>
-      <c r="NM32" s="98"/>
-      <c r="NN32" s="98"/>
-      <c r="NO32" s="98"/>
-      <c r="NP32" s="98"/>
-      <c r="NQ32" s="98"/>
-      <c r="NR32" s="98"/>
-      <c r="NS32" s="98"/>
-      <c r="NT32" s="98"/>
-      <c r="NU32" s="98"/>
-      <c r="NV32" s="98"/>
-      <c r="NW32" s="98"/>
-      <c r="NX32" s="98"/>
-      <c r="NY32" s="98"/>
-      <c r="NZ32" s="98"/>
-      <c r="OA32" s="98"/>
-      <c r="OB32" s="98"/>
-      <c r="OC32" s="98"/>
-      <c r="OD32" s="98"/>
-      <c r="OE32" s="98"/>
-      <c r="OF32" s="98"/>
-      <c r="OG32" s="98"/>
-      <c r="OH32" s="98"/>
-      <c r="OI32" s="98"/>
-      <c r="OJ32" s="98"/>
-      <c r="OK32" s="98"/>
-      <c r="OL32" s="98"/>
-      <c r="OM32" s="98"/>
-      <c r="ON32" s="98"/>
-      <c r="OO32" s="98"/>
-      <c r="OP32" s="98"/>
-      <c r="OQ32" s="98"/>
-      <c r="OR32" s="98"/>
-      <c r="OS32" s="98"/>
-      <c r="OT32" s="98"/>
-      <c r="OU32" s="98"/>
-      <c r="OV32" s="98"/>
-      <c r="OW32" s="98"/>
-      <c r="OX32" s="98"/>
-      <c r="OY32" s="98"/>
-      <c r="OZ32" s="98"/>
-      <c r="PA32" s="98"/>
-      <c r="PB32" s="98"/>
-      <c r="PC32" s="98"/>
-      <c r="PD32" s="98"/>
-      <c r="PE32" s="98"/>
-      <c r="PF32" s="98"/>
-      <c r="PG32" s="98"/>
-      <c r="PH32" s="98"/>
-      <c r="PI32" s="98"/>
-      <c r="PJ32" s="98"/>
-      <c r="PK32" s="98"/>
-      <c r="PL32" s="98"/>
-      <c r="PM32" s="98"/>
-      <c r="PN32" s="98"/>
-      <c r="PO32" s="98"/>
-      <c r="PP32" s="98"/>
-      <c r="PQ32" s="98"/>
-      <c r="PR32" s="98"/>
-      <c r="PS32" s="98"/>
-      <c r="PT32" s="98"/>
-      <c r="PU32" s="98"/>
-      <c r="PV32" s="98"/>
-      <c r="PW32" s="98"/>
-      <c r="PX32" s="98"/>
-      <c r="PY32" s="98"/>
-      <c r="PZ32" s="98"/>
-      <c r="QA32" s="98"/>
-      <c r="QB32" s="98"/>
-      <c r="QC32" s="98"/>
-      <c r="QD32" s="98"/>
-      <c r="QE32" s="98"/>
-      <c r="QF32" s="98"/>
-      <c r="QG32" s="98"/>
-      <c r="QH32" s="98"/>
-      <c r="QI32" s="98"/>
-      <c r="QJ32" s="98"/>
-      <c r="QK32" s="98"/>
-      <c r="QL32" s="98"/>
-      <c r="QM32" s="98"/>
-      <c r="QN32" s="98"/>
-      <c r="QO32" s="98"/>
-      <c r="QP32" s="98"/>
-      <c r="QQ32" s="98"/>
-      <c r="QR32" s="98"/>
-      <c r="QS32" s="98"/>
-      <c r="QT32" s="98"/>
-      <c r="QU32" s="98"/>
-      <c r="QV32" s="98"/>
-      <c r="QW32" s="98"/>
-      <c r="QX32" s="98"/>
-      <c r="QY32" s="98"/>
-      <c r="QZ32" s="98"/>
-      <c r="RA32" s="98"/>
-      <c r="RB32" s="98"/>
-      <c r="RC32" s="98"/>
-      <c r="RD32" s="98"/>
-      <c r="RE32" s="98"/>
-      <c r="RF32" s="98"/>
-      <c r="RG32" s="98"/>
-      <c r="RH32" s="98"/>
-      <c r="RI32" s="98"/>
-      <c r="RJ32" s="98"/>
-      <c r="RK32" s="98"/>
-      <c r="RL32" s="98"/>
-      <c r="RM32" s="98"/>
-      <c r="RN32" s="98"/>
-      <c r="RO32" s="98"/>
-      <c r="RP32" s="98"/>
-      <c r="RQ32" s="98"/>
-      <c r="RR32" s="98"/>
-      <c r="RS32" s="98"/>
-      <c r="RT32" s="98"/>
-      <c r="RU32" s="98"/>
-      <c r="RV32" s="98"/>
-      <c r="RW32" s="98"/>
-      <c r="RX32" s="98"/>
-      <c r="RY32" s="98"/>
-      <c r="RZ32" s="98"/>
-      <c r="SA32" s="98"/>
-      <c r="SB32" s="98"/>
-      <c r="SC32" s="98"/>
-      <c r="SD32" s="98"/>
-      <c r="SE32" s="98"/>
-      <c r="SF32" s="98"/>
-      <c r="SG32" s="98"/>
-      <c r="SH32" s="98"/>
-      <c r="SI32" s="98"/>
-      <c r="SJ32" s="98"/>
-      <c r="SK32" s="98"/>
-      <c r="SL32" s="98"/>
-      <c r="SM32" s="98"/>
-      <c r="SN32" s="98"/>
-      <c r="SO32" s="98"/>
-      <c r="SP32" s="98"/>
-      <c r="SQ32" s="98"/>
-      <c r="SR32" s="98"/>
-      <c r="SS32" s="98"/>
-      <c r="ST32" s="98"/>
-      <c r="SU32" s="98"/>
-      <c r="SV32" s="98"/>
-      <c r="SW32" s="98"/>
-      <c r="SX32" s="98"/>
-      <c r="SY32" s="98"/>
-      <c r="SZ32" s="98"/>
-      <c r="TA32" s="98"/>
-      <c r="TB32" s="98"/>
-      <c r="TC32" s="98"/>
-      <c r="TD32" s="98"/>
-      <c r="TE32" s="98"/>
-      <c r="TF32" s="98"/>
-      <c r="TG32" s="98"/>
-      <c r="TH32" s="98"/>
-      <c r="TI32" s="98"/>
-      <c r="TJ32" s="98"/>
-      <c r="TK32" s="98"/>
-      <c r="TL32" s="98"/>
-      <c r="TM32" s="98"/>
-      <c r="TN32" s="98"/>
-      <c r="TO32" s="98"/>
-      <c r="TP32" s="98"/>
-      <c r="TQ32" s="98"/>
-      <c r="TR32" s="98"/>
-      <c r="TS32" s="98"/>
-      <c r="TT32" s="98"/>
-      <c r="TU32" s="98"/>
-      <c r="TV32" s="98"/>
-      <c r="TW32" s="98"/>
-      <c r="TX32" s="98"/>
-      <c r="TY32" s="98"/>
-      <c r="TZ32" s="98"/>
-      <c r="UA32" s="98"/>
-      <c r="UB32" s="98"/>
-      <c r="UC32" s="98"/>
-      <c r="UD32" s="98"/>
-      <c r="UE32" s="98"/>
-      <c r="UF32" s="98"/>
-      <c r="UG32" s="98"/>
-      <c r="UH32" s="98"/>
-      <c r="UI32" s="98"/>
-      <c r="UJ32" s="98"/>
-      <c r="UK32" s="98"/>
-      <c r="UL32" s="98"/>
-      <c r="UM32" s="98"/>
-      <c r="UN32" s="98"/>
-      <c r="UO32" s="98"/>
-      <c r="UP32" s="98"/>
-      <c r="UQ32" s="98"/>
-      <c r="UR32" s="98"/>
-      <c r="US32" s="98"/>
-      <c r="UT32" s="98"/>
-      <c r="UU32" s="98"/>
-      <c r="UV32" s="98"/>
-      <c r="UW32" s="98"/>
-      <c r="UX32" s="98"/>
-      <c r="UY32" s="98"/>
-      <c r="UZ32" s="98"/>
-      <c r="VA32" s="98"/>
-      <c r="VB32" s="98"/>
-      <c r="VC32" s="98"/>
-      <c r="VD32" s="98"/>
-      <c r="VE32" s="98"/>
-      <c r="VF32" s="98"/>
-      <c r="VG32" s="98"/>
-      <c r="VH32" s="98"/>
-      <c r="VI32" s="98"/>
-      <c r="VJ32" s="98"/>
-      <c r="VK32" s="98"/>
-      <c r="VL32" s="98"/>
-      <c r="VM32" s="98"/>
-      <c r="VN32" s="98"/>
-      <c r="VO32" s="98"/>
-      <c r="VP32" s="98"/>
-      <c r="VQ32" s="98"/>
-      <c r="VR32" s="98"/>
-      <c r="VS32" s="98"/>
-      <c r="VT32" s="98"/>
-      <c r="VU32" s="98"/>
-      <c r="VV32" s="98"/>
-      <c r="VW32" s="98"/>
-      <c r="VX32" s="98"/>
-      <c r="VY32" s="98"/>
-      <c r="VZ32" s="98"/>
-      <c r="WA32" s="98"/>
-      <c r="WB32" s="98"/>
-      <c r="WC32" s="98"/>
-      <c r="WD32" s="98"/>
-      <c r="WE32" s="98"/>
-      <c r="WF32" s="98"/>
-      <c r="WG32" s="98"/>
-      <c r="WH32" s="98"/>
-      <c r="WI32" s="98"/>
-      <c r="WJ32" s="98"/>
-      <c r="WK32" s="98"/>
-      <c r="WL32" s="98"/>
-      <c r="WM32" s="98"/>
-      <c r="WN32" s="98"/>
-      <c r="WO32" s="98"/>
-      <c r="WP32" s="98"/>
-      <c r="WQ32" s="98"/>
-      <c r="WR32" s="98"/>
-      <c r="WS32" s="98"/>
-      <c r="WT32" s="98"/>
-      <c r="WU32" s="98"/>
-      <c r="WV32" s="98"/>
-      <c r="WW32" s="98"/>
-      <c r="WX32" s="98"/>
-      <c r="WY32" s="98"/>
-      <c r="WZ32" s="98"/>
-      <c r="XA32" s="98"/>
-      <c r="XB32" s="98"/>
-      <c r="XC32" s="98"/>
-      <c r="XD32" s="98"/>
-      <c r="XE32" s="98"/>
-      <c r="XF32" s="98"/>
-      <c r="XG32" s="98"/>
-      <c r="XH32" s="98"/>
-      <c r="XI32" s="98"/>
-      <c r="XJ32" s="98"/>
-      <c r="XK32" s="98"/>
-      <c r="XL32" s="98"/>
-      <c r="XM32" s="98"/>
-      <c r="XN32" s="98"/>
-      <c r="XO32" s="98"/>
-      <c r="XP32" s="98"/>
-      <c r="XQ32" s="98"/>
-      <c r="XR32" s="98"/>
-      <c r="XS32" s="98"/>
-      <c r="XT32" s="98"/>
-      <c r="XU32" s="98"/>
-      <c r="XV32" s="98"/>
-      <c r="XW32" s="98"/>
-      <c r="XX32" s="98"/>
-      <c r="XY32" s="98"/>
-      <c r="XZ32" s="98"/>
-      <c r="YA32" s="98"/>
-      <c r="YB32" s="98"/>
-      <c r="YC32" s="98"/>
-      <c r="YD32" s="98"/>
-      <c r="YE32" s="98"/>
-      <c r="YF32" s="98"/>
-      <c r="YG32" s="98"/>
-      <c r="YH32" s="98"/>
-      <c r="YI32" s="98"/>
-      <c r="YJ32" s="98"/>
-      <c r="YK32" s="98"/>
-      <c r="YL32" s="98"/>
-      <c r="YM32" s="98"/>
-      <c r="YN32" s="98"/>
-      <c r="YO32" s="98"/>
-      <c r="YP32" s="98"/>
-      <c r="YQ32" s="98"/>
-      <c r="YR32" s="98"/>
-      <c r="YS32" s="98"/>
-      <c r="YT32" s="98"/>
-      <c r="YU32" s="98"/>
-      <c r="YV32" s="98"/>
-      <c r="YW32" s="98"/>
-      <c r="YX32" s="98"/>
-      <c r="YY32" s="98"/>
-      <c r="YZ32" s="98"/>
-      <c r="ZA32" s="98"/>
-      <c r="ZB32" s="98"/>
-      <c r="ZC32" s="98"/>
-      <c r="ZD32" s="98"/>
-      <c r="ZE32" s="98"/>
-      <c r="ZF32" s="98"/>
-      <c r="ZG32" s="98"/>
-      <c r="ZH32" s="98"/>
-      <c r="ZI32" s="98"/>
-      <c r="ZJ32" s="98"/>
-      <c r="ZK32" s="98"/>
-      <c r="ZL32" s="98"/>
-      <c r="ZM32" s="98"/>
-      <c r="ZN32" s="98"/>
-      <c r="ZO32" s="98"/>
-      <c r="ZP32" s="98"/>
-      <c r="ZQ32" s="98"/>
-      <c r="ZR32" s="98"/>
-      <c r="ZS32" s="98"/>
-      <c r="ZT32" s="98"/>
-      <c r="ZU32" s="98"/>
-      <c r="ZV32" s="98"/>
-      <c r="ZW32" s="98"/>
-      <c r="ZX32" s="98"/>
-      <c r="ZY32" s="98"/>
-      <c r="ZZ32" s="98"/>
-      <c r="AAA32" s="98"/>
-      <c r="AAB32" s="98"/>
-      <c r="AAC32" s="98"/>
-      <c r="AAD32" s="98"/>
-      <c r="AAE32" s="98"/>
-      <c r="AAF32" s="98"/>
-      <c r="AAG32" s="98"/>
-      <c r="AAH32" s="98"/>
-      <c r="AAI32" s="98"/>
-      <c r="AAJ32" s="98"/>
-      <c r="AAK32" s="98"/>
-      <c r="AAL32" s="98"/>
-      <c r="AAM32" s="98"/>
-      <c r="AAN32" s="98"/>
-      <c r="AAO32" s="98"/>
-      <c r="AAP32" s="98"/>
-      <c r="AAQ32" s="98"/>
-      <c r="AAR32" s="98"/>
-      <c r="AAS32" s="98"/>
-      <c r="AAT32" s="98"/>
-      <c r="AAU32" s="98"/>
-      <c r="AAV32" s="98"/>
-      <c r="AAW32" s="98"/>
-      <c r="AAX32" s="98"/>
-      <c r="AAY32" s="98"/>
-      <c r="AAZ32" s="98"/>
-      <c r="ABA32" s="98"/>
-      <c r="ABB32" s="98"/>
-      <c r="ABC32" s="98"/>
-      <c r="ABD32" s="98"/>
-      <c r="ABE32" s="98"/>
-      <c r="ABF32" s="98"/>
-      <c r="ABG32" s="98"/>
-      <c r="ABH32" s="98"/>
-      <c r="ABI32" s="98"/>
-      <c r="ABJ32" s="98"/>
-      <c r="ABK32" s="98"/>
-      <c r="ABL32" s="98"/>
-      <c r="ABM32" s="98"/>
-      <c r="ABN32" s="98"/>
-      <c r="ABO32" s="98"/>
-      <c r="ABP32" s="98"/>
-      <c r="ABQ32" s="98"/>
-      <c r="ABR32" s="98"/>
-      <c r="ABS32" s="98"/>
-      <c r="ABT32" s="98"/>
-      <c r="ABU32" s="98"/>
-      <c r="ABV32" s="98"/>
-      <c r="ABW32" s="98"/>
-      <c r="ABX32" s="98"/>
-      <c r="ABY32" s="98"/>
-      <c r="ABZ32" s="98"/>
-      <c r="ACA32" s="98"/>
-      <c r="ACB32" s="98"/>
-      <c r="ACC32" s="98"/>
-      <c r="ACD32" s="98"/>
-      <c r="ACE32" s="98"/>
-      <c r="ACF32" s="98"/>
-      <c r="ACG32" s="98"/>
-      <c r="ACH32" s="98"/>
-      <c r="ACI32" s="98"/>
-      <c r="ACJ32" s="98"/>
-      <c r="ACK32" s="98"/>
-      <c r="ACL32" s="98"/>
-      <c r="ACM32" s="98"/>
-      <c r="ACN32" s="98"/>
-      <c r="ACO32" s="98"/>
-      <c r="ACP32" s="98"/>
-      <c r="ACQ32" s="98"/>
-      <c r="ACR32" s="98"/>
-      <c r="ACS32" s="98"/>
-      <c r="ACT32" s="98"/>
-      <c r="ACU32" s="98"/>
-      <c r="ACV32" s="98"/>
-      <c r="ACW32" s="98"/>
-      <c r="ACX32" s="98"/>
-      <c r="ACY32" s="98"/>
-      <c r="ACZ32" s="98"/>
-      <c r="ADA32" s="98"/>
-      <c r="ADB32" s="98"/>
-      <c r="ADC32" s="98"/>
-      <c r="ADD32" s="98"/>
-      <c r="ADE32" s="98"/>
-      <c r="ADF32" s="98"/>
-      <c r="ADG32" s="98"/>
-      <c r="ADH32" s="98"/>
-      <c r="ADI32" s="98"/>
-      <c r="ADJ32" s="98"/>
-      <c r="ADK32" s="98"/>
-      <c r="ADL32" s="98"/>
-      <c r="ADM32" s="98"/>
-      <c r="ADN32" s="98"/>
-      <c r="ADO32" s="98"/>
-      <c r="ADP32" s="98"/>
-      <c r="ADQ32" s="98"/>
-      <c r="ADR32" s="98"/>
-      <c r="ADS32" s="98"/>
-      <c r="ADT32" s="98"/>
-      <c r="ADU32" s="98"/>
-      <c r="ADV32" s="98"/>
-      <c r="ADW32" s="98"/>
-      <c r="ADX32" s="98"/>
-      <c r="ADY32" s="98"/>
-      <c r="ADZ32" s="98"/>
-      <c r="AEA32" s="98"/>
-      <c r="AEB32" s="98"/>
-      <c r="AEC32" s="98"/>
-      <c r="AED32" s="98"/>
-      <c r="AEE32" s="98"/>
-      <c r="AEF32" s="98"/>
-      <c r="AEG32" s="98"/>
-      <c r="AEH32" s="98"/>
-      <c r="AEI32" s="98"/>
-      <c r="AEJ32" s="98"/>
-      <c r="AEK32" s="98"/>
-      <c r="AEL32" s="98"/>
-      <c r="AEM32" s="98"/>
-      <c r="AEN32" s="98"/>
-      <c r="AEO32" s="98"/>
-      <c r="AEP32" s="98"/>
-      <c r="AEQ32" s="98"/>
-      <c r="AER32" s="98"/>
-      <c r="AES32" s="98"/>
-      <c r="AET32" s="98"/>
-      <c r="AEU32" s="98"/>
-      <c r="AEV32" s="98"/>
-      <c r="AEW32" s="98"/>
-      <c r="AEX32" s="98"/>
-      <c r="AEY32" s="98"/>
-      <c r="AEZ32" s="98"/>
-      <c r="AFA32" s="98"/>
-      <c r="AFB32" s="98"/>
-      <c r="AFC32" s="98"/>
-      <c r="AFD32" s="98"/>
-      <c r="AFE32" s="98"/>
-      <c r="AFF32" s="98"/>
-      <c r="AFG32" s="98"/>
-      <c r="AFH32" s="98"/>
-      <c r="AFI32" s="98"/>
-      <c r="AFJ32" s="98"/>
-      <c r="AFK32" s="98"/>
-      <c r="AFL32" s="98"/>
-      <c r="AFM32" s="98"/>
-      <c r="AFN32" s="98"/>
-      <c r="AFO32" s="98"/>
-      <c r="AFP32" s="98"/>
-      <c r="AFQ32" s="98"/>
-      <c r="AFR32" s="98"/>
-      <c r="AFS32" s="98"/>
-      <c r="AFT32" s="98"/>
-      <c r="AFU32" s="98"/>
-      <c r="AFV32" s="98"/>
-      <c r="AFW32" s="98"/>
-      <c r="AFX32" s="98"/>
-      <c r="AFY32" s="98"/>
-      <c r="AFZ32" s="98"/>
-      <c r="AGA32" s="98"/>
-      <c r="AGB32" s="98"/>
-      <c r="AGC32" s="98"/>
-      <c r="AGD32" s="98"/>
-      <c r="AGE32" s="98"/>
-      <c r="AGF32" s="98"/>
-      <c r="AGG32" s="98"/>
-      <c r="AGH32" s="98"/>
-      <c r="AGI32" s="98"/>
-      <c r="AGJ32" s="98"/>
-      <c r="AGK32" s="98"/>
-      <c r="AGL32" s="98"/>
-      <c r="AGM32" s="98"/>
-      <c r="AGN32" s="98"/>
-      <c r="AGO32" s="98"/>
-      <c r="AGP32" s="98"/>
-      <c r="AGQ32" s="98"/>
-      <c r="AGR32" s="98"/>
-      <c r="AGS32" s="98"/>
-      <c r="AGT32" s="98"/>
-      <c r="AGU32" s="98"/>
-      <c r="AGV32" s="98"/>
-      <c r="AGW32" s="98"/>
-      <c r="AGX32" s="98"/>
-      <c r="AGY32" s="98"/>
-      <c r="AGZ32" s="98"/>
-      <c r="AHA32" s="98"/>
-      <c r="AHB32" s="98"/>
-      <c r="AHC32" s="98"/>
-      <c r="AHD32" s="98"/>
-      <c r="AHE32" s="98"/>
-      <c r="AHF32" s="98"/>
-      <c r="AHG32" s="98"/>
-      <c r="AHH32" s="98"/>
-      <c r="AHI32" s="98"/>
-      <c r="AHJ32" s="98"/>
-      <c r="AHK32" s="98"/>
-      <c r="AHL32" s="98"/>
-      <c r="AHM32" s="98"/>
-      <c r="AHN32" s="98"/>
-      <c r="AHO32" s="98"/>
-      <c r="AHP32" s="98"/>
-      <c r="AHQ32" s="98"/>
-      <c r="AHR32" s="98"/>
-      <c r="AHS32" s="98"/>
-      <c r="AHT32" s="98"/>
-      <c r="AHU32" s="98"/>
-      <c r="AHV32" s="98"/>
-      <c r="AHW32" s="98"/>
-      <c r="AHX32" s="98"/>
-      <c r="AHY32" s="98"/>
-      <c r="AHZ32" s="98"/>
-      <c r="AIA32" s="98"/>
-      <c r="AIB32" s="98"/>
-      <c r="AIC32" s="98"/>
-      <c r="AID32" s="98"/>
-      <c r="AIE32" s="98"/>
-      <c r="AIF32" s="98"/>
-      <c r="AIG32" s="98"/>
-      <c r="AIH32" s="98"/>
-      <c r="AII32" s="98"/>
-      <c r="AIJ32" s="98"/>
-      <c r="AIK32" s="98"/>
-      <c r="AIL32" s="98"/>
-      <c r="AIM32" s="98"/>
-      <c r="AIN32" s="98"/>
-      <c r="AIO32" s="98"/>
-      <c r="AIP32" s="98"/>
-      <c r="AIQ32" s="98"/>
-      <c r="AIR32" s="98"/>
-      <c r="AIS32" s="98"/>
-      <c r="AIT32" s="98"/>
-      <c r="AIU32" s="98"/>
-      <c r="AIV32" s="98"/>
-      <c r="AIW32" s="98"/>
-      <c r="AIX32" s="98"/>
-      <c r="AIY32" s="98"/>
-      <c r="AIZ32" s="98"/>
-      <c r="AJA32" s="98"/>
-      <c r="AJB32" s="98"/>
-      <c r="AJC32" s="98"/>
-      <c r="AJD32" s="98"/>
-      <c r="AJE32" s="98"/>
-      <c r="AJF32" s="98"/>
-      <c r="AJG32" s="98"/>
-      <c r="AJH32" s="98"/>
-      <c r="AJI32" s="98"/>
-      <c r="AJJ32" s="98"/>
-      <c r="AJK32" s="98"/>
-      <c r="AJL32" s="98"/>
-      <c r="AJM32" s="98"/>
-      <c r="AJN32" s="98"/>
-      <c r="AJO32" s="98"/>
-      <c r="AJP32" s="98"/>
-      <c r="AJQ32" s="98"/>
-      <c r="AJR32" s="98"/>
-      <c r="AJS32" s="98"/>
-      <c r="AJT32" s="98"/>
-      <c r="AJU32" s="98"/>
-      <c r="AJV32" s="98"/>
-      <c r="AJW32" s="98"/>
-      <c r="AJX32" s="98"/>
-      <c r="AJY32" s="98"/>
-      <c r="AJZ32" s="98"/>
-      <c r="AKA32" s="98"/>
-      <c r="AKB32" s="98"/>
-      <c r="AKC32" s="98"/>
-      <c r="AKD32" s="98"/>
-      <c r="AKE32" s="98"/>
-      <c r="AKF32" s="98"/>
-      <c r="AKG32" s="98"/>
-      <c r="AKH32" s="98"/>
-      <c r="AKI32" s="98"/>
-      <c r="AKJ32" s="98"/>
-      <c r="AKK32" s="98"/>
-      <c r="AKL32" s="98"/>
-      <c r="AKM32" s="98"/>
-      <c r="AKN32" s="98"/>
-      <c r="AKO32" s="98"/>
-      <c r="AKP32" s="98"/>
-      <c r="AKQ32" s="98"/>
-      <c r="AKR32" s="98"/>
-      <c r="AKS32" s="98"/>
-      <c r="AKT32" s="98"/>
-      <c r="AKU32" s="98"/>
-      <c r="AKV32" s="98"/>
-      <c r="AKW32" s="98"/>
-      <c r="AKX32" s="98"/>
-      <c r="AKY32" s="98"/>
-      <c r="AKZ32" s="98"/>
-      <c r="ALA32" s="98"/>
-      <c r="ALB32" s="98"/>
-      <c r="ALC32" s="98"/>
-      <c r="ALD32" s="98"/>
-      <c r="ALE32" s="98"/>
-      <c r="ALF32" s="98"/>
-      <c r="ALG32" s="98"/>
-      <c r="ALH32" s="98"/>
-      <c r="ALI32" s="98"/>
-      <c r="ALJ32" s="98"/>
-      <c r="ALK32" s="98"/>
-      <c r="ALL32" s="98"/>
-      <c r="ALM32" s="98"/>
-      <c r="ALN32" s="98"/>
-      <c r="ALO32" s="98"/>
-      <c r="ALP32" s="98"/>
-      <c r="ALQ32" s="98"/>
-      <c r="ALR32" s="98"/>
-      <c r="ALS32" s="98"/>
-      <c r="ALT32" s="98"/>
-      <c r="ALU32" s="98"/>
-      <c r="ALV32" s="98"/>
-      <c r="ALW32" s="98"/>
-      <c r="ALX32" s="98"/>
-      <c r="ALY32" s="98"/>
-      <c r="ALZ32" s="98"/>
-      <c r="AMA32" s="98"/>
-      <c r="AMB32" s="98"/>
-      <c r="AMC32" s="98"/>
-      <c r="AMD32" s="98"/>
-      <c r="AME32" s="98"/>
-      <c r="AMF32" s="98"/>
-      <c r="AMG32" s="98"/>
-      <c r="AMH32" s="98"/>
-      <c r="AMI32" s="98"/>
-      <c r="AMJ32" s="98"/>
-      <c r="AMK32" s="98"/>
-      <c r="AML32" s="98"/>
-      <c r="AMM32" s="98"/>
+      <c r="I32" s="72" t="s">
+        <v>647</v>
+      </c>
+      <c r="J32" s="96"/>
+      <c r="K32" s="96"/>
+      <c r="L32" s="96"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="96"/>
+      <c r="O32" s="96"/>
+      <c r="P32" s="96"/>
+      <c r="Q32" s="96"/>
+      <c r="R32" s="96"/>
+      <c r="S32" s="96"/>
+      <c r="T32" s="96"/>
+      <c r="U32" s="96"/>
+      <c r="V32" s="96"/>
+      <c r="W32" s="96"/>
+      <c r="X32" s="96"/>
+      <c r="Y32" s="96"/>
+      <c r="Z32" s="96"/>
+      <c r="AA32" s="96"/>
+      <c r="AB32" s="96"/>
+      <c r="AC32" s="96"/>
+      <c r="AD32" s="96"/>
+      <c r="AE32" s="96"/>
+      <c r="AF32" s="96"/>
+      <c r="AG32" s="96"/>
+      <c r="AH32" s="96"/>
+      <c r="AI32" s="96"/>
+      <c r="AJ32" s="96"/>
+      <c r="AK32" s="96"/>
+      <c r="AL32" s="96"/>
+      <c r="AM32" s="96"/>
+      <c r="AN32" s="96"/>
+      <c r="AO32" s="96"/>
+      <c r="AP32" s="96"/>
+      <c r="AQ32" s="96"/>
+      <c r="AR32" s="96"/>
+      <c r="AS32" s="96"/>
+      <c r="AT32" s="96"/>
+      <c r="AU32" s="96"/>
+      <c r="AV32" s="96"/>
+      <c r="AW32" s="96"/>
+      <c r="AX32" s="96"/>
+      <c r="AY32" s="96"/>
+      <c r="AZ32" s="96"/>
+      <c r="BA32" s="96"/>
+      <c r="BB32" s="96"/>
+      <c r="BC32" s="96"/>
+      <c r="BD32" s="96"/>
+      <c r="BE32" s="96"/>
+      <c r="BF32" s="96"/>
+      <c r="BG32" s="96"/>
+      <c r="BH32" s="96"/>
+      <c r="BI32" s="96"/>
+      <c r="BJ32" s="96"/>
+      <c r="BK32" s="96"/>
+      <c r="BL32" s="96"/>
+      <c r="BM32" s="96"/>
+      <c r="BN32" s="96"/>
+      <c r="BO32" s="96"/>
+      <c r="BP32" s="96"/>
+      <c r="BQ32" s="96"/>
+      <c r="BR32" s="96"/>
+      <c r="BS32" s="96"/>
+      <c r="BT32" s="96"/>
+      <c r="BU32" s="96"/>
+      <c r="BV32" s="96"/>
+      <c r="BW32" s="96"/>
+      <c r="BX32" s="96"/>
+      <c r="BY32" s="96"/>
+      <c r="BZ32" s="96"/>
+      <c r="CA32" s="96"/>
+      <c r="CB32" s="96"/>
+      <c r="CC32" s="96"/>
+      <c r="CD32" s="96"/>
+      <c r="CE32" s="96"/>
+      <c r="CF32" s="96"/>
+      <c r="CG32" s="96"/>
+      <c r="CH32" s="96"/>
+      <c r="CI32" s="96"/>
+      <c r="CJ32" s="96"/>
+      <c r="CK32" s="96"/>
+      <c r="CL32" s="96"/>
+      <c r="CM32" s="96"/>
+      <c r="CN32" s="96"/>
+      <c r="CO32" s="96"/>
+      <c r="CP32" s="96"/>
+      <c r="CQ32" s="96"/>
+      <c r="CR32" s="96"/>
+      <c r="CS32" s="96"/>
+      <c r="CT32" s="96"/>
+      <c r="CU32" s="96"/>
+      <c r="CV32" s="96"/>
+      <c r="CW32" s="96"/>
+      <c r="CX32" s="96"/>
+      <c r="CY32" s="96"/>
+      <c r="CZ32" s="96"/>
+      <c r="DA32" s="96"/>
+      <c r="DB32" s="96"/>
+      <c r="DC32" s="96"/>
+      <c r="DD32" s="96"/>
+      <c r="DE32" s="96"/>
+      <c r="DF32" s="96"/>
+      <c r="DG32" s="96"/>
+      <c r="DH32" s="96"/>
+      <c r="DI32" s="96"/>
+      <c r="DJ32" s="96"/>
+      <c r="DK32" s="96"/>
+      <c r="DL32" s="96"/>
+      <c r="DM32" s="96"/>
+      <c r="DN32" s="96"/>
+      <c r="DO32" s="96"/>
+      <c r="DP32" s="96"/>
+      <c r="DQ32" s="96"/>
+      <c r="DR32" s="96"/>
+      <c r="DS32" s="96"/>
+      <c r="DT32" s="96"/>
+      <c r="DU32" s="96"/>
+      <c r="DV32" s="96"/>
+      <c r="DW32" s="96"/>
+      <c r="DX32" s="96"/>
+      <c r="DY32" s="96"/>
+      <c r="DZ32" s="96"/>
+      <c r="EA32" s="96"/>
+      <c r="EB32" s="96"/>
+      <c r="EC32" s="96"/>
+      <c r="ED32" s="96"/>
+      <c r="EE32" s="96"/>
+      <c r="EF32" s="96"/>
+      <c r="EG32" s="96"/>
+      <c r="EH32" s="96"/>
+      <c r="EI32" s="96"/>
+      <c r="EJ32" s="96"/>
+      <c r="EK32" s="96"/>
+      <c r="EL32" s="96"/>
+      <c r="EM32" s="96"/>
+      <c r="EN32" s="96"/>
+      <c r="EO32" s="96"/>
+      <c r="EP32" s="96"/>
+      <c r="EQ32" s="96"/>
+      <c r="ER32" s="96"/>
+      <c r="ES32" s="96"/>
+      <c r="ET32" s="96"/>
+      <c r="EU32" s="96"/>
+      <c r="EV32" s="96"/>
+      <c r="EW32" s="96"/>
+      <c r="EX32" s="96"/>
+      <c r="EY32" s="96"/>
+      <c r="EZ32" s="96"/>
+      <c r="FA32" s="96"/>
+      <c r="FB32" s="96"/>
+      <c r="FC32" s="96"/>
+      <c r="FD32" s="96"/>
+      <c r="FE32" s="96"/>
+      <c r="FF32" s="96"/>
+      <c r="FG32" s="96"/>
+      <c r="FH32" s="96"/>
+      <c r="FI32" s="96"/>
+      <c r="FJ32" s="96"/>
+      <c r="FK32" s="96"/>
+      <c r="FL32" s="96"/>
+      <c r="FM32" s="96"/>
+      <c r="FN32" s="96"/>
+      <c r="FO32" s="96"/>
+      <c r="FP32" s="96"/>
+      <c r="FQ32" s="96"/>
+      <c r="FR32" s="96"/>
+      <c r="FS32" s="96"/>
+      <c r="FT32" s="96"/>
+      <c r="FU32" s="96"/>
+      <c r="FV32" s="96"/>
+      <c r="FW32" s="96"/>
+      <c r="FX32" s="96"/>
+      <c r="FY32" s="96"/>
+      <c r="FZ32" s="96"/>
+      <c r="GA32" s="96"/>
+      <c r="GB32" s="96"/>
+      <c r="GC32" s="96"/>
+      <c r="GD32" s="96"/>
+      <c r="GE32" s="96"/>
+      <c r="GF32" s="96"/>
+      <c r="GG32" s="96"/>
+      <c r="GH32" s="96"/>
+      <c r="GI32" s="96"/>
+      <c r="GJ32" s="96"/>
+      <c r="GK32" s="96"/>
+      <c r="GL32" s="96"/>
+      <c r="GM32" s="96"/>
+      <c r="GN32" s="96"/>
+      <c r="GO32" s="96"/>
+      <c r="GP32" s="96"/>
+      <c r="GQ32" s="96"/>
+      <c r="GR32" s="96"/>
+      <c r="GS32" s="96"/>
+      <c r="GT32" s="96"/>
+      <c r="GU32" s="96"/>
+      <c r="GV32" s="96"/>
+      <c r="GW32" s="96"/>
+      <c r="GX32" s="96"/>
+      <c r="GY32" s="96"/>
+      <c r="GZ32" s="96"/>
+      <c r="HA32" s="96"/>
+      <c r="HB32" s="96"/>
+      <c r="HC32" s="96"/>
+      <c r="HD32" s="96"/>
+      <c r="HE32" s="96"/>
+      <c r="HF32" s="96"/>
+      <c r="HG32" s="96"/>
+      <c r="HH32" s="96"/>
+      <c r="HI32" s="96"/>
+      <c r="HJ32" s="96"/>
+      <c r="HK32" s="96"/>
+      <c r="HL32" s="96"/>
+      <c r="HM32" s="96"/>
+      <c r="HN32" s="96"/>
+      <c r="HO32" s="96"/>
+      <c r="HP32" s="96"/>
+      <c r="HQ32" s="96"/>
+      <c r="HR32" s="96"/>
+      <c r="HS32" s="96"/>
+      <c r="HT32" s="96"/>
+      <c r="HU32" s="96"/>
+      <c r="HV32" s="96"/>
+      <c r="HW32" s="96"/>
+      <c r="HX32" s="96"/>
+      <c r="HY32" s="96"/>
+      <c r="HZ32" s="96"/>
+      <c r="IA32" s="96"/>
+      <c r="IB32" s="96"/>
+      <c r="IC32" s="96"/>
+      <c r="ID32" s="96"/>
+      <c r="IE32" s="96"/>
+      <c r="IF32" s="96"/>
+      <c r="IG32" s="96"/>
+      <c r="IH32" s="96"/>
+      <c r="II32" s="96"/>
+      <c r="IJ32" s="96"/>
+      <c r="IK32" s="96"/>
+      <c r="IL32" s="96"/>
+      <c r="IM32" s="96"/>
+      <c r="IN32" s="96"/>
+      <c r="IO32" s="96"/>
+      <c r="IP32" s="96"/>
+      <c r="IQ32" s="96"/>
+      <c r="IR32" s="96"/>
+      <c r="IS32" s="96"/>
+      <c r="IT32" s="96"/>
+      <c r="IU32" s="96"/>
+      <c r="IV32" s="96"/>
+      <c r="IW32" s="96"/>
+      <c r="IX32" s="96"/>
+      <c r="IY32" s="96"/>
+      <c r="IZ32" s="96"/>
+      <c r="JA32" s="96"/>
+      <c r="JB32" s="96"/>
+      <c r="JC32" s="96"/>
+      <c r="JD32" s="96"/>
+      <c r="JE32" s="96"/>
+      <c r="JF32" s="96"/>
+      <c r="JG32" s="96"/>
+      <c r="JH32" s="96"/>
+      <c r="JI32" s="96"/>
+      <c r="JJ32" s="96"/>
+      <c r="JK32" s="96"/>
+      <c r="JL32" s="96"/>
+      <c r="JM32" s="96"/>
+      <c r="JN32" s="96"/>
+      <c r="JO32" s="96"/>
+      <c r="JP32" s="96"/>
+      <c r="JQ32" s="96"/>
+      <c r="JR32" s="96"/>
+      <c r="JS32" s="96"/>
+      <c r="JT32" s="96"/>
+      <c r="JU32" s="96"/>
+      <c r="JV32" s="96"/>
+      <c r="JW32" s="96"/>
+      <c r="JX32" s="96"/>
+      <c r="JY32" s="96"/>
+      <c r="JZ32" s="96"/>
+      <c r="KA32" s="96"/>
+      <c r="KB32" s="96"/>
+      <c r="KC32" s="96"/>
+      <c r="KD32" s="96"/>
+      <c r="KE32" s="96"/>
+      <c r="KF32" s="96"/>
+      <c r="KG32" s="96"/>
+      <c r="KH32" s="96"/>
+      <c r="KI32" s="96"/>
+      <c r="KJ32" s="96"/>
+      <c r="KK32" s="96"/>
+      <c r="KL32" s="96"/>
+      <c r="KM32" s="96"/>
+      <c r="KN32" s="96"/>
+      <c r="KO32" s="96"/>
+      <c r="KP32" s="96"/>
+      <c r="KQ32" s="96"/>
+      <c r="KR32" s="96"/>
+      <c r="KS32" s="96"/>
+      <c r="KT32" s="96"/>
+      <c r="KU32" s="96"/>
+      <c r="KV32" s="96"/>
+      <c r="KW32" s="96"/>
+      <c r="KX32" s="96"/>
+      <c r="KY32" s="96"/>
+      <c r="KZ32" s="96"/>
+      <c r="LA32" s="96"/>
+      <c r="LB32" s="96"/>
+      <c r="LC32" s="96"/>
+      <c r="LD32" s="96"/>
+      <c r="LE32" s="96"/>
+      <c r="LF32" s="96"/>
+      <c r="LG32" s="96"/>
+      <c r="LH32" s="96"/>
+      <c r="LI32" s="96"/>
+      <c r="LJ32" s="96"/>
+      <c r="LK32" s="96"/>
+      <c r="LL32" s="96"/>
+      <c r="LM32" s="96"/>
+      <c r="LN32" s="96"/>
+      <c r="LO32" s="96"/>
+      <c r="LP32" s="96"/>
+      <c r="LQ32" s="96"/>
+      <c r="LR32" s="96"/>
+      <c r="LS32" s="96"/>
+      <c r="LT32" s="96"/>
+      <c r="LU32" s="96"/>
+      <c r="LV32" s="96"/>
+      <c r="LW32" s="96"/>
+      <c r="LX32" s="96"/>
+      <c r="LY32" s="96"/>
+      <c r="LZ32" s="96"/>
+      <c r="MA32" s="96"/>
+      <c r="MB32" s="96"/>
+      <c r="MC32" s="96"/>
+      <c r="MD32" s="96"/>
+      <c r="ME32" s="96"/>
+      <c r="MF32" s="96"/>
+      <c r="MG32" s="96"/>
+      <c r="MH32" s="96"/>
+      <c r="MI32" s="96"/>
+      <c r="MJ32" s="96"/>
+      <c r="MK32" s="96"/>
+      <c r="ML32" s="96"/>
+      <c r="MM32" s="96"/>
+      <c r="MN32" s="96"/>
+      <c r="MO32" s="96"/>
+      <c r="MP32" s="96"/>
+      <c r="MQ32" s="96"/>
+      <c r="MR32" s="96"/>
+      <c r="MS32" s="96"/>
+      <c r="MT32" s="96"/>
+      <c r="MU32" s="96"/>
+      <c r="MV32" s="96"/>
+      <c r="MW32" s="96"/>
+      <c r="MX32" s="96"/>
+      <c r="MY32" s="96"/>
+      <c r="MZ32" s="96"/>
+      <c r="NA32" s="96"/>
+      <c r="NB32" s="96"/>
+      <c r="NC32" s="96"/>
+      <c r="ND32" s="96"/>
+      <c r="NE32" s="96"/>
+      <c r="NF32" s="96"/>
+      <c r="NG32" s="96"/>
+      <c r="NH32" s="96"/>
+      <c r="NI32" s="96"/>
+      <c r="NJ32" s="96"/>
+      <c r="NK32" s="96"/>
+      <c r="NL32" s="96"/>
+      <c r="NM32" s="96"/>
+      <c r="NN32" s="96"/>
+      <c r="NO32" s="96"/>
+      <c r="NP32" s="96"/>
+      <c r="NQ32" s="96"/>
+      <c r="NR32" s="96"/>
+      <c r="NS32" s="96"/>
+      <c r="NT32" s="96"/>
+      <c r="NU32" s="96"/>
+      <c r="NV32" s="96"/>
+      <c r="NW32" s="96"/>
+      <c r="NX32" s="96"/>
+      <c r="NY32" s="96"/>
+      <c r="NZ32" s="96"/>
+      <c r="OA32" s="96"/>
+      <c r="OB32" s="96"/>
+      <c r="OC32" s="96"/>
+      <c r="OD32" s="96"/>
+      <c r="OE32" s="96"/>
+      <c r="OF32" s="96"/>
+      <c r="OG32" s="96"/>
+      <c r="OH32" s="96"/>
+      <c r="OI32" s="96"/>
+      <c r="OJ32" s="96"/>
+      <c r="OK32" s="96"/>
+      <c r="OL32" s="96"/>
+      <c r="OM32" s="96"/>
+      <c r="ON32" s="96"/>
+      <c r="OO32" s="96"/>
+      <c r="OP32" s="96"/>
+      <c r="OQ32" s="96"/>
+      <c r="OR32" s="96"/>
+      <c r="OS32" s="96"/>
+      <c r="OT32" s="96"/>
+      <c r="OU32" s="96"/>
+      <c r="OV32" s="96"/>
+      <c r="OW32" s="96"/>
+      <c r="OX32" s="96"/>
+      <c r="OY32" s="96"/>
+      <c r="OZ32" s="96"/>
+      <c r="PA32" s="96"/>
+      <c r="PB32" s="96"/>
+      <c r="PC32" s="96"/>
+      <c r="PD32" s="96"/>
+      <c r="PE32" s="96"/>
+      <c r="PF32" s="96"/>
+      <c r="PG32" s="96"/>
+      <c r="PH32" s="96"/>
+      <c r="PI32" s="96"/>
+      <c r="PJ32" s="96"/>
+      <c r="PK32" s="96"/>
+      <c r="PL32" s="96"/>
+      <c r="PM32" s="96"/>
+      <c r="PN32" s="96"/>
+      <c r="PO32" s="96"/>
+      <c r="PP32" s="96"/>
+      <c r="PQ32" s="96"/>
+      <c r="PR32" s="96"/>
+      <c r="PS32" s="96"/>
+      <c r="PT32" s="96"/>
+      <c r="PU32" s="96"/>
+      <c r="PV32" s="96"/>
+      <c r="PW32" s="96"/>
+      <c r="PX32" s="96"/>
+      <c r="PY32" s="96"/>
+      <c r="PZ32" s="96"/>
+      <c r="QA32" s="96"/>
+      <c r="QB32" s="96"/>
+      <c r="QC32" s="96"/>
+      <c r="QD32" s="96"/>
+      <c r="QE32" s="96"/>
+      <c r="QF32" s="96"/>
+      <c r="QG32" s="96"/>
+      <c r="QH32" s="96"/>
+      <c r="QI32" s="96"/>
+      <c r="QJ32" s="96"/>
+      <c r="QK32" s="96"/>
+      <c r="QL32" s="96"/>
+      <c r="QM32" s="96"/>
+      <c r="QN32" s="96"/>
+      <c r="QO32" s="96"/>
+      <c r="QP32" s="96"/>
+      <c r="QQ32" s="96"/>
+      <c r="QR32" s="96"/>
+      <c r="QS32" s="96"/>
+      <c r="QT32" s="96"/>
+      <c r="QU32" s="96"/>
+      <c r="QV32" s="96"/>
+      <c r="QW32" s="96"/>
+      <c r="QX32" s="96"/>
+      <c r="QY32" s="96"/>
+      <c r="QZ32" s="96"/>
+      <c r="RA32" s="96"/>
+      <c r="RB32" s="96"/>
+      <c r="RC32" s="96"/>
+      <c r="RD32" s="96"/>
+      <c r="RE32" s="96"/>
+      <c r="RF32" s="96"/>
+      <c r="RG32" s="96"/>
+      <c r="RH32" s="96"/>
+      <c r="RI32" s="96"/>
+      <c r="RJ32" s="96"/>
+      <c r="RK32" s="96"/>
+      <c r="RL32" s="96"/>
+      <c r="RM32" s="96"/>
+      <c r="RN32" s="96"/>
+      <c r="RO32" s="96"/>
+      <c r="RP32" s="96"/>
+      <c r="RQ32" s="96"/>
+      <c r="RR32" s="96"/>
+      <c r="RS32" s="96"/>
+      <c r="RT32" s="96"/>
+      <c r="RU32" s="96"/>
+      <c r="RV32" s="96"/>
+      <c r="RW32" s="96"/>
+      <c r="RX32" s="96"/>
+      <c r="RY32" s="96"/>
+      <c r="RZ32" s="96"/>
+      <c r="SA32" s="96"/>
+      <c r="SB32" s="96"/>
+      <c r="SC32" s="96"/>
+      <c r="SD32" s="96"/>
+      <c r="SE32" s="96"/>
+      <c r="SF32" s="96"/>
+      <c r="SG32" s="96"/>
+      <c r="SH32" s="96"/>
+      <c r="SI32" s="96"/>
+      <c r="SJ32" s="96"/>
+      <c r="SK32" s="96"/>
+      <c r="SL32" s="96"/>
+      <c r="SM32" s="96"/>
+      <c r="SN32" s="96"/>
+      <c r="SO32" s="96"/>
+      <c r="SP32" s="96"/>
+      <c r="SQ32" s="96"/>
+      <c r="SR32" s="96"/>
+      <c r="SS32" s="96"/>
+      <c r="ST32" s="96"/>
+      <c r="SU32" s="96"/>
+      <c r="SV32" s="96"/>
+      <c r="SW32" s="96"/>
+      <c r="SX32" s="96"/>
+      <c r="SY32" s="96"/>
+      <c r="SZ32" s="96"/>
+      <c r="TA32" s="96"/>
+      <c r="TB32" s="96"/>
+      <c r="TC32" s="96"/>
+      <c r="TD32" s="96"/>
+      <c r="TE32" s="96"/>
+      <c r="TF32" s="96"/>
+      <c r="TG32" s="96"/>
+      <c r="TH32" s="96"/>
+      <c r="TI32" s="96"/>
+      <c r="TJ32" s="96"/>
+      <c r="TK32" s="96"/>
+      <c r="TL32" s="96"/>
+      <c r="TM32" s="96"/>
+      <c r="TN32" s="96"/>
+      <c r="TO32" s="96"/>
+      <c r="TP32" s="96"/>
+      <c r="TQ32" s="96"/>
+      <c r="TR32" s="96"/>
+      <c r="TS32" s="96"/>
+      <c r="TT32" s="96"/>
+      <c r="TU32" s="96"/>
+      <c r="TV32" s="96"/>
+      <c r="TW32" s="96"/>
+      <c r="TX32" s="96"/>
+      <c r="TY32" s="96"/>
+      <c r="TZ32" s="96"/>
+      <c r="UA32" s="96"/>
+      <c r="UB32" s="96"/>
+      <c r="UC32" s="96"/>
+      <c r="UD32" s="96"/>
+      <c r="UE32" s="96"/>
+      <c r="UF32" s="96"/>
+      <c r="UG32" s="96"/>
+      <c r="UH32" s="96"/>
+      <c r="UI32" s="96"/>
+      <c r="UJ32" s="96"/>
+      <c r="UK32" s="96"/>
+      <c r="UL32" s="96"/>
+      <c r="UM32" s="96"/>
+      <c r="UN32" s="96"/>
+      <c r="UO32" s="96"/>
+      <c r="UP32" s="96"/>
+      <c r="UQ32" s="96"/>
+      <c r="UR32" s="96"/>
+      <c r="US32" s="96"/>
+      <c r="UT32" s="96"/>
+      <c r="UU32" s="96"/>
+      <c r="UV32" s="96"/>
+      <c r="UW32" s="96"/>
+      <c r="UX32" s="96"/>
+      <c r="UY32" s="96"/>
+      <c r="UZ32" s="96"/>
+      <c r="VA32" s="96"/>
+      <c r="VB32" s="96"/>
+      <c r="VC32" s="96"/>
+      <c r="VD32" s="96"/>
+      <c r="VE32" s="96"/>
+      <c r="VF32" s="96"/>
+      <c r="VG32" s="96"/>
+      <c r="VH32" s="96"/>
+      <c r="VI32" s="96"/>
+      <c r="VJ32" s="96"/>
+      <c r="VK32" s="96"/>
+      <c r="VL32" s="96"/>
+      <c r="VM32" s="96"/>
+      <c r="VN32" s="96"/>
+      <c r="VO32" s="96"/>
+      <c r="VP32" s="96"/>
+      <c r="VQ32" s="96"/>
+      <c r="VR32" s="96"/>
+      <c r="VS32" s="96"/>
+      <c r="VT32" s="96"/>
+      <c r="VU32" s="96"/>
+      <c r="VV32" s="96"/>
+      <c r="VW32" s="96"/>
+      <c r="VX32" s="96"/>
+      <c r="VY32" s="96"/>
+      <c r="VZ32" s="96"/>
+      <c r="WA32" s="96"/>
+      <c r="WB32" s="96"/>
+      <c r="WC32" s="96"/>
+      <c r="WD32" s="96"/>
+      <c r="WE32" s="96"/>
+      <c r="WF32" s="96"/>
+      <c r="WG32" s="96"/>
+      <c r="WH32" s="96"/>
+      <c r="WI32" s="96"/>
+      <c r="WJ32" s="96"/>
+      <c r="WK32" s="96"/>
+      <c r="WL32" s="96"/>
+      <c r="WM32" s="96"/>
+      <c r="WN32" s="96"/>
+      <c r="WO32" s="96"/>
+      <c r="WP32" s="96"/>
+      <c r="WQ32" s="96"/>
+      <c r="WR32" s="96"/>
+      <c r="WS32" s="96"/>
+      <c r="WT32" s="96"/>
+      <c r="WU32" s="96"/>
+      <c r="WV32" s="96"/>
+      <c r="WW32" s="96"/>
+      <c r="WX32" s="96"/>
+      <c r="WY32" s="96"/>
+      <c r="WZ32" s="96"/>
+      <c r="XA32" s="96"/>
+      <c r="XB32" s="96"/>
+      <c r="XC32" s="96"/>
+      <c r="XD32" s="96"/>
+      <c r="XE32" s="96"/>
+      <c r="XF32" s="96"/>
+      <c r="XG32" s="96"/>
+      <c r="XH32" s="96"/>
+      <c r="XI32" s="96"/>
+      <c r="XJ32" s="96"/>
+      <c r="XK32" s="96"/>
+      <c r="XL32" s="96"/>
+      <c r="XM32" s="96"/>
+      <c r="XN32" s="96"/>
+      <c r="XO32" s="96"/>
+      <c r="XP32" s="96"/>
+      <c r="XQ32" s="96"/>
+      <c r="XR32" s="96"/>
+      <c r="XS32" s="96"/>
+      <c r="XT32" s="96"/>
+      <c r="XU32" s="96"/>
+      <c r="XV32" s="96"/>
+      <c r="XW32" s="96"/>
+      <c r="XX32" s="96"/>
+      <c r="XY32" s="96"/>
+      <c r="XZ32" s="96"/>
+      <c r="YA32" s="96"/>
+      <c r="YB32" s="96"/>
+      <c r="YC32" s="96"/>
+      <c r="YD32" s="96"/>
+      <c r="YE32" s="96"/>
+      <c r="YF32" s="96"/>
+      <c r="YG32" s="96"/>
+      <c r="YH32" s="96"/>
+      <c r="YI32" s="96"/>
+      <c r="YJ32" s="96"/>
+      <c r="YK32" s="96"/>
+      <c r="YL32" s="96"/>
+      <c r="YM32" s="96"/>
+      <c r="YN32" s="96"/>
+      <c r="YO32" s="96"/>
+      <c r="YP32" s="96"/>
+      <c r="YQ32" s="96"/>
+      <c r="YR32" s="96"/>
+      <c r="YS32" s="96"/>
+      <c r="YT32" s="96"/>
+      <c r="YU32" s="96"/>
+      <c r="YV32" s="96"/>
+      <c r="YW32" s="96"/>
+      <c r="YX32" s="96"/>
+      <c r="YY32" s="96"/>
+      <c r="YZ32" s="96"/>
+      <c r="ZA32" s="96"/>
+      <c r="ZB32" s="96"/>
+      <c r="ZC32" s="96"/>
+      <c r="ZD32" s="96"/>
+      <c r="ZE32" s="96"/>
+      <c r="ZF32" s="96"/>
+      <c r="ZG32" s="96"/>
+      <c r="ZH32" s="96"/>
+      <c r="ZI32" s="96"/>
+      <c r="ZJ32" s="96"/>
+      <c r="ZK32" s="96"/>
+      <c r="ZL32" s="96"/>
+      <c r="ZM32" s="96"/>
+      <c r="ZN32" s="96"/>
+      <c r="ZO32" s="96"/>
+      <c r="ZP32" s="96"/>
+      <c r="ZQ32" s="96"/>
+      <c r="ZR32" s="96"/>
+      <c r="ZS32" s="96"/>
+      <c r="ZT32" s="96"/>
+      <c r="ZU32" s="96"/>
+      <c r="ZV32" s="96"/>
+      <c r="ZW32" s="96"/>
+      <c r="ZX32" s="96"/>
+      <c r="ZY32" s="96"/>
+      <c r="ZZ32" s="96"/>
+      <c r="AAA32" s="96"/>
+      <c r="AAB32" s="96"/>
+      <c r="AAC32" s="96"/>
+      <c r="AAD32" s="96"/>
+      <c r="AAE32" s="96"/>
+      <c r="AAF32" s="96"/>
+      <c r="AAG32" s="96"/>
+      <c r="AAH32" s="96"/>
+      <c r="AAI32" s="96"/>
+      <c r="AAJ32" s="96"/>
+      <c r="AAK32" s="96"/>
+      <c r="AAL32" s="96"/>
+      <c r="AAM32" s="96"/>
+      <c r="AAN32" s="96"/>
+      <c r="AAO32" s="96"/>
+      <c r="AAP32" s="96"/>
+      <c r="AAQ32" s="96"/>
+      <c r="AAR32" s="96"/>
+      <c r="AAS32" s="96"/>
+      <c r="AAT32" s="96"/>
+      <c r="AAU32" s="96"/>
+      <c r="AAV32" s="96"/>
+      <c r="AAW32" s="96"/>
+      <c r="AAX32" s="96"/>
+      <c r="AAY32" s="96"/>
+      <c r="AAZ32" s="96"/>
+      <c r="ABA32" s="96"/>
+      <c r="ABB32" s="96"/>
+      <c r="ABC32" s="96"/>
+      <c r="ABD32" s="96"/>
+      <c r="ABE32" s="96"/>
+      <c r="ABF32" s="96"/>
+      <c r="ABG32" s="96"/>
+      <c r="ABH32" s="96"/>
+      <c r="ABI32" s="96"/>
+      <c r="ABJ32" s="96"/>
+      <c r="ABK32" s="96"/>
+      <c r="ABL32" s="96"/>
+      <c r="ABM32" s="96"/>
+      <c r="ABN32" s="96"/>
+      <c r="ABO32" s="96"/>
+      <c r="ABP32" s="96"/>
+      <c r="ABQ32" s="96"/>
+      <c r="ABR32" s="96"/>
+      <c r="ABS32" s="96"/>
+      <c r="ABT32" s="96"/>
+      <c r="ABU32" s="96"/>
+      <c r="ABV32" s="96"/>
+      <c r="ABW32" s="96"/>
+      <c r="ABX32" s="96"/>
+      <c r="ABY32" s="96"/>
+      <c r="ABZ32" s="96"/>
+      <c r="ACA32" s="96"/>
+      <c r="ACB32" s="96"/>
+      <c r="ACC32" s="96"/>
+      <c r="ACD32" s="96"/>
+      <c r="ACE32" s="96"/>
+      <c r="ACF32" s="96"/>
+      <c r="ACG32" s="96"/>
+      <c r="ACH32" s="96"/>
+      <c r="ACI32" s="96"/>
+      <c r="ACJ32" s="96"/>
+      <c r="ACK32" s="96"/>
+      <c r="ACL32" s="96"/>
+      <c r="ACM32" s="96"/>
+      <c r="ACN32" s="96"/>
+      <c r="ACO32" s="96"/>
+      <c r="ACP32" s="96"/>
+      <c r="ACQ32" s="96"/>
+      <c r="ACR32" s="96"/>
+      <c r="ACS32" s="96"/>
+      <c r="ACT32" s="96"/>
+      <c r="ACU32" s="96"/>
+      <c r="ACV32" s="96"/>
+      <c r="ACW32" s="96"/>
+      <c r="ACX32" s="96"/>
+      <c r="ACY32" s="96"/>
+      <c r="ACZ32" s="96"/>
+      <c r="ADA32" s="96"/>
+      <c r="ADB32" s="96"/>
+      <c r="ADC32" s="96"/>
+      <c r="ADD32" s="96"/>
+      <c r="ADE32" s="96"/>
+      <c r="ADF32" s="96"/>
+      <c r="ADG32" s="96"/>
+      <c r="ADH32" s="96"/>
+      <c r="ADI32" s="96"/>
+      <c r="ADJ32" s="96"/>
+      <c r="ADK32" s="96"/>
+      <c r="ADL32" s="96"/>
+      <c r="ADM32" s="96"/>
+      <c r="ADN32" s="96"/>
+      <c r="ADO32" s="96"/>
+      <c r="ADP32" s="96"/>
+      <c r="ADQ32" s="96"/>
+      <c r="ADR32" s="96"/>
+      <c r="ADS32" s="96"/>
+      <c r="ADT32" s="96"/>
+      <c r="ADU32" s="96"/>
+      <c r="ADV32" s="96"/>
+      <c r="ADW32" s="96"/>
+      <c r="ADX32" s="96"/>
+      <c r="ADY32" s="96"/>
+      <c r="ADZ32" s="96"/>
+      <c r="AEA32" s="96"/>
+      <c r="AEB32" s="96"/>
+      <c r="AEC32" s="96"/>
+      <c r="AED32" s="96"/>
+      <c r="AEE32" s="96"/>
+      <c r="AEF32" s="96"/>
+      <c r="AEG32" s="96"/>
+      <c r="AEH32" s="96"/>
+      <c r="AEI32" s="96"/>
+      <c r="AEJ32" s="96"/>
+      <c r="AEK32" s="96"/>
+      <c r="AEL32" s="96"/>
+      <c r="AEM32" s="96"/>
+      <c r="AEN32" s="96"/>
+      <c r="AEO32" s="96"/>
+      <c r="AEP32" s="96"/>
+      <c r="AEQ32" s="96"/>
+      <c r="AER32" s="96"/>
+      <c r="AES32" s="96"/>
+      <c r="AET32" s="96"/>
+      <c r="AEU32" s="96"/>
+      <c r="AEV32" s="96"/>
+      <c r="AEW32" s="96"/>
+      <c r="AEX32" s="96"/>
+      <c r="AEY32" s="96"/>
+      <c r="AEZ32" s="96"/>
+      <c r="AFA32" s="96"/>
+      <c r="AFB32" s="96"/>
+      <c r="AFC32" s="96"/>
+      <c r="AFD32" s="96"/>
+      <c r="AFE32" s="96"/>
+      <c r="AFF32" s="96"/>
+      <c r="AFG32" s="96"/>
+      <c r="AFH32" s="96"/>
+      <c r="AFI32" s="96"/>
+      <c r="AFJ32" s="96"/>
+      <c r="AFK32" s="96"/>
+      <c r="AFL32" s="96"/>
+      <c r="AFM32" s="96"/>
+      <c r="AFN32" s="96"/>
+      <c r="AFO32" s="96"/>
+      <c r="AFP32" s="96"/>
+      <c r="AFQ32" s="96"/>
+      <c r="AFR32" s="96"/>
+      <c r="AFS32" s="96"/>
+      <c r="AFT32" s="96"/>
+      <c r="AFU32" s="96"/>
+      <c r="AFV32" s="96"/>
+      <c r="AFW32" s="96"/>
+      <c r="AFX32" s="96"/>
+      <c r="AFY32" s="96"/>
+      <c r="AFZ32" s="96"/>
+      <c r="AGA32" s="96"/>
+      <c r="AGB32" s="96"/>
+      <c r="AGC32" s="96"/>
+      <c r="AGD32" s="96"/>
+      <c r="AGE32" s="96"/>
+      <c r="AGF32" s="96"/>
+      <c r="AGG32" s="96"/>
+      <c r="AGH32" s="96"/>
+      <c r="AGI32" s="96"/>
+      <c r="AGJ32" s="96"/>
+      <c r="AGK32" s="96"/>
+      <c r="AGL32" s="96"/>
+      <c r="AGM32" s="96"/>
+      <c r="AGN32" s="96"/>
+      <c r="AGO32" s="96"/>
+      <c r="AGP32" s="96"/>
+      <c r="AGQ32" s="96"/>
+      <c r="AGR32" s="96"/>
+      <c r="AGS32" s="96"/>
+      <c r="AGT32" s="96"/>
+      <c r="AGU32" s="96"/>
+      <c r="AGV32" s="96"/>
+      <c r="AGW32" s="96"/>
+      <c r="AGX32" s="96"/>
+      <c r="AGY32" s="96"/>
+      <c r="AGZ32" s="96"/>
+      <c r="AHA32" s="96"/>
+      <c r="AHB32" s="96"/>
+      <c r="AHC32" s="96"/>
+      <c r="AHD32" s="96"/>
+      <c r="AHE32" s="96"/>
+      <c r="AHF32" s="96"/>
+      <c r="AHG32" s="96"/>
+      <c r="AHH32" s="96"/>
+      <c r="AHI32" s="96"/>
+      <c r="AHJ32" s="96"/>
+      <c r="AHK32" s="96"/>
+      <c r="AHL32" s="96"/>
+      <c r="AHM32" s="96"/>
+      <c r="AHN32" s="96"/>
+      <c r="AHO32" s="96"/>
+      <c r="AHP32" s="96"/>
+      <c r="AHQ32" s="96"/>
+      <c r="AHR32" s="96"/>
+      <c r="AHS32" s="96"/>
+      <c r="AHT32" s="96"/>
+      <c r="AHU32" s="96"/>
+      <c r="AHV32" s="96"/>
+      <c r="AHW32" s="96"/>
+      <c r="AHX32" s="96"/>
+      <c r="AHY32" s="96"/>
+      <c r="AHZ32" s="96"/>
+      <c r="AIA32" s="96"/>
+      <c r="AIB32" s="96"/>
+      <c r="AIC32" s="96"/>
+      <c r="AID32" s="96"/>
+      <c r="AIE32" s="96"/>
+      <c r="AIF32" s="96"/>
+      <c r="AIG32" s="96"/>
+      <c r="AIH32" s="96"/>
+      <c r="AII32" s="96"/>
+      <c r="AIJ32" s="96"/>
+      <c r="AIK32" s="96"/>
+      <c r="AIL32" s="96"/>
+      <c r="AIM32" s="96"/>
+      <c r="AIN32" s="96"/>
+      <c r="AIO32" s="96"/>
+      <c r="AIP32" s="96"/>
+      <c r="AIQ32" s="96"/>
+      <c r="AIR32" s="96"/>
+      <c r="AIS32" s="96"/>
+      <c r="AIT32" s="96"/>
+      <c r="AIU32" s="96"/>
+      <c r="AIV32" s="96"/>
+      <c r="AIW32" s="96"/>
+      <c r="AIX32" s="96"/>
+      <c r="AIY32" s="96"/>
+      <c r="AIZ32" s="96"/>
+      <c r="AJA32" s="96"/>
+      <c r="AJB32" s="96"/>
+      <c r="AJC32" s="96"/>
+      <c r="AJD32" s="96"/>
+      <c r="AJE32" s="96"/>
+      <c r="AJF32" s="96"/>
+      <c r="AJG32" s="96"/>
+      <c r="AJH32" s="96"/>
+      <c r="AJI32" s="96"/>
+      <c r="AJJ32" s="96"/>
+      <c r="AJK32" s="96"/>
+      <c r="AJL32" s="96"/>
+      <c r="AJM32" s="96"/>
+      <c r="AJN32" s="96"/>
+      <c r="AJO32" s="96"/>
+      <c r="AJP32" s="96"/>
+      <c r="AJQ32" s="96"/>
+      <c r="AJR32" s="96"/>
+      <c r="AJS32" s="96"/>
+      <c r="AJT32" s="96"/>
+      <c r="AJU32" s="96"/>
+      <c r="AJV32" s="96"/>
+      <c r="AJW32" s="96"/>
+      <c r="AJX32" s="96"/>
+      <c r="AJY32" s="96"/>
+      <c r="AJZ32" s="96"/>
+      <c r="AKA32" s="96"/>
+      <c r="AKB32" s="96"/>
+      <c r="AKC32" s="96"/>
+      <c r="AKD32" s="96"/>
+      <c r="AKE32" s="96"/>
+      <c r="AKF32" s="96"/>
+      <c r="AKG32" s="96"/>
+      <c r="AKH32" s="96"/>
+      <c r="AKI32" s="96"/>
+      <c r="AKJ32" s="96"/>
+      <c r="AKK32" s="96"/>
+      <c r="AKL32" s="96"/>
+      <c r="AKM32" s="96"/>
+      <c r="AKN32" s="96"/>
+      <c r="AKO32" s="96"/>
+      <c r="AKP32" s="96"/>
+      <c r="AKQ32" s="96"/>
+      <c r="AKR32" s="96"/>
+      <c r="AKS32" s="96"/>
+      <c r="AKT32" s="96"/>
+      <c r="AKU32" s="96"/>
+      <c r="AKV32" s="96"/>
+      <c r="AKW32" s="96"/>
+      <c r="AKX32" s="96"/>
+      <c r="AKY32" s="96"/>
+      <c r="AKZ32" s="96"/>
+      <c r="ALA32" s="96"/>
+      <c r="ALB32" s="96"/>
+      <c r="ALC32" s="96"/>
+      <c r="ALD32" s="96"/>
+      <c r="ALE32" s="96"/>
+      <c r="ALF32" s="96"/>
+      <c r="ALG32" s="96"/>
+      <c r="ALH32" s="96"/>
+      <c r="ALI32" s="96"/>
+      <c r="ALJ32" s="96"/>
+      <c r="ALK32" s="96"/>
+      <c r="ALL32" s="96"/>
+      <c r="ALM32" s="96"/>
+      <c r="ALN32" s="96"/>
+      <c r="ALO32" s="96"/>
+      <c r="ALP32" s="96"/>
+      <c r="ALQ32" s="96"/>
+      <c r="ALR32" s="96"/>
+      <c r="ALS32" s="96"/>
+      <c r="ALT32" s="96"/>
+      <c r="ALU32" s="96"/>
+      <c r="ALV32" s="96"/>
+      <c r="ALW32" s="96"/>
+      <c r="ALX32" s="96"/>
+      <c r="ALY32" s="96"/>
+      <c r="ALZ32" s="96"/>
+      <c r="AMA32" s="96"/>
+      <c r="AMB32" s="96"/>
+      <c r="AMC32" s="96"/>
+      <c r="AMD32" s="96"/>
+      <c r="AME32" s="96"/>
+      <c r="AMF32" s="96"/>
+      <c r="AMG32" s="96"/>
+      <c r="AMH32" s="96"/>
+      <c r="AMI32" s="96"/>
+      <c r="AMJ32" s="96"/>
+      <c r="AMK32" s="96"/>
+      <c r="AML32" s="96"/>
+      <c r="AMM32" s="96"/>
+    </row>
+    <row r="33" spans="1:9" ht="162.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="129">
+        <v>11</v>
+      </c>
+      <c r="B33" s="126" t="s">
+        <v>648</v>
+      </c>
+      <c r="C33" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="130" t="s">
+        <v>651</v>
+      </c>
+      <c r="E33" s="127" t="s">
+        <v>652</v>
+      </c>
+      <c r="F33" s="125"/>
+      <c r="G33" s="131"/>
+      <c r="H33" s="131" t="s">
+        <v>649</v>
+      </c>
+      <c r="I33" s="125" t="s">
+        <v>650</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -21826,17 +21924,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
     </row>
     <row r="2" spans="1:9" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -22012,10 +22110,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK53"/>
+  <dimension ref="A1:AMK54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A47" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22033,17 +22131,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="119" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -22379,7 +22477,7 @@
       <c r="C10" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="105" t="s">
+      <c r="D10" s="103" t="s">
         <v>311</v>
       </c>
       <c r="E10" s="41"/>
@@ -25958,7 +26056,7 @@
       <c r="C27" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="106" t="s">
+      <c r="D27" s="104" t="s">
         <v>325</v>
       </c>
       <c r="E27" s="41"/>
@@ -26030,7 +26128,7 @@
       <c r="C30" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="107" t="s">
+      <c r="D30" s="105" t="s">
         <v>326</v>
       </c>
       <c r="E30" s="41"/>
@@ -26102,7 +26200,7 @@
       <c r="C33" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="106" t="s">
+      <c r="D33" s="104" t="s">
         <v>327</v>
       </c>
       <c r="E33" s="41"/>
@@ -27160,7 +27258,7 @@
       <c r="C35" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="105" t="s">
+      <c r="D35" s="103" t="s">
         <v>224</v>
       </c>
       <c r="E35" s="41"/>
@@ -27170,7 +27268,7 @@
         <v>293</v>
       </c>
       <c r="I35" s="36" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="36" spans="1:1025" ht="135" x14ac:dyDescent="0.25">
@@ -27194,7 +27292,7 @@
         <v>294</v>
       </c>
       <c r="I36" s="36" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="37" spans="1:1025" ht="90" x14ac:dyDescent="0.25">
@@ -27218,7 +27316,7 @@
         <v>295</v>
       </c>
       <c r="I37" s="36" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="38" spans="1:1025" ht="75" x14ac:dyDescent="0.25">
@@ -27302,7 +27400,7 @@
       <c r="C41" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="105" t="s">
+      <c r="D41" s="103" t="s">
         <v>336</v>
       </c>
       <c r="E41" s="41"/>
@@ -27348,7 +27446,7 @@
       <c r="C43" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="108">
+      <c r="D43" s="106">
         <v>43466</v>
       </c>
       <c r="E43" s="41"/>
@@ -27394,7 +27492,7 @@
       <c r="C45" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="105" t="s">
+      <c r="D45" s="103" t="s">
         <v>371</v>
       </c>
       <c r="E45" s="41"/>
@@ -27446,7 +27544,7 @@
       <c r="E47" s="41"/>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
-      <c r="H47" s="104" t="s">
+      <c r="H47" s="102" t="s">
         <v>515</v>
       </c>
       <c r="I47" s="36" t="s">
@@ -27469,7 +27567,7 @@
       <c r="E48" s="41"/>
       <c r="F48" s="41"/>
       <c r="G48" s="41"/>
-      <c r="H48" s="104" t="s">
+      <c r="H48" s="102" t="s">
         <v>527</v>
       </c>
       <c r="I48" s="36"/>
@@ -27490,7 +27588,7 @@
       <c r="E49" s="41"/>
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
-      <c r="H49" s="104" t="s">
+      <c r="H49" s="102" t="s">
         <v>527</v>
       </c>
       <c r="I49" s="36"/>
@@ -27511,7 +27609,7 @@
       <c r="E50" s="41"/>
       <c r="F50" s="41"/>
       <c r="G50" s="41"/>
-      <c r="H50" s="104" t="s">
+      <c r="H50" s="102" t="s">
         <v>527</v>
       </c>
       <c r="I50" s="36"/>
@@ -27532,7 +27630,7 @@
       <c r="E51" s="41"/>
       <c r="F51" s="41"/>
       <c r="G51" s="41"/>
-      <c r="H51" s="104" t="s">
+      <c r="H51" s="102" t="s">
         <v>404</v>
       </c>
       <c r="I51" s="36" t="s">
@@ -27555,11 +27653,11 @@
       <c r="E52" s="41"/>
       <c r="F52" s="41"/>
       <c r="G52" s="41"/>
-      <c r="H52" s="104" t="s">
+      <c r="H52" s="102" t="s">
         <v>531</v>
       </c>
       <c r="I52" s="36" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -27567,23 +27665,34 @@
         <v>50</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="13" t="s">
+        <v>642</v>
+      </c>
+      <c r="E53" s="41" t="s">
         <v>643</v>
-      </c>
-      <c r="E53" s="41" t="s">
-        <v>644</v>
       </c>
       <c r="F53" s="41"/>
       <c r="G53" s="41"/>
-      <c r="H53" s="104"/>
+      <c r="H53" s="102"/>
       <c r="I53" s="36" t="s">
-        <v>647</v>
-      </c>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="102"/>
+      <c r="I54" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added a config for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
+++ b/docs/requirements/MOSIP_Configurations_Consolidated List_Updated_14Nov18_CV_Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1972D176-60EA-44F1-B46F-8EBEC41D0152}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B8D4EA1B-3DDD-4EBB-A568-9775A1797907}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2595" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="1166">
   <si>
     <r>
       <rPr>
@@ -4397,6 +4397,37 @@
   <si>
     <t>OK. Will be updated
 &lt;05 08&gt; Updated</t>
+  </si>
+  <si>
+    <t>Set up  Internal Authentication Quality Composite Threshold for Fingerprints (3-10)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+For Composite Fingerprint Authentication for Intenal Auth, the Match Score generated from the Fingerprint SDK will be validated against the Composite quality threshold set
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+On change:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Bookman Old Style"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> When these values are changed the match scores will be compared against the changed values.
+This configuration can be modified as as per the scenario and the business need in the country </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4689,6 +4720,7 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Bookman Old Style"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -5656,6 +5688,12 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5691,12 +5729,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7436,18 +7468,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="194" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="194"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="196"/>
     </row>
     <row r="2" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -8049,19 +8081,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="195" t="s">
+      <c r="A1" s="197" t="s">
         <v>1153</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
-      <c r="F1" s="196"/>
-      <c r="G1" s="196"/>
-      <c r="H1" s="196"/>
-      <c r="I1" s="196"/>
-      <c r="J1" s="196"/>
-      <c r="K1" s="197"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198"/>
+      <c r="K1" s="199"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A2" s="162" t="s">
@@ -8856,19 +8888,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="200"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="202"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -13256,19 +13288,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17 1030:1030" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="194" t="s">
         <v>1100</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="193"/>
-      <c r="K1" s="200"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="202"/>
       <c r="L1" s="3"/>
       <c r="AMP1"/>
     </row>
@@ -19776,13 +19808,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AML33"/>
+  <dimension ref="A1:AML34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19803,20 +19835,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1026" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="202"/>
-      <c r="J1" s="202"/>
-      <c r="K1" s="202"/>
-      <c r="L1" s="202"/>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
     </row>
     <row r="2" spans="1:1026" s="137" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="133" t="s">
@@ -31766,7 +31798,7 @@
       <c r="B31" s="58" t="s">
         <v>332</v>
       </c>
-      <c r="C31" s="204" t="s">
+      <c r="C31" s="192" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="58" t="s">
@@ -31775,7 +31807,7 @@
       <c r="E31" s="58" t="s">
         <v>613</v>
       </c>
-      <c r="F31" s="205"/>
+      <c r="F31" s="193"/>
       <c r="G31" s="56"/>
       <c r="H31" s="56" t="s">
         <v>614</v>
@@ -32869,6 +32901,31 @@
         <v>1147</v>
       </c>
     </row>
+    <row r="34" spans="1:12" ht="372.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="152">
+        <v>12</v>
+      </c>
+      <c r="B34" s="71" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="145">
+        <v>60</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71" t="s">
+        <v>1165</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:AML33" xr:uid="{0660994A-5737-439E-900F-70E6CC425AEC}"/>
   <mergeCells count="1">
@@ -32901,17 +32958,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="205" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="205"/>
+      <c r="I1" s="205"/>
     </row>
     <row r="2" spans="1:10" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -33118,20 +33175,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="194" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="193"/>
-      <c r="K1" s="193"/>
-      <c r="L1" s="194"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="196"/>
     </row>
     <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">

</xml_diff>